<commit_message>
Can be run with cmd now
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A34AB6C1-E8C9-4E7B-A591-D6510DA5A81E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3120671-F34E-4397-98E2-C333D681BCE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
@@ -19,10 +19,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$K$18</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -843,9 +848,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9188EC-3268-404A-8733-94DAF537670F}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:J17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1061,7 +1069,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1093,7 +1101,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1320,7 +1328,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
@@ -1384,7 +1392,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
@@ -1433,6 +1441,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:K18" xr:uid="{49361AC2-0FC4-4902-86C7-B4FB07E48568}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="400"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A3:K18">
       <sortCondition ref="I2:I18"/>
     </sortState>

</xml_diff>

<commit_message>
Post-processor via cmd; more testing Kim model
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3120671-F34E-4397-98E2-C333D681BCE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A37099-4DF4-4BBB-BF2F-9A4137FEA53D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="VarPropEta" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$K$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$N$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
   <si>
     <t>Folder ID</t>
   </si>
@@ -160,6 +160,18 @@
   </si>
   <si>
     <t>T&gt;=2500 K for v&gt;0</t>
+  </si>
+  <si>
+    <t>Mesh-1</t>
+  </si>
+  <si>
+    <t>N_x</t>
+  </si>
+  <si>
+    <t>N_y</t>
+  </si>
+  <si>
+    <t>Reaction Zone Width (um)</t>
   </si>
 </sst>
 </file>
@@ -210,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -223,6 +235,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -848,606 +861,871 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9188EC-3268-404A-8733-94DAF537670F}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:J17"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="79.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="79.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" t="s">
+      <c r="C1" s="8"/>
+      <c r="I1" s="3"/>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B3">
-        <v>400</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="8">
+        <v>101</v>
+      </c>
+      <c r="C3" s="8">
+        <v>601</v>
+      </c>
+      <c r="D3">
+        <v>400</v>
+      </c>
+      <c r="E3">
         <v>800</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3">
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3">
         <v>70</v>
       </c>
-      <c r="F3" s="2">
+      <c r="H3" s="2">
         <v>4890000</v>
       </c>
-      <c r="G3" s="3">
+      <c r="I3" s="3">
         <v>63</v>
       </c>
-      <c r="H3" s="4">
+      <c r="J3" s="4">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="I3" s="4">
+      <c r="K3" s="4">
         <v>0</v>
       </c>
-      <c r="J3" s="4">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="4">
+        <v>400</v>
+      </c>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B4">
-        <v>400</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="8">
+        <v>101</v>
+      </c>
+      <c r="C4" s="8">
+        <v>601</v>
+      </c>
+      <c r="D4">
+        <v>400</v>
+      </c>
+      <c r="E4">
         <v>800</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4">
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4">
         <v>48</v>
       </c>
-      <c r="F4" s="2">
+      <c r="H4" s="2">
         <v>4890000</v>
       </c>
-      <c r="G4" s="3">
+      <c r="I4" s="3">
         <v>63</v>
       </c>
-      <c r="H4" s="4">
+      <c r="J4" s="4">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="I4" s="4">
+      <c r="K4" s="4">
         <v>0</v>
       </c>
-      <c r="J4" s="4">
+      <c r="L4" s="4">
         <v>368</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B5">
-        <v>400</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="8">
+        <v>101</v>
+      </c>
+      <c r="C5" s="8">
+        <v>601</v>
+      </c>
+      <c r="D5">
+        <v>400</v>
+      </c>
+      <c r="E5">
         <v>900</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5">
         <v>70</v>
       </c>
-      <c r="F5" s="2">
+      <c r="H5" s="2">
         <v>4890000</v>
       </c>
-      <c r="G5" s="3">
+      <c r="I5" s="3">
         <v>63</v>
       </c>
-      <c r="H5" s="4">
+      <c r="J5" s="4">
         <v>0.13</v>
       </c>
-      <c r="I5" s="4">
+      <c r="K5" s="4">
         <v>0</v>
       </c>
-      <c r="J5" s="4">
+      <c r="L5" s="4">
         <v>460</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B6">
-        <v>400</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="8">
+        <v>101</v>
+      </c>
+      <c r="C6" s="8">
+        <v>601</v>
+      </c>
+      <c r="D6">
+        <v>400</v>
+      </c>
+      <c r="E6">
         <v>1000</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6">
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6">
         <v>70</v>
       </c>
-      <c r="F6" s="2">
+      <c r="H6" s="2">
         <v>4890000</v>
       </c>
-      <c r="G6" s="3">
+      <c r="I6" s="3">
         <v>63</v>
       </c>
-      <c r="H6" s="4">
+      <c r="J6" s="4">
         <v>0.15</v>
       </c>
-      <c r="I6" s="4">
+      <c r="K6" s="4">
         <v>0</v>
       </c>
-      <c r="J6" s="4">
+      <c r="L6" s="4">
         <v>500</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B7">
-        <v>400</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="8">
+        <v>101</v>
+      </c>
+      <c r="C7" s="8">
+        <v>601</v>
+      </c>
+      <c r="D7">
+        <v>400</v>
+      </c>
+      <c r="E7">
         <v>1200</v>
       </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7">
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7">
         <v>78</v>
       </c>
-      <c r="F7" s="2">
+      <c r="H7" s="2">
         <v>4890000</v>
       </c>
-      <c r="G7" s="3">
+      <c r="I7" s="3">
         <v>63</v>
       </c>
-      <c r="H7" s="4">
+      <c r="J7" s="4">
         <v>0.22</v>
       </c>
-      <c r="I7" s="4">
+      <c r="K7" s="4">
         <v>0</v>
       </c>
-      <c r="J7" s="4">
+      <c r="L7" s="4">
         <v>640</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
+        <v>101</v>
+      </c>
+      <c r="C8" s="8">
+        <v>601</v>
+      </c>
+      <c r="D8">
         <v>200</v>
       </c>
-      <c r="C8" s="1">
+      <c r="E8" s="1">
         <v>1200</v>
       </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8">
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8">
         <v>48</v>
       </c>
-      <c r="F8" s="2">
+      <c r="H8" s="2">
         <v>4890000</v>
       </c>
-      <c r="G8" s="3">
+      <c r="I8" s="3">
         <v>63</v>
       </c>
-      <c r="H8" s="1">
+      <c r="J8" s="1">
         <v>0.4</v>
       </c>
-      <c r="I8" s="4">
+      <c r="K8" s="4">
         <v>1.7</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>2500</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="8">
+        <v>101</v>
+      </c>
+      <c r="C9" s="8">
+        <v>601</v>
+      </c>
+      <c r="D9">
         <v>200</v>
       </c>
-      <c r="C9" s="1">
+      <c r="E9" s="1">
         <v>1200</v>
       </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9">
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9">
         <v>48</v>
       </c>
-      <c r="F9" s="2">
+      <c r="H9" s="2">
         <v>4890000</v>
       </c>
-      <c r="G9" s="7">
+      <c r="I9" s="7">
         <v>4.07</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>0.22</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>5.2</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>9000</v>
       </c>
-      <c r="K9" t="s">
+      <c r="N9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B10">
-        <v>400</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="8">
+        <v>101</v>
+      </c>
+      <c r="C10" s="8">
+        <v>601</v>
+      </c>
+      <c r="D10">
+        <v>400</v>
+      </c>
+      <c r="E10">
         <v>1200</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10">
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10">
         <v>70</v>
       </c>
-      <c r="F10" s="2">
+      <c r="H10" s="2">
         <v>4890000</v>
       </c>
-      <c r="G10" s="3">
+      <c r="I10" s="3">
         <v>63</v>
       </c>
-      <c r="H10" s="4">
+      <c r="J10" s="4">
         <v>0.17</v>
       </c>
-      <c r="I10" s="4">
+      <c r="K10" s="4">
         <v>6.9</v>
       </c>
-      <c r="J10" s="4">
+      <c r="L10" s="4">
         <v>22500</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B11">
-        <v>400</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
+      <c r="B11" s="8">
+        <v>101</v>
+      </c>
+      <c r="C11" s="8">
+        <v>601</v>
       </c>
       <c r="D11">
+        <v>400</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11">
         <v>0.999</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>70</v>
       </c>
-      <c r="F11" s="2">
+      <c r="H11" s="2">
         <v>4890000</v>
       </c>
-      <c r="G11" s="3">
+      <c r="I11" s="3">
         <v>63</v>
       </c>
-      <c r="H11" s="4">
+      <c r="J11" s="4">
         <v>0.18</v>
       </c>
-      <c r="I11" s="4">
+      <c r="K11" s="4">
         <v>7</v>
       </c>
-      <c r="J11" s="4">
+      <c r="L11" s="4">
         <v>20000</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12">
-        <v>400</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
+      <c r="B12" s="8">
+        <v>101</v>
+      </c>
+      <c r="C12" s="8">
+        <v>601</v>
       </c>
       <c r="D12">
+        <v>400</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12">
         <v>0.9</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>70</v>
       </c>
-      <c r="F12" s="2">
+      <c r="H12" s="2">
         <v>4890000</v>
       </c>
-      <c r="G12" s="3">
+      <c r="I12" s="3">
         <v>63</v>
       </c>
-      <c r="H12" s="4">
+      <c r="J12" s="4">
         <v>0.18</v>
       </c>
-      <c r="I12" s="4">
+      <c r="K12" s="4">
         <v>7</v>
       </c>
-      <c r="J12" s="4">
+      <c r="L12" s="4">
         <v>20000</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13">
-        <v>400</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
+      <c r="B13" s="8">
+        <v>101</v>
+      </c>
+      <c r="C13" s="8">
+        <v>601</v>
       </c>
       <c r="D13">
+        <v>400</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13">
         <v>0.8</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>70</v>
       </c>
-      <c r="F13" s="2">
+      <c r="H13" s="2">
         <v>4890000</v>
       </c>
-      <c r="G13" s="3">
+      <c r="I13" s="3">
         <v>63</v>
       </c>
-      <c r="H13" s="4">
+      <c r="J13" s="4">
         <v>0.18</v>
       </c>
-      <c r="I13" s="4">
+      <c r="K13" s="4">
         <v>7</v>
       </c>
-      <c r="J13" s="4">
+      <c r="L13" s="4">
         <v>20000</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B14">
-        <v>400</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
+      <c r="B14" s="8">
+        <v>101</v>
+      </c>
+      <c r="C14" s="8">
+        <v>601</v>
       </c>
       <c r="D14">
+        <v>400</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14">
         <v>0.7</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>70</v>
       </c>
-      <c r="F14" s="2">
+      <c r="H14" s="2">
         <v>4890000</v>
       </c>
-      <c r="G14" s="3">
+      <c r="I14" s="3">
         <v>63</v>
       </c>
-      <c r="H14" s="4">
+      <c r="J14" s="4">
         <v>0.18</v>
       </c>
-      <c r="I14" s="4">
+      <c r="K14" s="4">
         <v>7</v>
       </c>
-      <c r="J14" s="4">
+      <c r="L14" s="4">
         <v>20000</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15">
-        <v>400</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
+      <c r="B15" s="8">
+        <v>101</v>
+      </c>
+      <c r="C15" s="8">
+        <v>601</v>
       </c>
       <c r="D15">
+        <v>400</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15">
         <v>0.5</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>70</v>
       </c>
-      <c r="F15" s="2">
+      <c r="H15" s="2">
         <v>4890000</v>
       </c>
-      <c r="G15" s="3">
+      <c r="I15" s="3">
         <v>63</v>
       </c>
-      <c r="H15" s="4">
+      <c r="J15" s="4">
         <v>0.18</v>
       </c>
-      <c r="I15" s="4">
+      <c r="K15" s="4">
         <v>7</v>
       </c>
-      <c r="J15" s="4">
+      <c r="L15" s="4">
         <v>20000</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="8">
+        <v>101</v>
+      </c>
+      <c r="C16" s="8">
+        <v>601</v>
+      </c>
+      <c r="D16">
         <v>200</v>
       </c>
-      <c r="C16">
+      <c r="E16">
         <v>1200</v>
       </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16">
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16">
         <v>70</v>
       </c>
-      <c r="F16" s="2">
+      <c r="H16" s="2">
         <v>4890000</v>
       </c>
-      <c r="G16" s="3">
+      <c r="I16" s="3">
         <v>63</v>
       </c>
-      <c r="H16" s="4">
+      <c r="J16" s="4">
         <v>0.54</v>
       </c>
-      <c r="I16" s="4">
+      <c r="K16" s="4">
         <v>7</v>
       </c>
-      <c r="J16" s="4">
+      <c r="L16" s="4">
         <v>20000</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B17">
-        <v>400</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="8">
+        <v>101</v>
+      </c>
+      <c r="C17" s="8">
+        <v>601</v>
+      </c>
+      <c r="D17">
+        <v>400</v>
+      </c>
+      <c r="E17">
         <v>1200</v>
       </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17">
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17">
         <v>48</v>
       </c>
-      <c r="F17" s="2">
+      <c r="H17" s="2">
         <v>4890000</v>
       </c>
-      <c r="G17" s="3">
+      <c r="I17" s="3">
         <v>63</v>
       </c>
-      <c r="H17" s="4">
+      <c r="J17" s="4">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="I17" s="4">
+      <c r="K17" s="4">
         <v>8.6999999999999993</v>
       </c>
-      <c r="J17" s="4">
+      <c r="L17" s="4">
         <v>21000</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="8">
+        <v>101</v>
+      </c>
+      <c r="C18" s="8">
+        <v>601</v>
+      </c>
+      <c r="D18">
         <v>200</v>
       </c>
-      <c r="C18">
+      <c r="E18">
         <v>1200</v>
       </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18">
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18">
         <v>48</v>
       </c>
-      <c r="F18" s="2">
+      <c r="H18" s="2">
         <v>4890000</v>
       </c>
-      <c r="G18" s="3">
+      <c r="I18" s="3">
         <v>63</v>
       </c>
-      <c r="H18" s="4">
+      <c r="J18" s="4">
         <v>0.15</v>
       </c>
-      <c r="I18" s="4">
+      <c r="K18" s="4">
         <v>9.1999999999999993</v>
       </c>
-      <c r="J18" s="4">
+      <c r="L18" s="4">
         <v>20000</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="4">
+        <v>101</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1201</v>
+      </c>
+      <c r="D19">
+        <v>400</v>
+      </c>
+      <c r="E19">
+        <v>1200</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>48</v>
+      </c>
+      <c r="H19" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="I19" s="3">
+        <v>63</v>
+      </c>
+      <c r="J19" s="4">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="K19" s="4">
+        <v>8.1</v>
+      </c>
+      <c r="L19" s="4">
+        <v>20000</v>
+      </c>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" t="s">
         <v>41</v>
       </c>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="I39" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K18" xr:uid="{49361AC2-0FC4-4902-86C7-B4FB07E48568}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="400"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A3:K18">
-      <sortCondition ref="I2:I18"/>
+  <autoFilter ref="A2:N19" xr:uid="{49361AC2-0FC4-4902-86C7-B4FB07E48568}">
+    <sortState ref="A3:N18">
+      <sortCondition ref="K2:K18"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Testing and adjust FileClasses regarding input file extension
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A37099-4DF4-4BBB-BF2F-9A4137FEA53D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4CBECD-A202-43DA-A92A-788FB8450BD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
   <sheets>
     <sheet name="ConstantProp" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="51">
   <si>
     <t>Folder ID</t>
   </si>
@@ -57,9 +57,6 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>dH [J/kg]</t>
-  </si>
-  <si>
     <t>Parameters</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>v [m/s]</t>
   </si>
   <si>
-    <t>Temp. OOM [K]</t>
-  </si>
-  <si>
     <t>Tests-1</t>
   </si>
   <si>
@@ -172,6 +166,27 @@
   </si>
   <si>
     <t>Reaction Zone Width (um)</t>
+  </si>
+  <si>
+    <t>A0-1</t>
+  </si>
+  <si>
+    <t>A0-2</t>
+  </si>
+  <si>
+    <t>Div</t>
+  </si>
+  <si>
+    <t>Material properties</t>
+  </si>
+  <si>
+    <t>rho [kg/m^3]</t>
+  </si>
+  <si>
+    <t>Cp [J/kg/K]</t>
+  </si>
+  <si>
+    <t>k [W/m/K]</t>
   </si>
 </sst>
 </file>
@@ -222,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -236,6 +251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,308 +566,438 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3C7F47-CBB8-4962-A50C-2146AC268A42}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="3"/>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="3"/>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="L2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="O2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="3"/>
+      <c r="E3">
+        <v>101</v>
+      </c>
+      <c r="F3">
+        <v>601</v>
+      </c>
+      <c r="G3">
+        <v>400</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>40</v>
+      </c>
+      <c r="K3" s="9">
+        <v>100000000</v>
+      </c>
+      <c r="L3" s="3">
+        <v>300000</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="O3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="3"/>
+      <c r="E4">
+        <v>101</v>
+      </c>
+      <c r="F4">
+        <v>601</v>
+      </c>
+      <c r="G4">
+        <v>400</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>40</v>
+      </c>
+      <c r="K4" s="9">
+        <v>100000000</v>
+      </c>
+      <c r="L4" s="3">
+        <v>30000</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
-        <v>400</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="3"/>
+      <c r="E5">
+        <v>101</v>
+      </c>
+      <c r="F5">
+        <v>601</v>
+      </c>
+      <c r="G5">
+        <v>400</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="J5">
         <v>40</v>
       </c>
-      <c r="F3" s="2">
+      <c r="K5" s="9">
         <v>100000000</v>
       </c>
-      <c r="G3" s="3">
+      <c r="L5" s="3">
+        <v>1200</v>
+      </c>
+      <c r="M5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="3"/>
+      <c r="E6">
+        <v>101</v>
+      </c>
+      <c r="F6">
+        <v>601</v>
+      </c>
+      <c r="G6">
+        <v>400</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>40</v>
+      </c>
+      <c r="K6" s="9">
+        <v>1000000</v>
+      </c>
+      <c r="L6" s="3">
+        <v>30000</v>
+      </c>
+      <c r="M6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="3"/>
+      <c r="E7">
+        <v>101</v>
+      </c>
+      <c r="F7">
+        <v>601</v>
+      </c>
+      <c r="G7">
+        <v>400</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>40</v>
+      </c>
+      <c r="K7" s="9">
+        <v>10000000</v>
+      </c>
+      <c r="L7" s="3">
         <v>300000</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="4">
-        <v>1.7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>400</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
+      <c r="M7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="3"/>
+      <c r="E8">
+        <v>101</v>
+      </c>
+      <c r="F8">
+        <v>601</v>
+      </c>
+      <c r="G8">
+        <v>400</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>40</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="J8">
+        <v>70</v>
+      </c>
+      <c r="K8" s="9">
         <v>100000000</v>
       </c>
-      <c r="G4" s="3">
-        <v>30000</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4">
+      <c r="L8" s="3">
+        <v>300000</v>
+      </c>
+      <c r="M8" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>400</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
+      <c r="O8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="3"/>
+      <c r="E9">
+        <v>101</v>
+      </c>
+      <c r="F9">
+        <v>601</v>
+      </c>
+      <c r="G9">
+        <v>400</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>40</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="J9">
+        <v>170</v>
+      </c>
+      <c r="K9" s="9">
         <v>100000000</v>
       </c>
-      <c r="G5" s="3">
-        <v>1200</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5">
+      <c r="L9" s="3">
+        <v>300000</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9">
         <v>0</v>
       </c>
-      <c r="J5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>400</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>40</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1000000</v>
-      </c>
-      <c r="G6" s="3">
-        <v>30000</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>400</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>40</v>
-      </c>
-      <c r="F7" s="2">
-        <v>10000000</v>
-      </c>
-      <c r="G7" s="3">
-        <v>300000</v>
-      </c>
-      <c r="H7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>400</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>70</v>
-      </c>
-      <c r="F8" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G8" s="3">
-        <v>300000</v>
-      </c>
-      <c r="H8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9">
-        <v>400</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>170</v>
-      </c>
-      <c r="F9" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G9" s="3">
-        <v>300000</v>
-      </c>
-      <c r="H9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="3"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="3"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="3"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="3"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="3"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="3"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -863,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9188EC-3268-404A-8733-94DAF537670F}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,12 +1026,12 @@
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="8"/>
       <c r="I1" s="3"/>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -893,10 +1039,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -914,27 +1060,27 @@
         <v>4</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" t="s">
         <v>21</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="8">
         <v>101</v>
@@ -973,7 +1119,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="8">
         <v>101</v>
@@ -1012,7 +1158,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="8">
         <v>101</v>
@@ -1051,7 +1197,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="8">
         <v>101</v>
@@ -1090,7 +1236,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="8">
         <v>101</v>
@@ -1129,7 +1275,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="8">
         <v>101</v>
@@ -1167,7 +1313,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="8">
         <v>101</v>
@@ -1203,12 +1349,12 @@
         <v>9000</v>
       </c>
       <c r="N9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8">
         <v>101</v>
@@ -1247,7 +1393,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="8">
         <v>101</v>
@@ -1286,7 +1432,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="8">
         <v>101</v>
@@ -1325,7 +1471,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="8">
         <v>101</v>
@@ -1364,7 +1510,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="8">
         <v>101</v>
@@ -1403,7 +1549,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="8">
         <v>101</v>
@@ -1442,7 +1588,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="8">
         <v>101</v>
@@ -1481,7 +1627,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="8">
         <v>101</v>
@@ -1520,7 +1666,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="8">
         <v>101</v>
@@ -1559,7 +1705,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" s="4">
         <v>101</v>
@@ -1597,33 +1743,121 @@
       <c r="M19" s="4"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="I20" s="3"/>
+      <c r="A20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="4">
+        <v>101</v>
+      </c>
+      <c r="C20" s="4">
+        <v>601</v>
+      </c>
+      <c r="D20">
+        <v>400</v>
+      </c>
+      <c r="E20">
+        <v>1200</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>70</v>
+      </c>
+      <c r="H20" s="2">
+        <v>489000</v>
+      </c>
+      <c r="I20" s="3">
+        <v>63</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
+      <c r="L20" s="4">
+        <v>700</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="I21" s="3"/>
+      <c r="B21" s="4">
+        <v>101</v>
+      </c>
+      <c r="C21" s="4">
+        <v>601</v>
+      </c>
+      <c r="D21">
+        <v>400</v>
+      </c>
+      <c r="E21">
+        <v>1200</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>70</v>
+      </c>
+      <c r="H21" s="2">
+        <v>48900000</v>
+      </c>
+      <c r="I21" s="3">
+        <v>63</v>
+      </c>
+      <c r="J21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" t="s">
+        <v>46</v>
+      </c>
+      <c r="L21" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="3"/>
+      <c r="A22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="4">
+        <v>101</v>
+      </c>
+      <c r="C22" s="4">
+        <v>601</v>
+      </c>
+      <c r="D22">
+        <v>400</v>
+      </c>
+      <c r="E22">
+        <v>1200</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>78</v>
+      </c>
+      <c r="H22" s="2">
+        <v>48900000</v>
+      </c>
+      <c r="I22" s="3">
+        <v>63</v>
+      </c>
+      <c r="J22" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
-      <c r="D23" t="s">
-        <v>41</v>
-      </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1678,12 +1912,18 @@
       <c r="A32" s="6"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
       <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
+      <c r="D33" t="s">
+        <v>39</v>
+      </c>
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Timer in main.py; more testing
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\School\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6C3FF6-566A-43E6-A772-646570366358}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF501470-BA1D-46A5-9CA1-9B428A31ECF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="VarPropEta" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$N$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$O$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="64">
   <si>
     <t>Folder ID</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Enthalpy has units MJ/kg</t>
-  </si>
-  <si>
     <t>Eign-1</t>
   </si>
   <si>
@@ -196,6 +193,39 @@
   </si>
   <si>
     <t>dH-6</t>
+  </si>
+  <si>
+    <t>Conservative formulation</t>
+  </si>
+  <si>
+    <t>Conserv-1</t>
+  </si>
+  <si>
+    <t>Conserv-2</t>
+  </si>
+  <si>
+    <t>dH from Baijot 2016</t>
+  </si>
+  <si>
+    <t>Enthalpy has units MJ/kg; From FlorinPetre 2014</t>
+  </si>
+  <si>
+    <t>dH from Nicollet 2017</t>
+  </si>
+  <si>
+    <t>Run time (min)</t>
+  </si>
+  <si>
+    <t>Conserv-3</t>
+  </si>
+  <si>
+    <t>5.56 (L)</t>
+  </si>
+  <si>
+    <t>6.27 (L)</t>
+  </si>
+  <si>
+    <t>6.08 (L)</t>
   </si>
 </sst>
 </file>
@@ -211,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +251,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -261,6 +297,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,7 +640,7 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="3"/>
@@ -619,19 +659,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="E2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
@@ -658,10 +698,10 @@
         <v>10</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q2" t="s">
         <v>21</v>
@@ -1016,24 +1056,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9188EC-3268-404A-8733-94DAF537670F}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="79.85546875" customWidth="1"/>
+    <col min="13" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="79.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" t="s">
         <v>7</v>
@@ -1044,15 +1085,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1079,18 +1120,21 @@
         <v>10</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="8">
         <v>101</v>
@@ -1126,10 +1170,14 @@
         <v>400</v>
       </c>
       <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N3" s="4"/>
+      <c r="O3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="8">
         <v>101</v>
@@ -1165,10 +1213,14 @@
         <v>368</v>
       </c>
       <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="4"/>
+      <c r="O4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="8">
         <v>101</v>
@@ -1204,10 +1256,14 @@
         <v>460</v>
       </c>
       <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" s="4"/>
+      <c r="O5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="8">
         <v>101</v>
@@ -1243,10 +1299,14 @@
         <v>500</v>
       </c>
       <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N6" s="4"/>
+      <c r="O6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="8">
         <v>101</v>
@@ -1282,8 +1342,12 @@
         <v>640</v>
       </c>
       <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7" s="4"/>
+      <c r="O7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1320,8 +1384,11 @@
       <c r="L8">
         <v>2500</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -1358,52 +1425,56 @@
       <c r="L9">
         <v>9000</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="11">
+        <v>101</v>
+      </c>
+      <c r="C10" s="11">
+        <v>601</v>
+      </c>
+      <c r="D10" s="12">
+        <v>400</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1200</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="12">
+        <v>70</v>
+      </c>
+      <c r="H10" s="13">
+        <v>4890000</v>
+      </c>
+      <c r="I10" s="10">
+        <v>63</v>
+      </c>
+      <c r="J10" s="11">
+        <v>0.17</v>
+      </c>
+      <c r="K10" s="11">
+        <v>6.9</v>
+      </c>
+      <c r="L10" s="11">
+        <v>22500</v>
+      </c>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="8">
-        <v>101</v>
-      </c>
-      <c r="C10" s="8">
-        <v>601</v>
-      </c>
-      <c r="D10">
-        <v>400</v>
-      </c>
-      <c r="E10">
-        <v>1200</v>
-      </c>
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10">
-        <v>70</v>
-      </c>
-      <c r="H10" s="2">
-        <v>4890000</v>
-      </c>
-      <c r="I10" s="3">
-        <v>63</v>
-      </c>
-      <c r="J10" s="4">
-        <v>0.17</v>
-      </c>
-      <c r="K10" s="4">
-        <v>6.9</v>
-      </c>
-      <c r="L10" s="4">
-        <v>22500</v>
-      </c>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="B11" s="8">
         <v>101</v>
@@ -1439,10 +1510,14 @@
         <v>20000</v>
       </c>
       <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N11" s="4"/>
+      <c r="O11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="8">
         <v>101</v>
@@ -1478,10 +1553,14 @@
         <v>20000</v>
       </c>
       <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" s="4"/>
+      <c r="O12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="8">
         <v>101</v>
@@ -1517,10 +1596,14 @@
         <v>20000</v>
       </c>
       <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N13" s="4"/>
+      <c r="O13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="8">
         <v>101</v>
@@ -1556,10 +1639,14 @@
         <v>20000</v>
       </c>
       <c r="M14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N14" s="4"/>
+      <c r="O14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="8">
         <v>101</v>
@@ -1595,10 +1682,14 @@
         <v>20000</v>
       </c>
       <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N15" s="4"/>
+      <c r="O15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="8">
         <v>101</v>
@@ -1612,7 +1703,7 @@
       <c r="E16">
         <v>1200</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G16">
@@ -1634,10 +1725,14 @@
         <v>20000</v>
       </c>
       <c r="M16" s="4"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="4"/>
+      <c r="O16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="8">
         <v>101</v>
@@ -1651,7 +1746,7 @@
       <c r="E17">
         <v>1200</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G17">
@@ -1673,10 +1768,14 @@
         <v>21000</v>
       </c>
       <c r="M17" s="4"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="4"/>
+      <c r="O17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="8">
         <v>101</v>
@@ -1690,7 +1789,7 @@
       <c r="E18">
         <v>1200</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G18">
@@ -1712,10 +1811,14 @@
         <v>20000</v>
       </c>
       <c r="M18" s="4"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="4"/>
+      <c r="O18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="4">
         <v>101</v>
@@ -1729,7 +1832,7 @@
       <c r="E19">
         <v>1200</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G19">
@@ -1751,10 +1854,14 @@
         <v>20000</v>
       </c>
       <c r="M19" s="4"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="4"/>
+      <c r="O19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="4">
         <v>101</v>
@@ -1768,7 +1875,7 @@
       <c r="E20">
         <v>1200</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G20">
@@ -1789,8 +1896,11 @@
       <c r="L20" s="4">
         <v>700</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="4">
         <v>101</v>
@@ -1804,7 +1914,7 @@
       <c r="E21">
         <v>1200</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G21">
@@ -1817,16 +1927,19 @@
         <v>63</v>
       </c>
       <c r="J21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="O21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="4">
         <v>101</v>
@@ -1840,7 +1953,7 @@
       <c r="E22">
         <v>1200</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G22">
@@ -1853,18 +1966,21 @@
         <v>63</v>
       </c>
       <c r="J22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="O22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="4">
         <v>101</v>
@@ -1878,7 +1994,7 @@
       <c r="E23">
         <v>1200</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G23">
@@ -1900,9 +2016,9 @@
         <v>800</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="4">
         <v>101</v>
@@ -1916,7 +2032,7 @@
       <c r="E24">
         <v>1200</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G24">
@@ -1938,9 +2054,9 @@
         <v>600</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="4">
         <v>101</v>
@@ -1954,7 +2070,7 @@
       <c r="E25">
         <v>1200</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G25">
@@ -1976,9 +2092,9 @@
         <v>17500</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="4">
         <v>101</v>
@@ -1992,7 +2108,7 @@
       <c r="E26">
         <v>1200</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G26">
@@ -2014,42 +2130,158 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="4">
+        <v>101</v>
+      </c>
+      <c r="C28" s="4">
+        <v>601</v>
+      </c>
+      <c r="D28">
+        <v>400</v>
+      </c>
+      <c r="E28">
+        <v>1200</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>70</v>
+      </c>
+      <c r="H28" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="I28" s="3">
+        <v>63</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="K28">
+        <v>6.9</v>
+      </c>
+      <c r="L28">
+        <v>17500</v>
+      </c>
+      <c r="N28" t="s">
+        <v>61</v>
+      </c>
+      <c r="O28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="4">
+        <v>101</v>
+      </c>
+      <c r="C29" s="4">
+        <v>601</v>
+      </c>
+      <c r="D29">
+        <v>400</v>
+      </c>
+      <c r="E29">
+        <v>1200</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>70</v>
+      </c>
+      <c r="H29" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="I29" s="3">
+        <v>20.6</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="K29" s="4">
+        <v>0</v>
+      </c>
+      <c r="L29" s="4">
+        <v>700</v>
+      </c>
+      <c r="N29" t="s">
+        <v>62</v>
+      </c>
+      <c r="O29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="4">
+        <v>101</v>
+      </c>
+      <c r="C30" s="4">
+        <v>601</v>
+      </c>
+      <c r="D30">
+        <v>400</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <v>0.7</v>
+      </c>
+      <c r="G30">
+        <v>70</v>
+      </c>
+      <c r="H30" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="I30" s="3">
+        <v>20.6</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="K30" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="L30" s="4">
+        <v>7000</v>
+      </c>
+      <c r="N30" t="s">
+        <v>63</v>
+      </c>
+      <c r="O30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I32" s="3"/>
     </row>
@@ -2058,7 +2290,7 @@
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I33" s="3"/>
     </row>
@@ -2099,8 +2331,8 @@
       <c r="I39" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:N19" xr:uid="{49361AC2-0FC4-4902-86C7-B4FB07E48568}">
-    <sortState ref="A3:N18">
+  <autoFilter ref="A2:O19" xr:uid="{49361AC2-0FC4-4902-86C7-B4FB07E48568}">
+    <sortState ref="A3:O18">
       <sortCondition ref="K2:K18"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Move ignition conditions and how to calculate thermal properties to input file; working
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\School\Research\2D_Conduction\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF501470-BA1D-46A5-9CA1-9B428A31ECF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27742006-793B-414B-A9DA-224DEF56F14D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="65">
   <si>
     <t>Folder ID</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>6.08 (L)</t>
+  </si>
+  <si>
+    <t>Conserv-4</t>
   </si>
 </sst>
 </file>
@@ -1059,8 +1062,8 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2271,27 +2274,41 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="I31" s="3"/>
+      <c r="A31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="4">
+        <v>101</v>
+      </c>
+      <c r="C31" s="4">
+        <v>601</v>
+      </c>
+      <c r="D31">
+        <v>400</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>70</v>
+      </c>
+      <c r="H31" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="I31" s="3">
+        <v>20.6</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" t="s">
-        <v>37</v>
-      </c>
       <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" t="s">
-        <v>38</v>
-      </c>
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2322,12 +2339,18 @@
       <c r="A38" s="6"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
+      <c r="D38" t="s">
+        <v>37</v>
+      </c>
       <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
       <c r="I39" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Batch solving and output ignition and solver times to input file; keyboardInterrupt NOT accounted for
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27742006-793B-414B-A9DA-224DEF56F14D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DBC25B-EE62-44D9-BFE5-FE422A741ECB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="67">
   <si>
     <t>Folder ID</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>Conserv-4</t>
+  </si>
+  <si>
+    <t>Conserv-5</t>
+  </si>
+  <si>
+    <t>Conserv-6</t>
   </si>
 </sst>
 </file>
@@ -1062,8 +1068,8 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2289,6 +2295,9 @@
       <c r="E31" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F31">
+        <v>0.8</v>
+      </c>
       <c r="G31">
         <v>70</v>
       </c>
@@ -2298,44 +2307,141 @@
       <c r="I31" s="3">
         <v>20.6</v>
       </c>
+      <c r="J31" s="4">
+        <v>0.27</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="8">
+        <v>101</v>
+      </c>
+      <c r="C32" s="8">
+        <v>601</v>
+      </c>
+      <c r="D32">
+        <v>400</v>
+      </c>
+      <c r="E32">
+        <v>800</v>
+      </c>
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <v>70</v>
+      </c>
+      <c r="H32" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="I32" s="3">
+        <v>63</v>
+      </c>
+      <c r="J32" s="4">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="8">
+        <v>101</v>
+      </c>
+      <c r="C33" s="8">
+        <v>601</v>
+      </c>
+      <c r="D33">
+        <v>400</v>
+      </c>
+      <c r="E33">
+        <v>800</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>48</v>
+      </c>
+      <c r="H33" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="I33" s="3">
+        <v>63</v>
+      </c>
+      <c r="J33" s="4">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="8">
+        <v>101</v>
+      </c>
+      <c r="C34" s="8">
+        <v>601</v>
+      </c>
+      <c r="D34">
+        <v>400</v>
+      </c>
+      <c r="E34">
+        <v>1200</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34">
+        <v>48</v>
+      </c>
+      <c r="H34" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="I34" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="8">
+        <v>101</v>
+      </c>
+      <c r="C35" s="8">
+        <v>601</v>
+      </c>
+      <c r="D35">
+        <v>200</v>
+      </c>
+      <c r="E35">
+        <v>1200</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>48</v>
+      </c>
+      <c r="H35" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="I35" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2344,7 +2450,7 @@
       </c>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>

</xml_diff>

<commit_message>
Combustion wave speed calculator; output to console and input file
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\School\Research\2D_Conduction\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D512A2E-4C3A-41FB-9852-877BF3290747}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AFE9C0-8426-40AF-A78B-6536D4AF9718}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="77">
   <si>
     <t>Folder ID</t>
   </si>
@@ -147,12 +147,6 @@
     <t>Max Temp [K]</t>
   </si>
   <si>
-    <t>Conclusions:</t>
-  </si>
-  <si>
-    <t>T&gt;=2500 K for v&gt;0</t>
-  </si>
-  <si>
     <t>Mesh-1</t>
   </si>
   <si>
@@ -235,6 +229,42 @@
   </si>
   <si>
     <t>Conserv-6</t>
+  </si>
+  <si>
+    <t>Conserv-7</t>
+  </si>
+  <si>
+    <t>Conserv-8</t>
+  </si>
+  <si>
+    <t>Conserv-9</t>
+  </si>
+  <si>
+    <t>Run time/1000 time steps (min)</t>
+  </si>
+  <si>
+    <t>6.9 (6.9)</t>
+  </si>
+  <si>
+    <t>0 (0.006)</t>
+  </si>
+  <si>
+    <t>2.9 (2.9)</t>
+  </si>
+  <si>
+    <t>0 (0.003)</t>
+  </si>
+  <si>
+    <t>0 (0.009)</t>
+  </si>
+  <si>
+    <t>9.3 (8.8)</t>
+  </si>
+  <si>
+    <t>8.7 (8.8)</t>
+  </si>
+  <si>
+    <t>5.2 (4.9)</t>
   </si>
 </sst>
 </file>
@@ -651,7 +681,7 @@
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="3"/>
@@ -670,19 +700,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
@@ -712,10 +742,10 @@
         <v>36</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>21</v>
@@ -1015,7 +1045,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1089,17 +1119,17 @@
     </row>
     <row r="28" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1110,11 +1140,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9188EC-3268-404A-8733-94DAF537670F}">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,10 +1174,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1177,10 +1207,10 @@
         <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="O2" t="s">
         <v>21</v>
@@ -1226,7 +1256,7 @@
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1269,7 +1299,7 @@
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1312,7 +1342,7 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1355,7 +1385,7 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1398,7 +1428,7 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1439,7 +1469,7 @@
         <v>2500</v>
       </c>
       <c r="O8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1480,7 +1510,7 @@
         <v>9000</v>
       </c>
       <c r="O9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1523,7 +1553,7 @@
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1566,7 +1596,7 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1609,7 +1639,7 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1652,7 +1682,7 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1695,7 +1725,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1738,7 +1768,7 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1781,7 +1811,7 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1824,7 +1854,7 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1867,12 +1897,12 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="4">
         <v>101</v>
@@ -1910,12 +1940,12 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20" s="4">
         <v>101</v>
@@ -1951,7 +1981,7 @@
         <v>700</v>
       </c>
       <c r="O20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1981,16 +2011,16 @@
         <v>63</v>
       </c>
       <c r="J21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2020,21 +2050,21 @@
         <v>63</v>
       </c>
       <c r="J22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" s="4">
         <v>101</v>
@@ -2072,7 +2102,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="4">
         <v>101</v>
@@ -2110,7 +2140,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" s="4">
         <v>101</v>
@@ -2148,7 +2178,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="4">
         <v>101</v>
@@ -2186,7 +2216,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2194,7 +2224,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="4">
         <v>101</v>
@@ -2223,22 +2253,19 @@
       <c r="J28" s="4">
         <v>0.17</v>
       </c>
-      <c r="K28">
-        <v>6.9</v>
+      <c r="K28" t="s">
+        <v>69</v>
       </c>
       <c r="L28">
         <v>17500</v>
       </c>
-      <c r="N28" t="s">
-        <v>61</v>
-      </c>
       <c r="O28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B29" s="4">
         <v>101</v>
@@ -2267,22 +2294,19 @@
       <c r="J29" s="4">
         <v>0.24</v>
       </c>
-      <c r="K29" s="4">
-        <v>0</v>
+      <c r="K29" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="L29" s="4">
         <v>700</v>
       </c>
-      <c r="N29" t="s">
-        <v>62</v>
-      </c>
       <c r="O29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B30" s="4">
         <v>101</v>
@@ -2311,22 +2335,19 @@
       <c r="J30" s="4">
         <v>0.27</v>
       </c>
-      <c r="K30" s="4">
-        <v>2.9</v>
+      <c r="K30" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="L30" s="4">
         <v>7000</v>
       </c>
-      <c r="N30" t="s">
-        <v>63</v>
-      </c>
       <c r="O30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B31" s="4">
         <v>101</v>
@@ -2355,19 +2376,19 @@
       <c r="J31" s="4">
         <v>0.27</v>
       </c>
-      <c r="K31" s="4">
-        <v>2.9</v>
+      <c r="K31" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="L31" s="4">
         <v>7000</v>
       </c>
       <c r="O31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B32" s="8">
         <v>101</v>
@@ -2396,19 +2417,19 @@
       <c r="J32" s="4">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="K32" s="4">
-        <v>0</v>
+      <c r="K32" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="L32" s="4">
         <v>400</v>
       </c>
       <c r="O32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B33" s="8">
         <v>101</v>
@@ -2437,18 +2458,20 @@
       <c r="J33" s="4">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="K33" s="4">
-        <v>0</v>
+      <c r="K33" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="L33" s="4">
         <v>368</v>
       </c>
       <c r="O33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
+      <c r="A34" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="B34" s="8">
         <v>101</v>
       </c>
@@ -2473,12 +2496,23 @@
       <c r="I34" s="3">
         <v>63</v>
       </c>
+      <c r="J34" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L34" s="4">
+        <v>20000</v>
+      </c>
       <c r="O34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
+      <c r="A35" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="B35" s="8">
         <v>101</v>
       </c>
@@ -2503,12 +2537,23 @@
       <c r="I35" s="3">
         <v>63</v>
       </c>
+      <c r="J35" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L35" s="4">
+        <v>20000</v>
+      </c>
       <c r="O35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
+      <c r="A36" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="B36" s="8">
         <v>101</v>
       </c>
@@ -2533,8 +2578,17 @@
       <c r="I36" s="7">
         <v>4.07</v>
       </c>
+      <c r="J36" s="4">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="K36" t="s">
+        <v>76</v>
+      </c>
+      <c r="L36" s="4">
+        <v>8000</v>
+      </c>
       <c r="O36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -2547,19 +2601,301 @@
       <c r="A38" s="6"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
-      <c r="D38" t="s">
-        <v>37</v>
-      </c>
       <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" t="s">
-        <v>38</v>
-      </c>
       <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="6"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="I57" s="3"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="6"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="I58" s="3"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="I59" s="3"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="6"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="I60" s="3"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="I61" s="3"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="6"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="I62" s="3"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="6"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="I63" s="3"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="6"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="I64" s="3"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="6"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="I65" s="3"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="6"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="I66" s="3"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="I67" s="3"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="I68" s="3"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="6"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="I69" s="3"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="I70" s="3"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="6"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="6"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="6"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="I74" s="3"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="6"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="I75" s="3"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="6"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="I76" s="3"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="6"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="I77" s="3"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="6"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="I78" s="3"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="6"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="I79" s="3"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="6"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="I80" s="3"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="6"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="I81" s="3"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="6"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="I82" s="3"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="6"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="I83" s="3"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="6"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="I84" s="3"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="6"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="I85" s="3"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="6"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="I86" s="3"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="6"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="I87" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:O19" xr:uid="{49361AC2-0FC4-4902-86C7-B4FB07E48568}">

</xml_diff>

<commit_message>
Add source term model from Umbrajkar; is too slow
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\School\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AFE9C0-8426-40AF-A78B-6536D4AF9718}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DB42AD-FD04-4F8D-950D-37C79531AB6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="VarPropEta" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$O$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$O$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1143,8 +1143,8 @@
   <dimension ref="A1:O87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H71" sqref="H71"/>
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,7 +1548,7 @@
         <v>6.9</v>
       </c>
       <c r="L10" s="11">
-        <v>22500</v>
+        <v>20000</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -2898,7 +2898,7 @@
       <c r="I87" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:O19" xr:uid="{49361AC2-0FC4-4902-86C7-B4FB07E48568}">
+  <autoFilter ref="A2:O36" xr:uid="{49361AC2-0FC4-4902-86C7-B4FB07E48568}">
     <sortState ref="A3:O18">
       <sortCondition ref="K2:K18"/>
     </sortState>

</xml_diff>

<commit_message>
Testing code; also with Al-MoO3
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\School\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DB42AD-FD04-4F8D-950D-37C79531AB6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BA303F-A3E0-4500-8BCA-384C2E0A15C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
   <sheets>
     <sheet name="ConstantProp" sheetId="1" r:id="rId1"/>
     <sheet name="VarPropEta" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$O$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$O$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="79">
   <si>
     <t>Folder ID</t>
   </si>
@@ -243,38 +243,50 @@
     <t>Run time/1000 time steps (min)</t>
   </si>
   <si>
-    <t>6.9 (6.9)</t>
-  </si>
-  <si>
-    <t>0 (0.006)</t>
-  </si>
-  <si>
-    <t>2.9 (2.9)</t>
-  </si>
-  <si>
-    <t>0 (0.003)</t>
-  </si>
-  <si>
-    <t>0 (0.009)</t>
-  </si>
-  <si>
-    <t>9.3 (8.8)</t>
-  </si>
-  <si>
-    <t>8.7 (8.8)</t>
-  </si>
-  <si>
-    <t>5.2 (4.9)</t>
+    <t>Conserv-10</t>
+  </si>
+  <si>
+    <t>Conserv-11</t>
+  </si>
+  <si>
+    <t>0.167 (WU)</t>
+  </si>
+  <si>
+    <t>WW-Win10,WU-Ubuntu, L-laptop</t>
+  </si>
+  <si>
+    <t>0.158 (WU)</t>
+  </si>
+  <si>
+    <t>Conserv-12</t>
+  </si>
+  <si>
+    <t>0.159 (WU)</t>
+  </si>
+  <si>
+    <t>AlMoO3-1</t>
+  </si>
+  <si>
+    <t>dH from Kim 2014 [units of MJ/kg]</t>
+  </si>
+  <si>
+    <t>AlMoO3-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -321,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -340,6 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,12 +669,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3C7F47-CBB8-4962-A50C-2146AC268A42}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -1056,23 +1070,84 @@
       <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="3"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1523</v>
+      </c>
+      <c r="C11" s="8">
+        <v>625</v>
+      </c>
+      <c r="D11" s="3">
+        <v>156</v>
+      </c>
+      <c r="E11" s="8">
+        <v>101</v>
+      </c>
+      <c r="F11" s="8">
+        <v>601</v>
+      </c>
+      <c r="G11">
+        <v>200</v>
+      </c>
+      <c r="H11">
+        <v>1200</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <v>70</v>
+      </c>
+      <c r="K11" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L11" s="14">
+        <v>4.7</v>
+      </c>
       <c r="Q11" s="4"/>
+      <c r="R11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="3"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1523</v>
+      </c>
+      <c r="C12" s="8">
+        <v>625</v>
+      </c>
+      <c r="D12" s="3">
+        <v>156</v>
+      </c>
+      <c r="E12" s="8">
+        <v>101</v>
+      </c>
+      <c r="F12" s="8">
+        <v>601</v>
+      </c>
+      <c r="G12">
+        <v>200</v>
+      </c>
+      <c r="H12">
+        <v>1200</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="8">
+        <v>48</v>
+      </c>
+      <c r="K12" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L12" s="14">
+        <v>4.7</v>
+      </c>
       <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1142,14 +1217,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9188EC-3268-404A-8733-94DAF537670F}">
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -1168,6 +1243,9 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
+      <c r="N1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2253,8 +2331,8 @@
       <c r="J28" s="4">
         <v>0.17</v>
       </c>
-      <c r="K28" t="s">
-        <v>69</v>
+      <c r="K28">
+        <v>6.9</v>
       </c>
       <c r="L28">
         <v>17500</v>
@@ -2294,8 +2372,8 @@
       <c r="J29" s="4">
         <v>0.24</v>
       </c>
-      <c r="K29" s="4" t="s">
-        <v>70</v>
+      <c r="K29" s="4">
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="L29" s="4">
         <v>700</v>
@@ -2335,8 +2413,8 @@
       <c r="J30" s="4">
         <v>0.27</v>
       </c>
-      <c r="K30" s="4" t="s">
-        <v>71</v>
+      <c r="K30" s="4">
+        <v>2.9</v>
       </c>
       <c r="L30" s="4">
         <v>7000</v>
@@ -2376,8 +2454,8 @@
       <c r="J31" s="4">
         <v>0.27</v>
       </c>
-      <c r="K31" s="4" t="s">
-        <v>71</v>
+      <c r="K31" s="4">
+        <v>2.9</v>
       </c>
       <c r="L31" s="4">
         <v>7000</v>
@@ -2417,8 +2495,8 @@
       <c r="J32" s="4">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="K32" s="4" t="s">
-        <v>72</v>
+      <c r="K32" s="4">
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="L32" s="4">
         <v>400</v>
@@ -2458,8 +2536,8 @@
       <c r="J33" s="4">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="K33" s="4" t="s">
-        <v>73</v>
+      <c r="K33" s="4">
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="L33" s="4">
         <v>368</v>
@@ -2499,8 +2577,8 @@
       <c r="J34" s="4">
         <v>0.05</v>
       </c>
-      <c r="K34" s="4" t="s">
-        <v>74</v>
+      <c r="K34" s="4">
+        <v>8.8000000000000007</v>
       </c>
       <c r="L34" s="4">
         <v>20000</v>
@@ -2540,8 +2618,8 @@
       <c r="J35" s="4">
         <v>0.15</v>
       </c>
-      <c r="K35" s="4" t="s">
-        <v>75</v>
+      <c r="K35" s="4">
+        <v>8.8000000000000007</v>
       </c>
       <c r="L35" s="4">
         <v>20000</v>
@@ -2581,8 +2659,8 @@
       <c r="J36" s="4">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="K36" t="s">
-        <v>76</v>
+      <c r="K36">
+        <v>4.9000000000000004</v>
       </c>
       <c r="L36" s="4">
         <v>8000</v>
@@ -2592,22 +2670,127 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="I37" s="3"/>
+      <c r="A37" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="8">
+        <v>101</v>
+      </c>
+      <c r="C37" s="8">
+        <v>601</v>
+      </c>
+      <c r="D37">
+        <v>200</v>
+      </c>
+      <c r="E37">
+        <v>1200</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37">
+        <v>70</v>
+      </c>
+      <c r="H37" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="I37" s="3">
+        <v>63</v>
+      </c>
+      <c r="J37" s="4">
+        <v>0.54</v>
+      </c>
+      <c r="K37" s="4">
+        <v>6.9</v>
+      </c>
+      <c r="L37" s="4">
+        <v>17500</v>
+      </c>
+      <c r="N37" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="I38" s="3"/>
+      <c r="A38" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="8">
+        <v>101</v>
+      </c>
+      <c r="C38" s="8">
+        <v>601</v>
+      </c>
+      <c r="D38">
+        <v>200</v>
+      </c>
+      <c r="E38">
+        <v>1200</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38">
+        <v>70</v>
+      </c>
+      <c r="H38" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="I38" s="3">
+        <v>20.6</v>
+      </c>
+      <c r="J38" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="K38" s="4">
+        <v>2.76</v>
+      </c>
+      <c r="L38" s="4">
+        <v>6000</v>
+      </c>
+      <c r="N38" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="I39" s="3"/>
+      <c r="A39" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="8">
+        <v>101</v>
+      </c>
+      <c r="C39" s="8">
+        <v>601</v>
+      </c>
+      <c r="D39">
+        <v>200</v>
+      </c>
+      <c r="E39">
+        <v>1200</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39">
+        <v>48</v>
+      </c>
+      <c r="H39" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="I39" s="3">
+        <v>20.6</v>
+      </c>
+      <c r="J39" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="K39" s="4">
+        <v>4.28</v>
+      </c>
+      <c r="L39" s="4">
+        <v>6000</v>
+      </c>
+      <c r="N39" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
@@ -2898,7 +3081,7 @@
       <c r="I87" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:O36" xr:uid="{49361AC2-0FC4-4902-86C7-B4FB07E48568}">
+  <autoFilter ref="A2:O39" xr:uid="{49361AC2-0FC4-4902-86C7-B4FB07E48568}">
     <sortState ref="A3:O18">
       <sortCondition ref="K2:K18"/>
     </sortState>

</xml_diff>

<commit_message>
Testing AlMoO3 cases; comment out mass fraction variables
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\School\Research\2D_Conduction\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BA303F-A3E0-4500-8BCA-384C2E0A15C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1F159F-1205-4C53-A48E-B9EA07F47C21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
   <si>
     <t>Folder ID</t>
   </si>
@@ -267,10 +267,37 @@
     <t>AlMoO3-1</t>
   </si>
   <si>
-    <t>dH from Kim 2014 [units of MJ/kg]</t>
-  </si>
-  <si>
     <t>AlMoO3-2</t>
+  </si>
+  <si>
+    <t>AlMoO3-3</t>
+  </si>
+  <si>
+    <t>AlMoO3-4</t>
+  </si>
+  <si>
+    <t>AlMoO3-5</t>
+  </si>
+  <si>
+    <t>dH from Kim 2014 [MJ/kg], A0 from Stacy 2013; diverge at 0.23 ms because of eta</t>
+  </si>
+  <si>
+    <t>All values from from Stacy 2013; diverge at 0.032 ms because of eta</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>reduce k from AlMoO3-2; diverge at 0.024 ms (time step 7.9 us))</t>
+  </si>
+  <si>
+    <t>reduce k from AlMoO3-2;</t>
+  </si>
+  <si>
+    <t>try higher Ea; no ignition by 0.488 ms, 800 K (max)</t>
+  </si>
+  <si>
+    <t>dH from Kim 2014 [units of MJ/kg]; no ignition by 0.915 ms, 360 K (centreline), 10^-4 s^-1</t>
   </si>
 </sst>
 </file>
@@ -667,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3C7F47-CBB8-4962-A50C-2146AC268A42}">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,9 +1097,7 @@
       <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="A11" s="3"/>
       <c r="B11" s="8">
         <v>1523</v>
       </c>
@@ -1106,14 +1131,23 @@
       <c r="L11" s="14">
         <v>4.7</v>
       </c>
+      <c r="M11" t="s">
+        <v>83</v>
+      </c>
+      <c r="N11" t="s">
+        <v>83</v>
+      </c>
+      <c r="O11" t="s">
+        <v>83</v>
+      </c>
       <c r="Q11" s="4"/>
       <c r="R11" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="8">
         <v>1523</v>
@@ -1148,64 +1182,496 @@
       <c r="L12" s="14">
         <v>4.7</v>
       </c>
+      <c r="M12">
+        <v>0.44</v>
+      </c>
+      <c r="N12">
+        <v>21.2</v>
+      </c>
+      <c r="O12">
+        <v>8000</v>
+      </c>
       <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="3"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="8">
+        <v>3808</v>
+      </c>
+      <c r="C13" s="8">
+        <v>625</v>
+      </c>
+      <c r="D13" s="3">
+        <v>156</v>
+      </c>
+      <c r="E13" s="8">
+        <v>101</v>
+      </c>
+      <c r="F13" s="8">
+        <v>601</v>
+      </c>
+      <c r="G13">
+        <v>200</v>
+      </c>
+      <c r="H13">
+        <v>1200</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="8">
+        <v>48</v>
+      </c>
+      <c r="K13" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L13" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M13">
+        <v>0.67</v>
+      </c>
+      <c r="N13">
+        <v>12.7</v>
+      </c>
+      <c r="O13">
+        <v>8000</v>
+      </c>
       <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="3"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="3"/>
+      <c r="B14" s="8">
+        <v>1523</v>
+      </c>
+      <c r="C14" s="8">
+        <v>625</v>
+      </c>
+      <c r="D14" s="3">
+        <v>156</v>
+      </c>
+      <c r="E14" s="8">
+        <v>101</v>
+      </c>
+      <c r="F14" s="8">
+        <v>601</v>
+      </c>
+      <c r="G14">
+        <v>200</v>
+      </c>
+      <c r="H14">
+        <v>1200</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14">
+        <v>70</v>
+      </c>
+      <c r="K14" s="9">
+        <v>2200000000</v>
+      </c>
+      <c r="L14" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M14" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14" t="s">
+        <v>42</v>
+      </c>
       <c r="Q14" s="4"/>
+      <c r="R14" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="3"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2020</v>
+      </c>
+      <c r="C15" s="8">
+        <v>640</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E15" s="8">
+        <v>101</v>
+      </c>
+      <c r="F15" s="8">
+        <v>601</v>
+      </c>
+      <c r="G15">
+        <v>200</v>
+      </c>
+      <c r="H15">
+        <v>1200</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>106.2</v>
+      </c>
+      <c r="K15" s="9">
+        <v>2200000000</v>
+      </c>
+      <c r="L15" s="14">
+        <v>7.61</v>
+      </c>
+      <c r="M15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" t="s">
+        <v>42</v>
+      </c>
+      <c r="O15" t="s">
+        <v>42</v>
+      </c>
       <c r="Q15" s="4"/>
+      <c r="R15" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="8">
+        <v>1523</v>
+      </c>
+      <c r="C16" s="8">
+        <v>625</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E16" s="8">
+        <v>101</v>
+      </c>
+      <c r="F16" s="8">
+        <v>601</v>
+      </c>
+      <c r="G16">
+        <v>200</v>
+      </c>
+      <c r="H16">
+        <v>1200</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="8">
+        <v>48</v>
+      </c>
+      <c r="K16" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L16" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" t="s">
+        <v>42</v>
+      </c>
+      <c r="O16" t="s">
+        <v>42</v>
+      </c>
       <c r="Q16" s="4"/>
-    </row>
-    <row r="17" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1523</v>
+      </c>
+      <c r="C17" s="8">
+        <v>625</v>
+      </c>
+      <c r="D17" s="3">
+        <v>78</v>
+      </c>
+      <c r="E17" s="8">
+        <v>101</v>
+      </c>
+      <c r="F17" s="8">
+        <v>601</v>
+      </c>
+      <c r="G17">
+        <v>200</v>
+      </c>
+      <c r="H17">
+        <v>1200</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="8">
+        <v>48</v>
+      </c>
+      <c r="K17" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L17" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M17">
+        <v>0.18</v>
+      </c>
+      <c r="N17">
+        <v>14.2</v>
+      </c>
+      <c r="O17">
+        <v>8000</v>
+      </c>
       <c r="Q17" s="4"/>
-    </row>
-    <row r="18" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1523</v>
+      </c>
+      <c r="C18" s="8">
+        <v>625</v>
+      </c>
+      <c r="D18" s="3">
+        <v>78</v>
+      </c>
+      <c r="E18" s="8">
+        <v>101</v>
+      </c>
+      <c r="F18" s="8">
+        <v>601</v>
+      </c>
+      <c r="G18">
+        <v>200</v>
+      </c>
+      <c r="H18">
+        <v>1200</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="8">
+        <v>70</v>
+      </c>
+      <c r="K18" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L18" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M18" t="s">
+        <v>83</v>
+      </c>
+      <c r="N18" t="s">
+        <v>83</v>
+      </c>
+      <c r="O18" t="s">
+        <v>83</v>
+      </c>
       <c r="Q18" s="4"/>
-    </row>
-    <row r="19" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="3"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="3"/>
       <c r="Q19" s="4"/>
     </row>
-    <row r="28" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="3"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="3"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="3"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="3"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="3"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="3"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="3"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="3"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="3"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="3"/>
       <c r="Q28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="3"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="3"/>
       <c r="Q29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="3"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="3"/>
       <c r="Q30" t="s">
         <v>61</v>
       </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="3"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="3"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="3"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="3"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="3"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="3"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="3"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1218,8 +1684,8 @@
   <dimension ref="A1:O87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
More testing Al-MoO3; more promising results
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1F159F-1205-4C53-A48E-B9EA07F47C21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A725F6-D65E-482B-8712-B9816E116DBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="VarPropEta" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ConstantProp!$A$2:$R$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$O$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="95">
   <si>
     <t>Folder ID</t>
   </si>
@@ -213,15 +214,6 @@
     <t>Conserv-3</t>
   </si>
   <si>
-    <t>5.56 (L)</t>
-  </si>
-  <si>
-    <t>6.27 (L)</t>
-  </si>
-  <si>
-    <t>6.08 (L)</t>
-  </si>
-  <si>
     <t>Conserv-4</t>
   </si>
   <si>
@@ -279,9 +271,6 @@
     <t>AlMoO3-5</t>
   </si>
   <si>
-    <t>dH from Kim 2014 [MJ/kg], A0 from Stacy 2013; diverge at 0.23 ms because of eta</t>
-  </si>
-  <si>
     <t>All values from from Stacy 2013; diverge at 0.032 ms because of eta</t>
   </si>
   <si>
@@ -298,6 +287,39 @@
   </si>
   <si>
     <t>dH from Kim 2014 [units of MJ/kg]; no ignition by 0.915 ms, 360 K (centreline), 10^-4 s^-1</t>
+  </si>
+  <si>
+    <t>dH,Ea from Kim 2014; Ao from Stacy 2013</t>
+  </si>
+  <si>
+    <t>use rho_TMD instead</t>
+  </si>
+  <si>
+    <t>dH from Kim 2014, A0 from Stacy 2013; diverge at 0.23 ms because of eta</t>
+  </si>
+  <si>
+    <t>RED-MJ/kg</t>
+  </si>
+  <si>
+    <t>AlMoO3-6</t>
+  </si>
+  <si>
+    <t>use eta ign from AlMoO3-1</t>
+  </si>
+  <si>
+    <t>smaller A0 (Stacy 2013); no ignition by 0.37 ms, 780 K (max), 10^-3 s^-1</t>
+  </si>
+  <si>
+    <t>rho from Stacy 2013; rest from AlMoO3-6</t>
+  </si>
+  <si>
+    <t>k based on mass fraction of reactants;</t>
+  </si>
+  <si>
+    <t>AlMoO3-7</t>
+  </si>
+  <si>
+    <t>try higher Ea; ignition late and wave still developing by 0.777 ms</t>
   </si>
 </sst>
 </file>
@@ -694,10 +716,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3C7F47-CBB8-4962-A50C-2146AC268A42}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q28" sqref="Q28:Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +755,9 @@
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
-      <c r="L1" s="3"/>
+      <c r="L1" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="M1" t="s">
         <v>8</v>
       </c>
@@ -792,7 +818,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -834,7 +860,7 @@
       </c>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -876,7 +902,7 @@
       </c>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -918,7 +944,7 @@
       </c>
       <c r="Q5" s="4"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -960,7 +986,7 @@
       </c>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1002,7 +1028,7 @@
       </c>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1043,7 +1069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1084,7 +1110,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>51</v>
       </c>
@@ -1132,22 +1158,22 @@
         <v>4.7</v>
       </c>
       <c r="M11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="N11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="O11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="Q11" s="4"/>
       <c r="R11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B12" s="8">
         <v>1523</v>
@@ -1192,10 +1218,13 @@
         <v>8000</v>
       </c>
       <c r="Q12" s="4"/>
+      <c r="R12" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" s="8">
         <v>3808</v>
@@ -1240,6 +1269,9 @@
         <v>8000</v>
       </c>
       <c r="Q13" s="4"/>
+      <c r="R13" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -1287,13 +1319,11 @@
       </c>
       <c r="Q14" s="4"/>
       <c r="R14" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="A15" s="3"/>
       <c r="B15" s="8">
         <v>2020</v>
       </c>
@@ -1338,7 +1368,7 @@
       </c>
       <c r="Q15" s="4"/>
       <c r="R15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1387,12 +1417,12 @@
       </c>
       <c r="Q16" s="4"/>
       <c r="R16" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17" s="8">
         <v>1523</v>
@@ -1438,13 +1468,11 @@
       </c>
       <c r="Q17" s="4"/>
       <c r="R17" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="A18" s="3"/>
       <c r="B18" s="8">
         <v>1523</v>
       </c>
@@ -1479,64 +1507,267 @@
         <v>4.7</v>
       </c>
       <c r="M18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="N18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="O18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="Q18" s="4"/>
       <c r="R18" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="3"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="3"/>
+      <c r="B19" s="8">
+        <v>1523</v>
+      </c>
+      <c r="C19" s="8">
+        <v>625</v>
+      </c>
+      <c r="D19" s="3">
+        <v>78</v>
+      </c>
+      <c r="E19" s="8">
+        <v>101</v>
+      </c>
+      <c r="F19" s="8">
+        <v>601</v>
+      </c>
+      <c r="G19">
+        <v>200</v>
+      </c>
+      <c r="H19">
+        <v>1200</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="8">
+        <v>48</v>
+      </c>
+      <c r="K19" s="9">
+        <v>141000</v>
+      </c>
+      <c r="L19" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M19" t="s">
+        <v>79</v>
+      </c>
+      <c r="N19" t="s">
+        <v>79</v>
+      </c>
+      <c r="O19" t="s">
+        <v>79</v>
+      </c>
       <c r="Q19" s="4"/>
+      <c r="R19" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="3"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="3"/>
+      <c r="A20" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1523</v>
+      </c>
+      <c r="C20" s="8">
+        <v>625</v>
+      </c>
+      <c r="D20" s="3">
+        <v>78</v>
+      </c>
+      <c r="E20" s="8">
+        <v>101</v>
+      </c>
+      <c r="F20" s="8">
+        <v>601</v>
+      </c>
+      <c r="G20">
+        <v>200</v>
+      </c>
+      <c r="H20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J20" s="8">
+        <v>48</v>
+      </c>
+      <c r="K20" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L20" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M20">
+        <v>0.18</v>
+      </c>
+      <c r="N20">
+        <v>14.7</v>
+      </c>
+      <c r="O20">
+        <v>8000</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="3"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="3"/>
+      <c r="A21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="8">
+        <v>2020</v>
+      </c>
+      <c r="C21" s="8">
+        <v>625</v>
+      </c>
+      <c r="D21" s="3">
+        <v>78</v>
+      </c>
+      <c r="E21" s="8">
+        <v>101</v>
+      </c>
+      <c r="F21" s="8">
+        <v>601</v>
+      </c>
+      <c r="G21">
+        <v>200</v>
+      </c>
+      <c r="H21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J21" s="8">
+        <v>48</v>
+      </c>
+      <c r="K21" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L21" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M21">
+        <v>0.22</v>
+      </c>
+      <c r="N21">
+        <v>12.5</v>
+      </c>
+      <c r="O21">
+        <v>8000</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="3"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="3"/>
+      <c r="A22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="8">
+        <v>2020</v>
+      </c>
+      <c r="C22" s="8">
+        <v>625</v>
+      </c>
+      <c r="D22" s="3">
+        <v>65</v>
+      </c>
+      <c r="E22" s="8">
+        <v>101</v>
+      </c>
+      <c r="F22" s="8">
+        <v>601</v>
+      </c>
+      <c r="G22">
+        <v>200</v>
+      </c>
+      <c r="H22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J22" s="8">
+        <v>48</v>
+      </c>
+      <c r="K22" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L22" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M22">
+        <v>0.18</v>
+      </c>
+      <c r="N22">
+        <v>11.1</v>
+      </c>
+      <c r="O22">
+        <v>8000</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="3"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="3"/>
+      <c r="A23" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="8">
+        <v>2020</v>
+      </c>
+      <c r="C23" s="8">
+        <v>625</v>
+      </c>
+      <c r="D23" s="3">
+        <v>65</v>
+      </c>
+      <c r="E23" s="8">
+        <v>101</v>
+      </c>
+      <c r="F23" s="8">
+        <v>601</v>
+      </c>
+      <c r="G23">
+        <v>200</v>
+      </c>
+      <c r="H23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J23" s="8">
+        <v>70</v>
+      </c>
+      <c r="K23" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L23" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M23">
+        <v>0.73</v>
+      </c>
+      <c r="N23">
+        <v>3.14</v>
+      </c>
+      <c r="O23">
+        <v>8000</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
@@ -1582,9 +1813,6 @@
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="3"/>
-      <c r="Q28" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -1594,9 +1822,6 @@
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="L29" s="3"/>
-      <c r="Q29" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
@@ -1606,9 +1831,6 @@
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
       <c r="L30" s="3"/>
-      <c r="Q30" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -1674,6 +1896,18 @@
       <c r="L37" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:R22" xr:uid="{49C99752-6154-48AE-B9BC-04DA8123EC2F}">
+    <filterColumn colId="0">
+      <filters blank="1">
+        <filter val="AlMoO3-1"/>
+        <filter val="AlMoO3-2"/>
+        <filter val="AlMoO3-3"/>
+        <filter val="AlMoO3-4"/>
+        <filter val="AlMoO3-5"/>
+        <filter val="AlMoO3-6"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1710,7 +1944,7 @@
         <v>8</v>
       </c>
       <c r="N1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1754,7 +1988,7 @@
         <v>40</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O2" t="s">
         <v>21</v>
@@ -2891,7 +3125,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B31" s="4">
         <v>101</v>
@@ -2932,7 +3166,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B32" s="8">
         <v>101</v>
@@ -2973,7 +3207,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B33" s="8">
         <v>101</v>
@@ -3014,7 +3248,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B34" s="8">
         <v>101</v>
@@ -3055,7 +3289,7 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B35" s="8">
         <v>101</v>
@@ -3096,7 +3330,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B36" s="8">
         <v>101</v>
@@ -3137,7 +3371,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B37" s="8">
         <v>101</v>
@@ -3173,12 +3407,12 @@
         <v>17500</v>
       </c>
       <c r="N37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B38" s="8">
         <v>101</v>
@@ -3214,12 +3448,12 @@
         <v>6000</v>
       </c>
       <c r="N38" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B39" s="8">
         <v>101</v>
@@ -3255,7 +3489,7 @@
         <v>6000</v>
       </c>
       <c r="N39" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More testing with Al-MoO3
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A725F6-D65E-482B-8712-B9816E116DBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B68A38-ED60-4499-9F82-74858F2905D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="VarPropEta" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ConstantProp!$A$2:$R$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ConstantProp!$A$2:$R$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$O$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="99">
   <si>
     <t>Folder ID</t>
   </si>
@@ -286,9 +286,6 @@
     <t>try higher Ea; no ignition by 0.488 ms, 800 K (max)</t>
   </si>
   <si>
-    <t>dH from Kim 2014 [units of MJ/kg]; no ignition by 0.915 ms, 360 K (centreline), 10^-4 s^-1</t>
-  </si>
-  <si>
     <t>dH,Ea from Kim 2014; Ao from Stacy 2013</t>
   </si>
   <si>
@@ -307,9 +304,6 @@
     <t>use eta ign from AlMoO3-1</t>
   </si>
   <si>
-    <t>smaller A0 (Stacy 2013); no ignition by 0.37 ms, 780 K (max), 10^-3 s^-1</t>
-  </si>
-  <si>
     <t>rho from Stacy 2013; rest from AlMoO3-6</t>
   </si>
   <si>
@@ -319,7 +313,25 @@
     <t>AlMoO3-7</t>
   </si>
   <si>
-    <t>try higher Ea; ignition late and wave still developing by 0.777 ms</t>
+    <t>try higher Ea;</t>
+  </si>
+  <si>
+    <t>AlMoO3-8</t>
+  </si>
+  <si>
+    <t>AlMoO3-9</t>
+  </si>
+  <si>
+    <t>AlMoO3-10</t>
+  </si>
+  <si>
+    <t>AlMoO3-11</t>
+  </si>
+  <si>
+    <t>smaller A0 (Stacy 2013); combustion unsustainable</t>
+  </si>
+  <si>
+    <t>dH from Kim 2014 [units of MJ/kg]; no ignition by1.22 ms, 700 K (max), 24 s^-1</t>
   </si>
 </sst>
 </file>
@@ -719,14 +731,14 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q28" sqref="Q28:Q30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -756,7 +768,7 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
@@ -1123,7 +1135,9 @@
       <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="B11" s="8">
         <v>1523</v>
       </c>
@@ -1168,7 +1182,7 @@
       </c>
       <c r="Q11" s="4"/>
       <c r="R11" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1219,7 +1233,7 @@
       </c>
       <c r="Q12" s="4"/>
       <c r="R12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1270,10 +1284,10 @@
       </c>
       <c r="Q13" s="4"/>
       <c r="R13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="8">
         <v>1523</v>
@@ -1319,10 +1333,10 @@
       </c>
       <c r="Q14" s="4"/>
       <c r="R14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="8">
         <v>2020</v>
@@ -1371,7 +1385,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="8">
         <v>1523</v>
@@ -1472,7 +1486,9 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="B18" s="8">
         <v>1523</v>
       </c>
@@ -1506,14 +1522,14 @@
       <c r="L18" s="14">
         <v>4.7</v>
       </c>
-      <c r="M18" t="s">
-        <v>79</v>
-      </c>
-      <c r="N18" t="s">
-        <v>79</v>
-      </c>
-      <c r="O18" t="s">
-        <v>79</v>
+      <c r="M18">
+        <v>0.81</v>
+      </c>
+      <c r="N18">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="O18">
+        <v>8000</v>
       </c>
       <c r="Q18" s="4"/>
       <c r="R18" s="4" t="s">
@@ -1521,7 +1537,9 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="B19" s="8">
         <v>1523</v>
       </c>
@@ -1555,23 +1573,23 @@
       <c r="L19" s="14">
         <v>4.7</v>
       </c>
-      <c r="M19" t="s">
-        <v>79</v>
-      </c>
-      <c r="N19" t="s">
-        <v>79</v>
-      </c>
-      <c r="O19" t="s">
-        <v>79</v>
+      <c r="M19">
+        <v>1.01</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>1200</v>
       </c>
       <c r="Q19" s="4"/>
       <c r="R19" s="4" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="8">
         <v>1523</v>
@@ -1616,7 +1634,7 @@
         <v>8000</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -1666,7 +1684,7 @@
         <v>8000</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -1716,12 +1734,12 @@
         <v>8000</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B23" s="8">
         <v>2020</v>
@@ -1760,32 +1778,90 @@
         <v>0.73</v>
       </c>
       <c r="N23">
-        <v>3.14</v>
+        <v>8.1</v>
       </c>
       <c r="O23">
         <v>8000</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="3"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="3"/>
+      <c r="A24" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C24" s="4">
+        <v>625</v>
+      </c>
+      <c r="D24" s="3">
+        <v>65</v>
+      </c>
+      <c r="E24" s="8">
+        <v>101</v>
+      </c>
+      <c r="F24" s="8">
+        <v>601</v>
+      </c>
+      <c r="G24">
+        <v>200</v>
+      </c>
+      <c r="H24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J24" s="8">
+        <v>70</v>
+      </c>
+      <c r="K24" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L24" s="14">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="3"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="3"/>
+      <c r="A25" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C25" s="4">
+        <v>625</v>
+      </c>
+      <c r="D25" s="3">
+        <v>65</v>
+      </c>
+      <c r="E25" s="8">
+        <v>101</v>
+      </c>
+      <c r="F25" s="8">
+        <v>601</v>
+      </c>
+      <c r="G25">
+        <v>200</v>
+      </c>
+      <c r="H25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J25" s="8">
+        <v>48</v>
+      </c>
+      <c r="K25" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L25" s="14">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -1896,15 +1972,32 @@
       <c r="L37" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:R22" xr:uid="{49C99752-6154-48AE-B9BC-04DA8123EC2F}">
+  <autoFilter ref="A2:R25" xr:uid="{49C99752-6154-48AE-B9BC-04DA8123EC2F}">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="AlMoO3-1"/>
+        <filter val="AlMoO3-10"/>
+        <filter val="AlMoO3-11"/>
         <filter val="AlMoO3-2"/>
         <filter val="AlMoO3-3"/>
         <filter val="AlMoO3-4"/>
         <filter val="AlMoO3-5"/>
         <filter val="AlMoO3-6"/>
+        <filter val="AlMoO3-7"/>
+        <filter val="AlMoO3-8"/>
+        <filter val="AlMoO3-9"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="12">
+      <filters blank="1">
+        <filter val="-"/>
+        <filter val="0.18"/>
+        <filter val="0.22"/>
+        <filter val="0.44"/>
+        <filter val="0.67"/>
+        <filter val="0.73"/>
+        <filter val="0.81"/>
+        <filter val="1.01"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
More testing of Al-MoO3
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\School\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B68A38-ED60-4499-9F82-74858F2905D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A5760E-63C2-48CE-8AD2-EAF4C2569E78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
   <sheets>
     <sheet name="ConstantProp" sheetId="1" r:id="rId1"/>
     <sheet name="VarPropEta" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ConstantProp!$A$2:$R$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ConstantProp!$A$2:$R$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$O$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="110">
   <si>
     <t>Folder ID</t>
   </si>
@@ -332,6 +332,39 @@
   </si>
   <si>
     <t>dH from Kim 2014 [units of MJ/kg]; no ignition by1.22 ms, 700 K (max), 24 s^-1</t>
+  </si>
+  <si>
+    <t>AlMoO3-12</t>
+  </si>
+  <si>
+    <t>Higher A0 from case 8 (try and match t_ign)</t>
+  </si>
+  <si>
+    <t>Even higher A0 from case 12</t>
+  </si>
+  <si>
+    <t>AlMoO3-13</t>
+  </si>
+  <si>
+    <t>AlMoO3-14</t>
+  </si>
+  <si>
+    <t>0.15 (WU)</t>
+  </si>
+  <si>
+    <t>Even higher A0 from case 13</t>
+  </si>
+  <si>
+    <t>AlMoO3-15</t>
+  </si>
+  <si>
+    <t>Based on linear changes, estimated A0 to get t_ign</t>
+  </si>
+  <si>
+    <t>AlMoO3-16</t>
+  </si>
+  <si>
+    <t>Higher A0;</t>
   </si>
 </sst>
 </file>
@@ -394,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -414,6 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,9 +765,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20:G20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D11:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,9 +1169,7 @@
       <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="A11" s="3"/>
       <c r="B11" s="8">
         <v>1523</v>
       </c>
@@ -1287,7 +1319,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="8">
         <v>1523</v>
@@ -1336,7 +1368,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="8">
         <v>2020</v>
@@ -1385,7 +1417,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="8">
         <v>1523</v>
@@ -1824,6 +1856,15 @@
       <c r="L24" s="14">
         <v>4.7</v>
       </c>
+      <c r="M24">
+        <v>0.62</v>
+      </c>
+      <c r="N24">
+        <v>9.6</v>
+      </c>
+      <c r="O24">
+        <v>8000</v>
+      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -1862,51 +1903,241 @@
       <c r="L25" s="14">
         <v>4.7</v>
       </c>
+      <c r="M25">
+        <v>0.15</v>
+      </c>
+      <c r="N25">
+        <v>13.2</v>
+      </c>
+      <c r="O25">
+        <v>8000</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="3"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="3"/>
+      <c r="A26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C26" s="4">
+        <v>625</v>
+      </c>
+      <c r="D26" s="3">
+        <v>65</v>
+      </c>
+      <c r="E26" s="8">
+        <v>101</v>
+      </c>
+      <c r="F26" s="8">
+        <v>601</v>
+      </c>
+      <c r="G26">
+        <v>200</v>
+      </c>
+      <c r="H26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J26" s="8">
+        <v>70</v>
+      </c>
+      <c r="K26" s="2">
+        <v>5000000</v>
+      </c>
+      <c r="L26" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M26">
+        <v>0.61</v>
+      </c>
+      <c r="N26">
+        <v>9.6</v>
+      </c>
+      <c r="O26">
+        <v>8000</v>
+      </c>
+      <c r="R26" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="3"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="3"/>
+      <c r="A27" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C27" s="4">
+        <v>625</v>
+      </c>
+      <c r="D27" s="3">
+        <v>65</v>
+      </c>
+      <c r="E27" s="8">
+        <v>101</v>
+      </c>
+      <c r="F27" s="8">
+        <v>601</v>
+      </c>
+      <c r="G27">
+        <v>200</v>
+      </c>
+      <c r="H27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J27" s="8">
+        <v>70</v>
+      </c>
+      <c r="K27" s="2">
+        <v>5500000</v>
+      </c>
+      <c r="L27" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M27">
+        <v>0.59</v>
+      </c>
+      <c r="N27">
+        <v>10.1</v>
+      </c>
+      <c r="O27">
+        <v>8000</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>104</v>
+      </c>
+      <c r="R27" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="3"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="3"/>
+      <c r="A28" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C28" s="4">
+        <v>625</v>
+      </c>
+      <c r="D28" s="3">
+        <v>65</v>
+      </c>
+      <c r="E28" s="8">
+        <v>101</v>
+      </c>
+      <c r="F28" s="8">
+        <v>601</v>
+      </c>
+      <c r="G28">
+        <v>200</v>
+      </c>
+      <c r="H28" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J28" s="8">
+        <v>70</v>
+      </c>
+      <c r="K28" s="2">
+        <v>6000000</v>
+      </c>
+      <c r="L28" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M28">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="N28">
+        <v>10.4</v>
+      </c>
+      <c r="O28">
+        <v>8000</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>104</v>
+      </c>
+      <c r="R28" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="3"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="3"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+      <c r="A29" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C29" s="4">
+        <v>625</v>
+      </c>
+      <c r="D29" s="3">
+        <v>65</v>
+      </c>
+      <c r="E29" s="8">
+        <v>101</v>
+      </c>
+      <c r="F29" s="8">
+        <v>601</v>
+      </c>
+      <c r="G29">
+        <v>200</v>
+      </c>
+      <c r="H29" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J29" s="8">
+        <v>70</v>
+      </c>
+      <c r="K29" s="2">
+        <v>8000000</v>
+      </c>
+      <c r="L29" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M29">
+        <v>0.5</v>
+      </c>
+      <c r="N29">
+        <v>11.7</v>
+      </c>
+      <c r="O29">
+        <v>8000</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>104</v>
+      </c>
+      <c r="R29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
       <c r="D30" s="3"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="I30" s="1"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="3"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="15"/>
+      <c r="R30" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -1972,12 +2203,16 @@
       <c r="L37" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:R25" xr:uid="{49C99752-6154-48AE-B9BC-04DA8123EC2F}">
+  <autoFilter ref="A2:R30" xr:uid="{49C99752-6154-48AE-B9BC-04DA8123EC2F}">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="AlMoO3-1"/>
         <filter val="AlMoO3-10"/>
         <filter val="AlMoO3-11"/>
+        <filter val="AlMoO3-12"/>
+        <filter val="AlMoO3-13"/>
+        <filter val="AlMoO3-14"/>
+        <filter val="AlMoO3-15"/>
         <filter val="AlMoO3-2"/>
         <filter val="AlMoO3-3"/>
         <filter val="AlMoO3-4"/>
@@ -1986,18 +2221,6 @@
         <filter val="AlMoO3-7"/>
         <filter val="AlMoO3-8"/>
         <filter val="AlMoO3-9"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="12">
-      <filters blank="1">
-        <filter val="-"/>
-        <filter val="0.18"/>
-        <filter val="0.22"/>
-        <filter val="0.44"/>
-        <filter val="0.67"/>
-        <filter val="0.73"/>
-        <filter val="0.81"/>
-        <filter val="1.01"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2010,9 +2233,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9188EC-3268-404A-8733-94DAF537670F}">
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
More testing with AlMoO3; proper flux BC implemented
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF28513-AF5F-407C-BF92-5B42E5981467}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0190D2-0D3E-4F4A-B5B4-4C40ACF807E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="130">
   <si>
     <t>Folder ID</t>
   </si>
@@ -419,6 +419,12 @@
   </si>
   <si>
     <t>Reaction Rate peak (s^-1)</t>
+  </si>
+  <si>
+    <t>0.64 (WU), 1.8 (WW)</t>
+  </si>
+  <si>
+    <t>No ignition after 1.07ms;</t>
   </si>
 </sst>
 </file>
@@ -2232,13 +2238,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9.1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2330,13 +2336,13 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="3"/>
                       <c:pt idx="0">
-                        <c:v>0.44</c:v>
+                        <c:v>0.63</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>0.49</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.62</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2697,16 +2703,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7.5</c:v>
+                  <c:v>7.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.5</c:v>
+                  <c:v>10.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2801,16 +2807,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>0.48</c:v>
+                        <c:v>0.72</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.46</c:v>
+                        <c:v>0.68</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.44</c:v>
+                        <c:v>0.63</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.43</c:v>
+                        <c:v>0.62</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -6308,7 +6314,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7503,6 +7509,11 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="3"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="2"/>
       <c r="L27" s="14"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -7623,10 +7634,10 @@
         <v>4</v>
       </c>
       <c r="M32">
-        <v>0.46</v>
+        <v>0.68</v>
       </c>
       <c r="N32">
-        <v>8.6</v>
+        <v>8.5</v>
       </c>
       <c r="O32">
         <v>6600</v>
@@ -7673,10 +7684,10 @@
         <v>5</v>
       </c>
       <c r="M33">
-        <v>0.43</v>
+        <v>0.62</v>
       </c>
       <c r="N33">
-        <v>10.5</v>
+        <v>10.6</v>
       </c>
       <c r="O33">
         <v>8100</v>
@@ -7722,17 +7733,20 @@
       <c r="L34" s="14">
         <v>4.7</v>
       </c>
-      <c r="M34">
-        <v>0.62</v>
-      </c>
-      <c r="N34">
-        <v>11.6</v>
-      </c>
-      <c r="O34">
-        <v>7600</v>
+      <c r="M34" t="s">
+        <v>79</v>
+      </c>
+      <c r="N34" t="s">
+        <v>79</v>
+      </c>
+      <c r="O34" t="s">
+        <v>79</v>
       </c>
       <c r="Q34" t="s">
-        <v>122</v>
+        <v>128</v>
+      </c>
+      <c r="R34" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -7773,10 +7787,10 @@
         <v>3.5</v>
       </c>
       <c r="M35">
-        <v>0.48</v>
+        <v>0.72</v>
       </c>
       <c r="N35">
-        <v>7.5</v>
+        <v>7.4</v>
       </c>
       <c r="O35">
         <v>6000</v>
@@ -8138,13 +8152,13 @@
         <v>4.7</v>
       </c>
       <c r="M44" s="12">
-        <v>0.44</v>
+        <v>0.63</v>
       </c>
       <c r="N44" s="12">
-        <v>9.1</v>
+        <v>10</v>
       </c>
       <c r="O44" s="12">
-        <v>7600</v>
+        <v>7800</v>
       </c>
       <c r="P44" s="2">
         <v>600000</v>

</xml_diff>

<commit_message>
More testing AlMoO3, Ea=48
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0190D2-0D3E-4F4A-B5B4-4C40ACF807E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F0CA89-DDAB-4809-8E52-AB6B8BD9256C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="133">
   <si>
     <t>Folder ID</t>
   </si>
@@ -425,6 +425,15 @@
   </si>
   <si>
     <t>No ignition after 1.07ms;</t>
+  </si>
+  <si>
+    <t>0.66 (WW)</t>
+  </si>
+  <si>
+    <t>0.71 (WW)</t>
+  </si>
+  <si>
+    <t>0.63 (WW)</t>
   </si>
 </sst>
 </file>
@@ -6311,10 +6320,10 @@
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7506,42 +7515,210 @@
       <c r="A27" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="14"/>
+      <c r="B27" s="8">
+        <v>1523</v>
+      </c>
+      <c r="C27" s="8">
+        <v>625</v>
+      </c>
+      <c r="D27" s="3">
+        <v>100</v>
+      </c>
+      <c r="E27" s="8">
+        <v>101</v>
+      </c>
+      <c r="F27" s="8">
+        <v>601</v>
+      </c>
+      <c r="G27">
+        <v>200</v>
+      </c>
+      <c r="H27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J27" s="8">
+        <v>48</v>
+      </c>
+      <c r="K27" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L27" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="M27">
+        <v>0.24</v>
+      </c>
+      <c r="N27">
+        <v>16.7</v>
+      </c>
+      <c r="O27">
+        <v>7800</v>
+      </c>
+      <c r="P27" s="2">
+        <v>1000000</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="3"/>
-      <c r="L28" s="14"/>
+      <c r="B28" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C28" s="4">
+        <v>625</v>
+      </c>
+      <c r="D28" s="3">
+        <v>65</v>
+      </c>
+      <c r="E28" s="8">
+        <v>101</v>
+      </c>
+      <c r="F28" s="8">
+        <v>601</v>
+      </c>
+      <c r="G28">
+        <v>200</v>
+      </c>
+      <c r="H28" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J28" s="8">
+        <v>48</v>
+      </c>
+      <c r="K28" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L28" s="14">
+        <v>4</v>
+      </c>
+      <c r="M28">
+        <v>0.17</v>
+      </c>
+      <c r="N28">
+        <v>11.8</v>
+      </c>
+      <c r="O28">
+        <v>7600</v>
+      </c>
+      <c r="P28" s="2">
+        <v>800000</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="3"/>
-      <c r="L29" s="14"/>
+      <c r="B29" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C29" s="4">
+        <v>625</v>
+      </c>
+      <c r="D29" s="3">
+        <v>65</v>
+      </c>
+      <c r="E29" s="8">
+        <v>101</v>
+      </c>
+      <c r="F29" s="8">
+        <v>601</v>
+      </c>
+      <c r="G29">
+        <v>200</v>
+      </c>
+      <c r="H29" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J29" s="8">
+        <v>48</v>
+      </c>
+      <c r="K29" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L29" s="14">
+        <v>3.5</v>
+      </c>
+      <c r="M29">
+        <v>0.18</v>
+      </c>
+      <c r="N29">
+        <v>10.6</v>
+      </c>
+      <c r="O29">
+        <v>5900</v>
+      </c>
+      <c r="P29" s="2">
+        <v>700000</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="3"/>
-      <c r="L30" s="14"/>
+      <c r="B30" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C30" s="4">
+        <v>625</v>
+      </c>
+      <c r="D30" s="3">
+        <v>65</v>
+      </c>
+      <c r="E30" s="8">
+        <v>101</v>
+      </c>
+      <c r="F30" s="8">
+        <v>601</v>
+      </c>
+      <c r="G30">
+        <v>200</v>
+      </c>
+      <c r="H30" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J30" s="8">
+        <v>48</v>
+      </c>
+      <c r="K30" s="2">
+        <v>4890000</v>
+      </c>
+      <c r="L30" s="14">
+        <v>5</v>
+      </c>
+      <c r="M30">
+        <v>0.15</v>
+      </c>
+      <c r="N30">
+        <v>13.8</v>
+      </c>
+      <c r="O30">
+        <v>8500</v>
+      </c>
+      <c r="P30" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">

</xml_diff>

<commit_message>
First proper Al/CuO test with Kim model
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\School\Research\2D_Conduction\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC82891-DCC5-4F44-A097-50C4195B55E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F70451A-7139-4845-8BB1-FFBC715D198B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
   </bookViews>
   <sheets>
     <sheet name="ConstantProp" sheetId="1" r:id="rId1"/>
-    <sheet name="VarPropEta" sheetId="3" r:id="rId2"/>
+    <sheet name="ConstProp-Graphs" sheetId="5" r:id="rId2"/>
+    <sheet name="VarPropEta" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ConstantProp!$A$2:$R$47</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VarPropEta!$A$2:$O$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">VarPropEta!$A$2:$O$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="137">
   <si>
     <t>Folder ID</t>
   </si>
@@ -434,6 +435,18 @@
   </si>
   <si>
     <t>0.63 (WW)</t>
+  </si>
+  <si>
+    <t>-AlCuO folder</t>
+  </si>
+  <si>
+    <t>AlCuO-1</t>
+  </si>
+  <si>
+    <t>60% porosity of rho_TMD, average Cp and k, same Ea as Kim model, pre-exp from Umbrajkar, dH from FlorinPetre/Baijot</t>
+  </si>
+  <si>
+    <t>AlCuO-2</t>
   </si>
 </sst>
 </file>
@@ -575,15 +588,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Density;</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Ea=48, Cp=625; coarse</a:t>
+              <a:t>Thermal conductivity; Ea=48, Cp=625, rho=1523; coarse</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -629,15 +634,12 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>rho-156k_ign</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -648,11 +650,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -660,105 +662,53 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ConstantProp!$B$13:$B$14</c:f>
+              <c:f>(ConstantProp!$D$13,ConstantProp!$D$18,ConstantProp!$D$26)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1523</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3808</c:v>
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ConstantProp!$M$13:$M$14</c:f>
+              <c:f>(ConstantProp!$N$13,ConstantProp!$N$18,ConstantProp!$N$26)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.44</c:v>
+                  <c:v>21.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.67</c:v>
+                  <c:v>14.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.2</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:v>k-speed</c:v>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-652F-4EC6-A5C2-D43545F19E09}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>rho-78k_ign</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>ConstantProp!$B$21:$B$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1523</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2020</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>ConstantProp!$M$21:$M$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.18</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.22</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-652F-4EC6-A5C2-D43545F19E09}"/>
+              <c16:uniqueId val="{00000000-E87D-41B9-9490-92BB1BC962EC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -776,15 +726,12 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="4"/>
-                <c:order val="2"/>
-                <c:tx>
-                  <c:v>rho-156k_v</c:v>
-                </c:tx>
+                <c:idx val="1"/>
+                <c:order val="1"/>
                 <c:spPr>
                   <a:ln w="19050" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent5"/>
+                      <a:schemeClr val="accent2"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -795,11 +742,11 @@
                   <c:size val="5"/>
                   <c:spPr>
                     <a:solidFill>
-                      <a:schemeClr val="accent5"/>
+                      <a:schemeClr val="accent2"/>
                     </a:solidFill>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent5"/>
+                        <a:schemeClr val="accent2"/>
                       </a:solidFill>
                     </a:ln>
                     <a:effectLst/>
@@ -810,18 +757,21 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>ConstantProp!$B$13:$B$14</c15:sqref>
+                          <c15:sqref>(ConstantProp!$D$13,ConstantProp!$D$18,ConstantProp!$D$26)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="3"/>
                       <c:pt idx="0">
-                        <c:v>1523</c:v>
+                        <c:v>156</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>3808</c:v>
+                        <c:v>78</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>65</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -831,107 +781,36 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>ConstantProp!$N$13:$N$14</c15:sqref>
+                          <c15:sqref>(ConstantProp!$M$13,ConstantProp!$M$18,ConstantProp!$M$26)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="3"/>
                       <c:pt idx="0">
-                        <c:v>21.2</c:v>
+                        <c:v>0.44</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>12.7</c:v>
+                        <c:v>0.18</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.15</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
                 <c:extLst>
+                  <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:filteredSeriesTitle>
+                      <c15:tx>
+                        <c:v>k-ign</c:v>
+                      </c15:tx>
+                    </c15:filteredSeriesTitle>
+                  </c:ext>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000004-652F-4EC6-A5C2-D43545F19E09}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="5"/>
-                <c:order val="3"/>
-                <c:tx>
-                  <c:v>rho-78k_v</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent6"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>ConstantProp!$B$21:$B$22</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>1523</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2020</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>ConstantProp!$N$21:$N$22</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>14.7</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>12.5</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="1"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000005-652F-4EC6-A5C2-D43545F19E09}"/>
+                    <c16:uniqueId val="{00000001-E87D-41B9-9490-92BB1BC962EC}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1181,7 +1060,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Thermal conductivity; Ea=48, Cp=625, rho=1523; coarse</a:t>
+              <a:t>Density;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ea=48, Cp=625; coarse</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -1227,12 +1114,15 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>rho-156k_ign</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1243,11 +1133,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1255,53 +1145,105 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(ConstantProp!$D$13,ConstantProp!$D$18,ConstantProp!$D$26)</c:f>
+              <c:f>ConstantProp!$B$13:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>156</c:v>
+                  <c:v>1523</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>65</c:v>
+                  <c:v>3808</c:v>
                 </c:pt>
               </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(ConstantProp!$N$13,ConstantProp!$N$18,ConstantProp!$N$26)</c:f>
+              <c:f>ConstantProp!$M$13:$M$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>21.2</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.2</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
               </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredSeriesTitle>
-                <c15:tx>
-                  <c:v>k-speed</c:v>
-                </c15:tx>
-              </c15:filteredSeriesTitle>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B1CE-4819-8226-F1CAF93C42FB}"/>
             </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>rho-78k_ign</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ConstantProp!$B$21:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1523</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ConstantProp!$M$21:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B3B7-4943-BD69-01F641606504}"/>
+              <c16:uniqueId val="{00000001-B1CE-4819-8226-F1CAF93C42FB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1319,12 +1261,15 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
+                <c:idx val="4"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>rho-156k_v</c:v>
+                </c:tx>
                 <c:spPr>
                   <a:ln w="19050" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent5"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -1335,11 +1280,11 @@
                   <c:size val="5"/>
                   <c:spPr>
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent5"/>
                     </a:solidFill>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent2"/>
+                        <a:schemeClr val="accent5"/>
                       </a:solidFill>
                     </a:ln>
                     <a:effectLst/>
@@ -1350,21 +1295,18 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$D$13,ConstantProp!$D$18,ConstantProp!$D$26)</c15:sqref>
+                          <c15:sqref>ConstantProp!$B$13:$B$14</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="3"/>
+                      <c:ptCount val="2"/>
                       <c:pt idx="0">
-                        <c:v>156</c:v>
+                        <c:v>1523</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>78</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>65</c:v>
+                        <c:v>3808</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1374,36 +1316,107 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$M$13,ConstantProp!$M$18,ConstantProp!$M$26)</c15:sqref>
+                          <c15:sqref>ConstantProp!$N$13:$N$14</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="3"/>
+                      <c:ptCount val="2"/>
                       <c:pt idx="0">
-                        <c:v>0.44</c:v>
+                        <c:v>21.2</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.18</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.15</c:v>
+                        <c:v>12.7</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
                 <c:extLst>
-                  <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                    <c15:filteredSeriesTitle>
-                      <c15:tx>
-                        <c:v>k-ign</c:v>
-                      </c15:tx>
-                    </c15:filteredSeriesTitle>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-B1CE-4819-8226-F1CAF93C42FB}"/>
                   </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>rho-78k_v</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent6"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>ConstantProp!$B$21:$B$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>1523</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2020</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>ConstantProp!$N$21:$N$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>14.7</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>12.5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-B3B7-4943-BD69-01F641606504}"/>
+                    <c16:uniqueId val="{00000003-B1CE-4819-8226-F1CAF93C42FB}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1779,7 +1792,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C305-43A3-AC98-8B5E9E6163F8}"/>
+              <c16:uniqueId val="{00000000-A6E8-4EF2-9BD9-8A7C5EB7CBE0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1889,7 +1902,7 @@
                 <c:smooth val="1"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-C305-43A3-AC98-8B5E9E6163F8}"/>
+                    <c16:uniqueId val="{00000001-A6E8-4EF2-9BD9-8A7C5EB7CBE0}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -2139,15 +2152,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Thermal conductivity;</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Ea=70, Cp=625, rho=1523, dH=4.7; fine</a:t>
+              <a:t>Enthalpy of Combustion; Ea=70, Cp=625, rho=1523, k=65; fine</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -2193,15 +2198,15 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
-            <c:v>ignition</c:v>
+            <c:v>wave speed</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2212,11 +2217,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2224,46 +2229,50 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(ConstantProp!$D$44,ConstantProp!$D$47,ConstantProp!$D$34)</c:f>
+              <c:f>(ConstantProp!$L$35,ConstantProp!$L$32,ConstantProp!$L$44,ConstantProp!$L$33)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(ConstantProp!$M$44,ConstantProp!$M$47,ConstantProp!$M$34)</c:f>
+              <c:f>(ConstantProp!$N$35,ConstantProp!$N$32,ConstantProp!$N$44,ConstantProp!$N$33)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.63</c:v>
+                  <c:v>7.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.49</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.6</c:v>
                 </c:pt>
               </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-5890-4CE0-9A01-58004279B834}"/>
+              <c16:uniqueId val="{00000000-EE2E-4D86-BDD8-1D7FDAE15969}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2281,15 +2290,15 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
+                <c:idx val="0"/>
+                <c:order val="0"/>
                 <c:tx>
-                  <c:v>wave speed</c:v>
+                  <c:v>ignition</c:v>
                 </c:tx>
                 <c:spPr>
                   <a:ln w="19050" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent1"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -2300,11 +2309,11 @@
                   <c:size val="5"/>
                   <c:spPr>
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent1"/>
                     </a:solidFill>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent2"/>
+                        <a:schemeClr val="accent1"/>
                       </a:solidFill>
                     </a:ln>
                     <a:effectLst/>
@@ -2315,21 +2324,24 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$D$44,ConstantProp!$D$47,ConstantProp!$D$34)</c15:sqref>
+                          <c15:sqref>(ConstantProp!$L$35,ConstantProp!$L$32,ConstantProp!$L$44,ConstantProp!$L$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="3"/>
+                      <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>65</c:v>
+                        <c:v>3.5</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>78</c:v>
+                        <c:v>4</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>100</c:v>
+                        <c:v>4.7</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2339,21 +2351,24 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$N$44,ConstantProp!$N$47,ConstantProp!$N$34)</c15:sqref>
+                          <c15:sqref>(ConstantProp!$M$35,ConstantProp!$M$32,ConstantProp!$M$44,ConstantProp!$M$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="3"/>
+                      <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>10</c:v>
+                        <c:v>0.72</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>10.4</c:v>
+                        <c:v>0.68</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0</c:v>
+                        <c:v>0.63</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.62</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2361,7 +2376,7 @@
                 <c:smooth val="1"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000005-5890-4CE0-9A01-58004279B834}"/>
+                    <c16:uniqueId val="{00000001-EE2E-4D86-BDD8-1D7FDAE15969}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -2611,7 +2626,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Enthalpy of Combustion; Ea=70, Cp=625, rho=1523, k=65; fine</a:t>
+              <a:t>Thermal conductivity;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ea=70, Cp=625, rho=1523, dH=4.7; fine</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -2657,15 +2680,15 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:tx>
-            <c:v>wave speed</c:v>
+            <c:v>ignition</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2676,11 +2699,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2688,50 +2711,46 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(ConstantProp!$L$35,ConstantProp!$L$32,ConstantProp!$L$44,ConstantProp!$L$33)</c:f>
+              <c:f>(ConstantProp!$D$44,ConstantProp!$D$47,ConstantProp!$D$34)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.5</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(ConstantProp!$N$35,ConstantProp!$N$32,ConstantProp!$N$44,ConstantProp!$N$33)</c:f>
+              <c:f>(ConstantProp!$M$44,ConstantProp!$M$47,ConstantProp!$M$34)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.4</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.5</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D9D8-463E-8420-1FDC9D210B72}"/>
+              <c16:uniqueId val="{00000000-F6D2-4261-899A-D6BFBD62767B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2749,15 +2768,15 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
+                <c:idx val="1"/>
+                <c:order val="1"/>
                 <c:tx>
-                  <c:v>ignition</c:v>
+                  <c:v>wave speed</c:v>
                 </c:tx>
                 <c:spPr>
                   <a:ln w="19050" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent1"/>
+                      <a:schemeClr val="accent2"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -2768,11 +2787,11 @@
                   <c:size val="5"/>
                   <c:spPr>
                     <a:solidFill>
-                      <a:schemeClr val="accent1"/>
+                      <a:schemeClr val="accent2"/>
                     </a:solidFill>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent1"/>
+                        <a:schemeClr val="accent2"/>
                       </a:solidFill>
                     </a:ln>
                     <a:effectLst/>
@@ -2783,24 +2802,21 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$L$35,ConstantProp!$L$32,ConstantProp!$L$44,ConstantProp!$L$33)</c15:sqref>
+                          <c15:sqref>(ConstantProp!$D$44,ConstantProp!$D$47,ConstantProp!$D$34)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="4"/>
+                      <c:ptCount val="3"/>
                       <c:pt idx="0">
-                        <c:v>3.5</c:v>
+                        <c:v>65</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>4</c:v>
+                        <c:v>78</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>4.7</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>5</c:v>
+                        <c:v>100</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2810,24 +2826,21 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$M$35,ConstantProp!$M$32,ConstantProp!$M$44,ConstantProp!$M$33)</c15:sqref>
+                          <c15:sqref>(ConstantProp!$N$44,ConstantProp!$N$47,ConstantProp!$N$34)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="4"/>
+                      <c:ptCount val="3"/>
                       <c:pt idx="0">
-                        <c:v>0.72</c:v>
+                        <c:v>10</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.68</c:v>
+                        <c:v>10.4</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.63</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.62</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2835,7 +2848,7 @@
                 <c:smooth val="1"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-D9D8-463E-8420-1FDC9D210B72}"/>
+                    <c16:uniqueId val="{00000001-F6D2-4261-899A-D6BFBD62767B}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -3213,7 +3226,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8009-44B3-BD9C-9F994C38C407}"/>
+              <c16:uniqueId val="{00000000-D2CB-4A6A-A5CE-C61B545B5F83}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3317,7 +3330,7 @@
                 <c:smooth val="1"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-8009-44B3-BD9C-9F994C38C407}"/>
+                    <c16:uniqueId val="{00000001-D2CB-4A6A-A5CE-C61B545B5F83}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -3681,7 +3694,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-4A88-4040-ABF0-A00A19FE631A}"/>
+              <c16:uniqueId val="{00000000-3F03-4F07-BB48-633EBE5C4254}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3779,7 +3792,7 @@
                 <c:smooth val="1"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-4A88-4040-ABF0-A00A19FE631A}"/>
+                    <c16:uniqueId val="{00000001-3F03-4F07-BB48-633EBE5C4254}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -7891,22 +7904,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>147108</xdr:rowOff>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>67733</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>15875</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>26458</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>389589</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>137583</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="2" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8708E734-05CF-49B0-95AC-CC2920CCB8E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E705C9A9-47D3-49E1-9346-964F7B21AA8C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7927,28 +7940,26 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>153458</xdr:rowOff>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123295</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>15873</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>32808</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>370541</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>2645</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="3" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C0CE49-7A68-4046-A3CC-EFC5996D787A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8490420-A2CA-4C01-9258-D771CAC717A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -7965,22 +7976,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>262092</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>39095</xdr:rowOff>
+      <xdr:colOff>119217</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>15282</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>459440</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>119528</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>95715</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DD396C0-E431-470D-98EA-4BC119B7D7A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27AAEFE3-E3BF-4D28-94F9-8FBCE9A73F3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8000,29 +8011,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>211232</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>165037</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>575421</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>147574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1031128</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>44387</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>231586</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>26924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="5" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1431C0C-7B9D-4316-B987-52535EAB0B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40A65D23-2A18-447A-98F4-493523CB4AB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -8038,29 +8047,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>211230</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>171387</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>575423</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>141224</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1031126</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>50737</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>231588</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>20574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="6" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9388093A-247A-49DC-8E6A-DF7DB8DF78BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4DF3258-4786-4E26-9CF1-A73637F1754E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -8076,29 +8083,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1378325</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>16061</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>588310</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>182748</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>584574</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>85911</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>244475</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>62098</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92383634-983F-498A-8045-D6C1F2BD1975}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF3AD192-D970-4F29-8C2A-BE631E523F12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -8114,29 +8119,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1243853</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>22413</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>444313</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>189100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>450102</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>92263</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>110003</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>68450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBE19C9A-EEB8-4B6F-89FF-1CCBAE3B2F3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A8430A9-8B7B-441E-B69E-377A918D1627}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -8450,14 +8453,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3C7F47-CBB8-4962-A50C-2146AC268A42}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="H37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E47" sqref="E47"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10628,8 +10630,10 @@
       <c r="K48" s="8"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>133</v>
+      </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="3"/>
@@ -10637,25 +10641,95 @@
       <c r="K49" s="8"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="3"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="3"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="3"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="3"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="4">
+        <v>2043</v>
+      </c>
+      <c r="C50" s="4">
+        <v>550</v>
+      </c>
+      <c r="D50" s="3">
+        <v>70</v>
+      </c>
+      <c r="E50" s="4">
+        <v>101</v>
+      </c>
+      <c r="F50" s="4">
+        <v>601</v>
+      </c>
+      <c r="G50" s="4">
+        <v>200</v>
+      </c>
+      <c r="H50" t="s">
+        <v>6</v>
+      </c>
+      <c r="I50">
+        <v>0.8</v>
+      </c>
+      <c r="J50" s="4">
+        <v>48</v>
+      </c>
+      <c r="K50" s="9">
+        <v>4890000</v>
+      </c>
+      <c r="L50" s="7">
+        <v>4.07</v>
+      </c>
+      <c r="M50" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="N50" s="4">
+        <v>12.2</v>
+      </c>
+      <c r="O50" s="4">
+        <v>7600</v>
+      </c>
+      <c r="R50" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B51" s="4">
+        <v>2043</v>
+      </c>
+      <c r="C51" s="4">
+        <v>550</v>
+      </c>
+      <c r="D51" s="3">
+        <v>70</v>
+      </c>
+      <c r="E51" s="4">
+        <v>101</v>
+      </c>
+      <c r="F51" s="4">
+        <v>601</v>
+      </c>
+      <c r="G51" s="4">
+        <v>200</v>
+      </c>
+      <c r="H51" t="s">
+        <v>6</v>
+      </c>
+      <c r="I51">
+        <v>0.8</v>
+      </c>
+      <c r="J51" s="4">
+        <v>48</v>
+      </c>
+      <c r="K51" s="9">
+        <v>4890000</v>
+      </c>
+      <c r="L51" s="7">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -10664,7 +10738,7 @@
       <c r="K52" s="8"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -10673,7 +10747,7 @@
       <c r="K53" s="8"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -10682,7 +10756,7 @@
       <c r="K54" s="8"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
@@ -10691,7 +10765,7 @@
       <c r="K55" s="8"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -10701,58 +10775,34 @@
       <c r="L56" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:R47" xr:uid="{49C99752-6154-48AE-B9BC-04DA8123EC2F}">
-    <filterColumn colId="0">
-      <filters blank="1">
-        <filter val="1"/>
-        <filter val="11a"/>
-        <filter val="2"/>
-        <filter val="3"/>
-        <filter val="4"/>
-        <filter val="5"/>
-        <filter val="8a"/>
-        <filter val="8b"/>
-        <filter val="9a"/>
-        <filter val="--A0 folder"/>
-        <filter val="-AlMoO3 folder"/>
-        <filter val="AlMoO3-1"/>
-        <filter val="AlMoO3-10"/>
-        <filter val="AlMoO3-11"/>
-        <filter val="AlMoO3-12"/>
-        <filter val="AlMoO3-13"/>
-        <filter val="AlMoO3-14"/>
-        <filter val="AlMoO3-15"/>
-        <filter val="AlMoO3-16"/>
-        <filter val="AlMoO3-17"/>
-        <filter val="AlMoO3-18"/>
-        <filter val="AlMoO3-19"/>
-        <filter val="AlMoO3-2"/>
-        <filter val="AlMoO3-20"/>
-        <filter val="AlMoO3-3"/>
-        <filter val="AlMoO3-4"/>
-        <filter val="AlMoO3-5"/>
-        <filter val="AlMoO3-6"/>
-        <filter val="AlMoO3-7"/>
-        <filter val="AlMoO3-8"/>
-        <filter val="AlMoO3-9"/>
-        <filter val="Conserv folder"/>
-        <filter val="--Mesh folder"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:R47" xr:uid="{49C99752-6154-48AE-B9BC-04DA8123EC2F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBE568B-3744-4C31-902D-5B6E8133C9BD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9188EC-3268-404A-8733-94DAF537670F}">
   <dimension ref="A1:O87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G28" sqref="G28:I28"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="H31:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Redo tests with coarser mesh instead of fine mesh
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F70451A-7139-4845-8BB1-FFBC715D198B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6E05E2-3482-444B-A8CB-1E58E36CFDD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{81F571D9-55F4-4B7B-A7D4-75AF9D176B74}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
   </bookViews>
   <sheets>
     <sheet name="ConstantProp" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="137">
   <si>
     <t>Folder ID</t>
   </si>
@@ -284,9 +284,6 @@
     <t>reduce k from AlMoO3-2;</t>
   </si>
   <si>
-    <t>try higher Ea; no ignition by 0.488 ms, 800 K (max)</t>
-  </si>
-  <si>
     <t>dH,Ea from Kim 2014; Ao from Stacy 2013</t>
   </si>
   <si>
@@ -365,9 +362,6 @@
     <t>AlMoO3-16</t>
   </si>
   <si>
-    <t>Higher A0;</t>
-  </si>
-  <si>
     <t>Conserv folder</t>
   </si>
   <si>
@@ -398,12 +392,6 @@
     <t>1.74 (WU)</t>
   </si>
   <si>
-    <t>1.79 (WW)</t>
-  </si>
-  <si>
-    <t>1.91 (WW)</t>
-  </si>
-  <si>
     <t>0.64 (WU)</t>
   </si>
   <si>
@@ -422,12 +410,6 @@
     <t>Reaction Rate peak (s^-1)</t>
   </si>
   <si>
-    <t>0.64 (WU), 1.8 (WW)</t>
-  </si>
-  <si>
-    <t>No ignition after 1.07ms;</t>
-  </si>
-  <si>
     <t>0.66 (WW)</t>
   </si>
   <si>
@@ -447,6 +429,24 @@
   </si>
   <si>
     <t>AlCuO-2</t>
+  </si>
+  <si>
+    <t>0.84 (WW)</t>
+  </si>
+  <si>
+    <t>Higher A0; no ignition by 1.83 ms</t>
+  </si>
+  <si>
+    <t>0.85 (WW)</t>
+  </si>
+  <si>
+    <t>0.8 (WW)</t>
+  </si>
+  <si>
+    <t>Weird results</t>
+  </si>
+  <si>
+    <t>0.89 (WU)</t>
   </si>
 </sst>
 </file>
@@ -587,8 +587,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Thermal conductivity</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Thermal conductivity; Ea=48, Cp=625, rho=1523; coarse</a:t>
+              <a:t>; Ea=48, Cp=625, rho=1523; coarse</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -663,38 +667,12 @@
           <c:xVal>
             <c:numRef>
               <c:f>(ConstantProp!$D$13,ConstantProp!$D$18,ConstantProp!$D$26)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>156</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>65</c:v>
-                </c:pt>
-              </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>(ConstantProp!$N$13,ConstantProp!$N$18,ConstantProp!$N$26)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>21.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.2</c:v>
-                </c:pt>
-              </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
@@ -712,6 +690,59 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$D$13,ConstantProp!$D$18,ConstantProp!$D$26)</c:f>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$M$13,ConstantProp!$M$18,ConstantProp!$M$26)</c:f>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:v>k-ign</c:v>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E87D-41B9-9490-92BB1BC962EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -722,101 +753,7 @@
         </c:dLbls>
         <c:axId val="391594208"/>
         <c:axId val="391592568"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent2"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$D$13,ConstantProp!$D$18,ConstantProp!$D$26)</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="3"/>
-                      <c:pt idx="0">
-                        <c:v>156</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>78</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>65</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$M$13,ConstantProp!$M$18,ConstantProp!$M$26)</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="3"/>
-                      <c:pt idx="0">
-                        <c:v>0.44</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0.18</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.15</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="1"/>
-                <c:extLst>
-                  <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                    <c15:filteredSeriesTitle>
-                      <c15:tx>
-                        <c:v>k-ign</c:v>
-                      </c15:tx>
-                    </c15:filteredSeriesTitle>
-                  </c:ext>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-E87D-41B9-9490-92BB1BC962EC}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="391594208"/>
@@ -1059,8 +996,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Density</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Density;</a:t>
+              <a:t>;</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -1146,31 +1087,11 @@
           <c:xVal>
             <c:numRef>
               <c:f>ConstantProp!$B$13:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1523</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3808</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>ConstantProp!$M$13:$M$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.44</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.67</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -1213,37 +1134,115 @@
           <c:xVal>
             <c:numRef>
               <c:f>ConstantProp!$B$21:$B$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1523</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2020</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>ConstantProp!$M$21:$M$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.18</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.22</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B1CE-4819-8226-F1CAF93C42FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>rho-156k_v</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ConstantProp!$B$13:$B$14</c:f>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ConstantProp!$N$13:$N$14</c:f>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B1CE-4819-8226-F1CAF93C42FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>rho-78k_v</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ConstantProp!$B$21:$B$22</c:f>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ConstantProp!$N$21:$N$22</c:f>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B1CE-4819-8226-F1CAF93C42FB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1257,172 +1256,7 @@
         </c:dLbls>
         <c:axId val="391594208"/>
         <c:axId val="391592568"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="4"/>
-                <c:order val="2"/>
-                <c:tx>
-                  <c:v>rho-156k_v</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent5"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent5"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent5"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>ConstantProp!$B$13:$B$14</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>1523</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>3808</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>ConstantProp!$N$13:$N$14</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>21.2</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>12.7</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="1"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-B1CE-4819-8226-F1CAF93C42FB}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="5"/>
-                <c:order val="3"/>
-                <c:tx>
-                  <c:v>rho-78k_v</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent6"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>ConstantProp!$B$21:$B$22</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>1523</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2020</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>ConstantProp!$N$21:$N$22</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>14.7</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>12.5</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="1"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-B1CE-4819-8226-F1CAF93C42FB}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="391594208"/>
@@ -1746,21 +1580,9 @@
               <c:f>(ConstantProp!$K$25,ConstantProp!$K$38,ConstantProp!$K$39,ConstantProp!$K$40,ConstantProp!$K$41)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>4890000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5500000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1770,21 +1592,9 @@
               <c:f>(ConstantProp!$M$25,ConstantProp!$M$38,ConstantProp!$M$39,ConstantProp!$M$40,ConstantProp!$M$41)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>0.62</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.61</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.59</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.56999999999999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1850,21 +1660,9 @@
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>0.00E+00</c:formatCode>
-                      <c:ptCount val="5"/>
+                      <c:ptCount val="1"/>
                       <c:pt idx="0">
                         <c:v>4890000</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>5000000</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>5500000</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>6000000</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>8000000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1880,21 +1678,9 @@
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="5"/>
+                      <c:ptCount val="1"/>
                       <c:pt idx="0">
                         <c:v>9.6</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>9.6</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>10.1</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>10.4</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>11.7</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2151,8 +1937,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Enthalpy of Combustion</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Enthalpy of Combustion; Ea=70, Cp=625, rho=1523, k=65; fine</a:t>
+              <a:t>; </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" u="sng"/>
+              <a:t>Ea=70</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>, Cp=625, rho=1523, k=65; fine</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -2255,16 +2053,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7.4</c:v>
+                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.5</c:v>
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2359,16 +2154,13 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>0.72</c:v>
+                        <c:v>0.71</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.68</c:v>
+                        <c:v>0.67</c:v>
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>0.63</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.62</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2625,16 +2417,24 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Thermal conductivity</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Thermal conductivity;</a:t>
+              <a:t>;</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
               <a:t> </a:t>
             </a:r>
             <a:r>
+              <a:rPr lang="en-US" u="sng"/>
+              <a:t>Ea=70</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Ea=70, Cp=625, rho=1523, dH=4.7; fine</a:t>
+              <a:t>, Cp=625, rho=1523, dH=4.7; fine</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -2738,10 +2538,10 @@
                   <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.49</c:v>
+                  <c:v>0.87</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2837,10 +2637,10 @@
                         <c:v>10</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>10.4</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0</c:v>
+                        <c:v>12</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3097,16 +2897,24 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Enthalpy of combustion</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Enthalpy of combustion;</a:t>
+              <a:t>;</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
               <a:t> </a:t>
             </a:r>
             <a:r>
+              <a:rPr lang="en-US" u="sng"/>
+              <a:t>Ea=48</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Ea=48, Cp=625, rho=1523, k=65; coarse </a:t>
+              <a:t>, Cp=625, rho=1523, k=65; coarse </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -3152,6 +2960,55 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>ignition</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$L$29,ConstantProp!$L$28,ConstantProp!$L$26,ConstantProp!$L$30)</c:f>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$M$29,ConstantProp!$M$28,ConstantProp!$M$26,ConstantProp!$M$30)</c:f>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D2CB-4A6A-A5CE-C61B545B5F83}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
@@ -3184,43 +3041,11 @@
           <c:xVal>
             <c:numRef>
               <c:f>(ConstantProp!$L$29,ConstantProp!$L$28,ConstantProp!$L$26,ConstantProp!$L$30)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>(ConstantProp!$N$29,ConstantProp!$N$28,ConstantProp!$N$26,ConstantProp!$N$30)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10.6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.8</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -3240,103 +3065,7 @@
         </c:dLbls>
         <c:axId val="391594208"/>
         <c:axId val="391592568"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:tx>
-                  <c:v>ignition</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent1"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$L$29,ConstantProp!$L$28,ConstantProp!$L$26,ConstantProp!$L$30)</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="4"/>
-                      <c:pt idx="0">
-                        <c:v>3.5</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>4.7</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>5</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$M$29,ConstantProp!$M$28,ConstantProp!$M$26,ConstantProp!$M$30)</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="4"/>
-                      <c:pt idx="0">
-                        <c:v>0.18</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0.17</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.15</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.15</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="1"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-D2CB-4A6A-A5CE-C61B545B5F83}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="391594208"/>
@@ -3579,8 +3308,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Thermal Conductivity</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Thermal Conductivity; Ea=48, Cp=625, rho=1523, dH=4.7; coarse</a:t>
+              <a:t>; </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" u="sng"/>
+              <a:t>Ea=48</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>, Cp=625, rho=1523, dH=4.7; coarse</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -3658,43 +3399,66 @@
           <c:xVal>
             <c:numRef>
               <c:f>(ConstantProp!$D$26,ConstantProp!$D$21,ConstantProp!$D$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>(ConstantProp!$M$26,ConstantProp!$M$21,ConstantProp!$M$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.24</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3F03-4F07-BB48-633EBE5C4254}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>wave speed</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$D$26,ConstantProp!$D$21,ConstantProp!$D$27)</c:f>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$N$26,ConstantProp!$N$21,ConstantProp!$N$27)</c:f>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3F03-4F07-BB48-633EBE5C4254}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3708,97 +3472,7 @@
         </c:dLbls>
         <c:axId val="391594208"/>
         <c:axId val="391592568"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
-                <c:tx>
-                  <c:v>wave speed</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent2"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$D$26,ConstantProp!$D$21,ConstantProp!$D$27)</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="3"/>
-                      <c:pt idx="0">
-                        <c:v>65</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>78</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>100</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$N$26,ConstantProp!$N$21,ConstantProp!$N$27)</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="3"/>
-                      <c:pt idx="0">
-                        <c:v>13.2</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>14.7</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>16.7</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="1"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-3F03-4F07-BB48-633EBE5C4254}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="391594208"/>
@@ -8453,13 +8127,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3C7F47-CBB8-4962-A50C-2146AC268A42}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H37" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8494,7 +8166,7 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
@@ -8547,7 +8219,7 @@
         <v>36</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>57</v>
@@ -8848,9 +8520,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -8860,9 +8532,9 @@
       <c r="L10" s="3"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -8918,10 +8590,10 @@
       </c>
       <c r="Q12" s="4"/>
       <c r="R12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>74</v>
       </c>
@@ -8972,10 +8644,10 @@
       </c>
       <c r="Q13" s="4"/>
       <c r="R13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>75</v>
       </c>
@@ -9026,10 +8698,10 @@
       </c>
       <c r="Q14" s="4"/>
       <c r="R14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="8">
         <v>1523</v>
@@ -9075,10 +8747,10 @@
       </c>
       <c r="Q15" s="4"/>
       <c r="R15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="8">
         <v>2020</v>
@@ -9127,7 +8799,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="8">
         <v>1523</v>
@@ -9176,7 +8848,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>73</v>
       </c>
@@ -9232,7 +8904,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B19" s="8">
         <v>1523</v>
@@ -9252,11 +8924,11 @@
       <c r="G19">
         <v>200</v>
       </c>
-      <c r="H19">
-        <v>1200</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="H19" t="s">
         <v>6</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.8</v>
       </c>
       <c r="J19" s="8">
         <v>70</v>
@@ -9268,25 +8940,25 @@
         <v>4.7</v>
       </c>
       <c r="M19">
-        <v>0.81</v>
+        <v>0.85</v>
       </c>
       <c r="N19">
-        <v>8.8000000000000007</v>
+        <v>10.6</v>
       </c>
       <c r="O19">
         <v>7800</v>
       </c>
       <c r="P19" s="2">
-        <v>550000</v>
+        <v>650000</v>
       </c>
       <c r="Q19" s="4"/>
       <c r="R19" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="8">
         <v>1523</v>
@@ -9332,12 +9004,12 @@
       </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" s="8">
         <v>1523</v>
@@ -9385,10 +9057,10 @@
         <v>1000000</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>76</v>
       </c>
@@ -9438,10 +9110,10 @@
         <v>1000000</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>77</v>
       </c>
@@ -9491,12 +9163,12 @@
         <v>900000</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" s="8">
         <v>2020</v>
@@ -9544,12 +9216,12 @@
         <v>600000</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B25" s="11">
         <v>1523</v>
@@ -9597,9 +9269,9 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B26" s="4">
         <v>1523</v>
@@ -9647,9 +9319,9 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" s="8">
         <v>1523</v>
@@ -9697,9 +9369,9 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B28" s="4">
         <v>1523</v>
@@ -9747,12 +9419,12 @@
         <v>800000</v>
       </c>
       <c r="Q28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29" s="4">
         <v>1523</v>
@@ -9800,12 +9472,12 @@
         <v>700000</v>
       </c>
       <c r="Q29" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B30" s="4">
         <v>1523</v>
@@ -9853,12 +9525,12 @@
         <v>1000000</v>
       </c>
       <c r="Q30" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B31" s="4">
         <v>1523</v>
@@ -9869,11 +9541,11 @@
       <c r="D31" s="3">
         <v>156</v>
       </c>
-      <c r="E31" s="4">
-        <v>201</v>
-      </c>
-      <c r="F31" s="4">
-        <v>1201</v>
+      <c r="E31" s="8">
+        <v>101</v>
+      </c>
+      <c r="F31" s="8">
+        <v>601</v>
       </c>
       <c r="G31" s="4">
         <v>200</v>
@@ -9902,16 +9574,19 @@
       <c r="O31" t="s">
         <v>79</v>
       </c>
+      <c r="P31" t="s">
+        <v>79</v>
+      </c>
       <c r="Q31" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="R31" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B32" s="4">
         <v>1523</v>
@@ -9922,11 +9597,11 @@
       <c r="D32" s="3">
         <v>65</v>
       </c>
-      <c r="E32" s="4">
-        <v>201</v>
-      </c>
-      <c r="F32" s="4">
-        <v>1201</v>
+      <c r="E32" s="8">
+        <v>101</v>
+      </c>
+      <c r="F32" s="8">
+        <v>601</v>
       </c>
       <c r="G32" s="4">
         <v>200</v>
@@ -9947,21 +9622,24 @@
         <v>4</v>
       </c>
       <c r="M32">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="N32">
-        <v>8.5</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="O32">
         <v>6600</v>
       </c>
+      <c r="P32" s="2">
+        <v>500000</v>
+      </c>
       <c r="Q32" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B33" s="4">
         <v>1523</v>
@@ -9972,11 +9650,11 @@
       <c r="D33" s="3">
         <v>65</v>
       </c>
-      <c r="E33" s="4">
-        <v>201</v>
-      </c>
-      <c r="F33" s="4">
-        <v>1201</v>
+      <c r="E33" s="8">
+        <v>101</v>
+      </c>
+      <c r="F33" s="8">
+        <v>601</v>
       </c>
       <c r="G33" s="4">
         <v>200</v>
@@ -9996,22 +9674,13 @@
       <c r="L33" s="14">
         <v>5</v>
       </c>
-      <c r="M33">
-        <v>0.62</v>
-      </c>
-      <c r="N33">
-        <v>10.6</v>
-      </c>
-      <c r="O33">
-        <v>8100</v>
-      </c>
       <c r="Q33" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B34" s="8">
         <v>1523</v>
@@ -10023,10 +9692,10 @@
         <v>100</v>
       </c>
       <c r="E34" s="8">
-        <v>201</v>
+        <v>101</v>
       </c>
       <c r="F34" s="8">
-        <v>1201</v>
+        <v>601</v>
       </c>
       <c r="G34">
         <v>200</v>
@@ -10046,25 +9715,28 @@
       <c r="L34" s="14">
         <v>4.7</v>
       </c>
-      <c r="M34" t="s">
-        <v>79</v>
-      </c>
-      <c r="N34" t="s">
-        <v>79</v>
-      </c>
-      <c r="O34" t="s">
-        <v>79</v>
+      <c r="M34">
+        <v>1.4</v>
+      </c>
+      <c r="N34">
+        <v>12</v>
+      </c>
+      <c r="O34">
+        <v>8000</v>
+      </c>
+      <c r="P34" s="2">
+        <v>0</v>
       </c>
       <c r="Q34" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="R34" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B35" s="4">
         <v>1523</v>
@@ -10076,10 +9748,10 @@
         <v>65</v>
       </c>
       <c r="E35" s="8">
-        <v>201</v>
+        <v>101</v>
       </c>
       <c r="F35" s="8">
-        <v>1201</v>
+        <v>601</v>
       </c>
       <c r="G35">
         <v>200</v>
@@ -10100,19 +9772,22 @@
         <v>3.5</v>
       </c>
       <c r="M35">
-        <v>0.72</v>
+        <v>0.71</v>
       </c>
       <c r="N35">
-        <v>7.4</v>
+        <v>7.2</v>
       </c>
       <c r="O35">
         <v>6000</v>
       </c>
+      <c r="P35" s="2">
+        <v>400000</v>
+      </c>
       <c r="Q35" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -10124,9 +9799,9 @@
       <c r="K36" s="2"/>
       <c r="L36" s="14"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -10138,7 +9813,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="15"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>1</v>
       </c>
@@ -10188,10 +9863,10 @@
         <v>680000</v>
       </c>
       <c r="R38" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>2</v>
       </c>
@@ -10241,13 +9916,13 @@
         <v>700000</v>
       </c>
       <c r="Q39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R39" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>3</v>
       </c>
@@ -10297,13 +9972,13 @@
         <v>800000</v>
       </c>
       <c r="Q40" t="s">
+        <v>103</v>
+      </c>
+      <c r="R40" t="s">
         <v>104</v>
       </c>
-      <c r="R40" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>4</v>
       </c>
@@ -10353,13 +10028,13 @@
         <v>1200000</v>
       </c>
       <c r="Q41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R41" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>5</v>
       </c>
@@ -10409,15 +10084,15 @@
         <v>1200000</v>
       </c>
       <c r="Q42" t="s">
+        <v>118</v>
+      </c>
+      <c r="R42" t="s">
         <v>122</v>
       </c>
-      <c r="R42" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="8"/>
@@ -10429,7 +10104,7 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B44" s="11">
         <v>1523</v>
@@ -10477,9 +10152,9 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B45" s="4">
         <v>1523</v>
@@ -10526,7 +10201,7 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B46" s="4">
         <v>1523</v>
@@ -10573,7 +10248,7 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B47" s="8">
         <v>1523</v>
@@ -10593,11 +10268,11 @@
       <c r="G47">
         <v>200</v>
       </c>
-      <c r="H47">
-        <v>1200</v>
-      </c>
-      <c r="I47" s="1" t="s">
+      <c r="H47" t="s">
         <v>6</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0.8</v>
       </c>
       <c r="J47" s="8">
         <v>70</v>
@@ -10609,16 +10284,19 @@
         <v>4.7</v>
       </c>
       <c r="M47">
-        <v>0.49</v>
+        <v>0.87</v>
       </c>
       <c r="N47">
-        <v>10.4</v>
+        <v>11</v>
       </c>
       <c r="O47">
         <v>7800</v>
       </c>
+      <c r="P47" s="2">
+        <v>600000</v>
+      </c>
       <c r="Q47" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
@@ -10632,7 +10310,7 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -10643,7 +10321,7 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B50" s="4">
         <v>2043</v>
@@ -10688,12 +10366,12 @@
         <v>7600</v>
       </c>
       <c r="R50" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B51" s="4">
         <v>2043</v>
@@ -10775,7 +10453,55 @@
       <c r="L56" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:R47" xr:uid="{49C99752-6154-48AE-B9BC-04DA8123EC2F}"/>
+  <autoFilter ref="A2:R47" xr:uid="{49C99752-6154-48AE-B9BC-04DA8123EC2F}">
+    <filterColumn colId="0">
+      <filters blank="1">
+        <filter val="1"/>
+        <filter val="11a"/>
+        <filter val="2"/>
+        <filter val="3"/>
+        <filter val="4"/>
+        <filter val="5"/>
+        <filter val="8a"/>
+        <filter val="8b"/>
+        <filter val="9a"/>
+        <filter val="--A0 folder"/>
+        <filter val="-AlMoO3 folder"/>
+        <filter val="AlMoO3-1"/>
+        <filter val="AlMoO3-10"/>
+        <filter val="AlMoO3-11"/>
+        <filter val="AlMoO3-12"/>
+        <filter val="AlMoO3-13"/>
+        <filter val="AlMoO3-14"/>
+        <filter val="AlMoO3-15"/>
+        <filter val="AlMoO3-16"/>
+        <filter val="AlMoO3-17"/>
+        <filter val="AlMoO3-18"/>
+        <filter val="AlMoO3-19"/>
+        <filter val="AlMoO3-2"/>
+        <filter val="AlMoO3-20"/>
+        <filter val="AlMoO3-3"/>
+        <filter val="AlMoO3-4"/>
+        <filter val="AlMoO3-5"/>
+        <filter val="AlMoO3-6"/>
+        <filter val="AlMoO3-7"/>
+        <filter val="AlMoO3-8"/>
+        <filter val="AlMoO3-9"/>
+        <filter val="Conserv folder"/>
+        <filter val="--Mesh folder"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="70"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="10">
+      <filters>
+        <filter val="4.89E+06"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10785,8 +10511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBE568B-3744-4C31-902D-5B6E8133C9BD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10800,10 +10526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9188EC-3268-404A-8733-94DAF537670F}">
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K31" sqref="H31:K31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Last test redo with coarse mesh
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6E05E2-3482-444B-A8CB-1E58E36CFDD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22ED0FE0-1FA7-4D32-A49D-B9144252C9C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
   </bookViews>
@@ -640,6 +640,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>wave speed</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -667,24 +670,43 @@
           <c:xVal>
             <c:numRef>
               <c:f>(ConstantProp!$D$13,ConstantProp!$D$18,ConstantProp!$D$26)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>(ConstantProp!$N$13,ConstantProp!$N$18,ConstantProp!$N$26)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>21.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.2</c:v>
+                </c:pt>
+              </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredSeriesTitle>
-                <c15:tx>
-                  <c:v>k-speed</c:v>
-                </c15:tx>
-              </c15:filteredSeriesTitle>
-            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E87D-41B9-9490-92BB1BC962EC}"/>
             </c:ext>
@@ -693,6 +715,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>ignition</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -720,24 +745,43 @@
           <c:xVal>
             <c:numRef>
               <c:f>(ConstantProp!$D$13,ConstantProp!$D$18,ConstantProp!$D$26)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>(ConstantProp!$M$13,ConstantProp!$M$18,ConstantProp!$M$26)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15</c:v>
+                </c:pt>
+              </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
           <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredSeriesTitle>
-                <c15:tx>
-                  <c:v>k-ign</c:v>
-                </c15:tx>
-              </c15:filteredSeriesTitle>
-            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E87D-41B9-9490-92BB1BC962EC}"/>
             </c:ext>
@@ -1087,11 +1131,25 @@
           <c:xVal>
             <c:numRef>
               <c:f>ConstantProp!$B$13:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1523</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>ConstantProp!$M$13:$M$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.44</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -1134,11 +1192,25 @@
           <c:xVal>
             <c:numRef>
               <c:f>ConstantProp!$B$21:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1523</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>ConstantProp!$M$21:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.18</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -1181,12 +1253,26 @@
           <c:xVal>
             <c:numRef>
               <c:f>ConstantProp!$B$13:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1523</c:v>
+                </c:pt>
+              </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>ConstantProp!$N$13:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>21.2</c:v>
+                </c:pt>
+              </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
@@ -1230,12 +1316,26 @@
           <c:xVal>
             <c:numRef>
               <c:f>ConstantProp!$B$21:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1523</c:v>
+                </c:pt>
+              </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>ConstantProp!$N$21:$N$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>14.7</c:v>
+                </c:pt>
+              </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
@@ -1950,13 +2050,8 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>, Cp=625, rho=1523, k=65; fine</a:t>
+              <a:t>, Cp=625, rho=1523, k=65</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> mesh</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2027,7 +2122,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(ConstantProp!$L$35,ConstantProp!$L$32,ConstantProp!$L$44,ConstantProp!$L$33)</c:f>
+              <c:f>(ConstantProp!$L$35,ConstantProp!$L$32,ConstantProp!$L$25,ConstantProp!$L$33)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2048,7 +2143,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(ConstantProp!$N$35,ConstantProp!$N$32,ConstantProp!$N$44,ConstantProp!$N$33)</c:f>
+              <c:f>(ConstantProp!$N$35,ConstantProp!$N$32,ConstantProp!$N$25,ConstantProp!$N$33)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2059,7 +2154,10 @@
                   <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2119,7 +2217,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$L$35,ConstantProp!$L$32,ConstantProp!$L$44,ConstantProp!$L$33)</c15:sqref>
+                          <c15:sqref>(ConstantProp!$L$35,ConstantProp!$L$32,ConstantProp!$L$25,ConstantProp!$L$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2146,7 +2244,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$M$35,ConstantProp!$M$32,ConstantProp!$M$44,ConstantProp!$M$33)</c15:sqref>
+                          <c15:sqref>(ConstantProp!$M$35,ConstantProp!$M$32,ConstantProp!$M$25,ConstantProp!$M$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2160,7 +2258,10 @@
                         <c:v>0.67</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.63</c:v>
+                        <c:v>0.62</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.6</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2434,13 +2535,8 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>, Cp=625, rho=1523, dH=4.7; fine</a:t>
+              <a:t>, Cp=625, rho=1523, dH=4.7</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> mesh</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2480,15 +2576,15 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
-            <c:v>ignition</c:v>
+            <c:v>wave speed</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2499,11 +2595,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2511,10 +2607,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(ConstantProp!$D$44,ConstantProp!$D$47,ConstantProp!$D$34)</c:f>
+              <c:f>(ConstantProp!$D$25,ConstantProp!$D$19,ConstantProp!$D$34,ConstantProp!$D$31)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>65</c:v>
                 </c:pt>
@@ -2524,33 +2620,37 @@
                 <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>156</c:v>
+                </c:pt>
               </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(ConstantProp!$M$44,ConstantProp!$M$47,ConstantProp!$M$34)</c:f>
+              <c:f>(ConstantProp!$N$25,ConstantProp!$N$19,ConstantProp!$N$34,ConstantProp!$N$31)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.63</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.87</c:v>
+                  <c:v>10.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4</c:v>
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
           <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F6D2-4261-899A-D6BFBD62767B}"/>
+              <c16:uniqueId val="{00000001-F6D2-4261-899A-D6BFBD62767B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2568,15 +2668,15 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
+                <c:idx val="0"/>
+                <c:order val="0"/>
                 <c:tx>
-                  <c:v>wave speed</c:v>
+                  <c:v>ignition</c:v>
                 </c:tx>
                 <c:spPr>
                   <a:ln w="19050" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent1"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -2587,11 +2687,11 @@
                   <c:size val="5"/>
                   <c:spPr>
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent1"/>
                     </a:solidFill>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent2"/>
+                        <a:schemeClr val="accent1"/>
                       </a:solidFill>
                     </a:ln>
                     <a:effectLst/>
@@ -2602,13 +2702,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$D$44,ConstantProp!$D$47,ConstantProp!$D$34)</c15:sqref>
+                          <c15:sqref>(ConstantProp!$D$25,ConstantProp!$D$19,ConstantProp!$D$34,ConstantProp!$D$31)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="3"/>
+                      <c:ptCount val="4"/>
                       <c:pt idx="0">
                         <c:v>65</c:v>
                       </c:pt>
@@ -2618,6 +2718,9 @@
                       <c:pt idx="2">
                         <c:v>100</c:v>
                       </c:pt>
+                      <c:pt idx="3">
+                        <c:v>156</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:xVal>
@@ -2626,21 +2729,24 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$N$44,ConstantProp!$N$47,ConstantProp!$N$34)</c15:sqref>
+                          <c15:sqref>(ConstantProp!$M$25,ConstantProp!$M$19,ConstantProp!$M$34,ConstantProp!$M$31)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="3"/>
+                      <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>10</c:v>
+                        <c:v>0.62</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>11</c:v>
+                        <c:v>0.85</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>12</c:v>
+                        <c:v>1.4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2648,7 +2754,7 @@
                 <c:smooth val="1"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-F6D2-4261-899A-D6BFBD62767B}"/>
+                    <c16:uniqueId val="{00000000-F6D2-4261-899A-D6BFBD62767B}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -2914,13 +3020,8 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>, Cp=625, rho=1523, k=65; coarse </a:t>
+              <a:t>, Cp=625, rho=1523, k=65</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>mesh</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2992,12 +3093,44 @@
           <c:xVal>
             <c:numRef>
               <c:f>(ConstantProp!$L$29,ConstantProp!$L$28,ConstantProp!$L$26,ConstantProp!$L$30)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>(ConstantProp!$M$29,ConstantProp!$M$28,ConstantProp!$M$26,ConstantProp!$M$30)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+              </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
@@ -3005,53 +3138,6 @@
           <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D2CB-4A6A-A5CE-C61B545B5F83}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>wave speed</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>(ConstantProp!$L$29,ConstantProp!$L$28,ConstantProp!$L$26,ConstantProp!$L$30)</c:f>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>(ConstantProp!$N$29,ConstantProp!$N$28,ConstantProp!$N$26,ConstantProp!$N$30)</c:f>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D2CB-4A6A-A5CE-C61B545B5F83}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3065,7 +3151,103 @@
         </c:dLbls>
         <c:axId val="391594208"/>
         <c:axId val="391592568"/>
-        <c:extLst/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>wave speed</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(ConstantProp!$L$29,ConstantProp!$L$28,ConstantProp!$L$26,ConstantProp!$L$30)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>3.5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4.7</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(ConstantProp!$N$29,ConstantProp!$N$28,ConstantProp!$N$26,ConstantProp!$N$30)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>10.6</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>11.8</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>13.2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>13.8</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-D2CB-4A6A-A5CE-C61B545B5F83}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="391594208"/>
@@ -3321,13 +3503,8 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>, Cp=625, rho=1523, dH=4.7; coarse</a:t>
+              <a:t>, Cp=625, rho=1523, dH=4.7</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> mesh</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3399,66 +3576,43 @@
           <c:xVal>
             <c:numRef>
               <c:f>(ConstantProp!$D$26,ConstantProp!$D$21,ConstantProp!$D$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>(ConstantProp!$M$26,ConstantProp!$M$21,ConstantProp!$M$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3F03-4F07-BB48-633EBE5C4254}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>wave speed</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>(ConstantProp!$D$26,ConstantProp!$D$21,ConstantProp!$D$27)</c:f>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>(ConstantProp!$N$26,ConstantProp!$N$21,ConstantProp!$N$27)</c:f>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3F03-4F07-BB48-633EBE5C4254}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3472,7 +3626,97 @@
         </c:dLbls>
         <c:axId val="391594208"/>
         <c:axId val="391592568"/>
-        <c:extLst/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>wave speed</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(ConstantProp!$D$26,ConstantProp!$D$21,ConstantProp!$D$27)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>65</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>78</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>100</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(ConstantProp!$N$26,ConstantProp!$N$21,ConstantProp!$N$27)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>13.2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>14.7</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>16.7</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-3F03-4F07-BB48-633EBE5C4254}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="391594208"/>
@@ -3663,6 +3907,735 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" b="1"/>
+              <a:t>Peak Temperature </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>vs Enthalpy of Combustion, Ea=48</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$L$29,ConstantProp!$L$28,ConstantProp!$L$26,ConstantProp!$L$30)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$O$29,ConstantProp!$O$28,ConstantProp!$O$26,ConstantProp!$O$30)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-9ED2-4161-9252-94A052C67018}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$L$29,ConstantProp!$L$28,ConstantProp!$L$26,ConstantProp!$L$30)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$O$29,ConstantProp!$O$28,ConstantProp!$O$26,ConstantProp!$O$30)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-9ED2-4161-9252-94A052C67018}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$L$29,ConstantProp!$L$28,ConstantProp!$L$26,ConstantProp!$L$30)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$O$29,ConstantProp!$O$28,ConstantProp!$O$26,ConstantProp!$O$30)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-9ED2-4161-9252-94A052C67018}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$L$29,ConstantProp!$L$28,ConstantProp!$L$26,ConstantProp!$L$30)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$O$29,ConstantProp!$O$28,ConstantProp!$O$26,ConstantProp!$O$30)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-9ED2-4161-9252-94A052C67018}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="539910720"/>
+        <c:axId val="539914000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="539910720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="539914000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="539914000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="539910720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" b="1"/>
+              <a:t>Peak Temperature </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>vs Enthalpy of Combustion, Ea=70</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$L$35,ConstantProp!$L$32,ConstantProp!$L$25,ConstantProp!$L$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(ConstantProp!$O$35,ConstantProp!$O$32,ConstantProp!$O$25,ConstantProp!$O$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A7CF-4567-BBB6-DDC134EB9488}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="539910720"/>
+        <c:axId val="539914000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="539910720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="539914000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="539914000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="539910720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -7822,6 +8795,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE96FA6B-F4AD-4D36-8FCD-26A81C8FA767}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A52B9C14-41AD-45DC-A592-FFA0573874B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8130,8 +9177,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8593,7 +9640,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>74</v>
       </c>
@@ -8799,7 +9846,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="8">
         <v>1523</v>
@@ -8848,7 +9895,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>73</v>
       </c>
@@ -9007,7 +10054,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>86</v>
       </c>
@@ -9166,7 +10213,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>90</v>
       </c>
@@ -9269,7 +10316,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>95</v>
       </c>
@@ -9319,7 +10366,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>98</v>
       </c>
@@ -9369,7 +10416,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>101</v>
       </c>
@@ -9422,7 +10469,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>102</v>
       </c>
@@ -9475,7 +10522,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>105</v>
       </c>
@@ -9673,6 +10720,18 @@
       </c>
       <c r="L33" s="14">
         <v>5</v>
+      </c>
+      <c r="M33">
+        <v>0.6</v>
+      </c>
+      <c r="N33">
+        <v>10.1</v>
+      </c>
+      <c r="O33">
+        <v>8100</v>
+      </c>
+      <c r="P33" s="2">
+        <v>600000</v>
       </c>
       <c r="Q33" t="s">
         <v>118</v>
@@ -10152,7 +11211,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>112</v>
       </c>
@@ -10491,9 +11550,9 @@
         <filter val="--Mesh folder"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="9">
+    <filterColumn colId="1">
       <filters>
-        <filter val="70"/>
+        <filter val="1523"/>
       </filters>
     </filterColumn>
     <filterColumn colId="10">

</xml_diff>

<commit_message>
Extend test to find ignition (not found)
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22ED0FE0-1FA7-4D32-A49D-B9144252C9C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8809EB9C-7975-4FB0-B5BC-F107EF954476}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="137">
   <si>
     <t>Folder ID</t>
   </si>
@@ -434,9 +434,6 @@
     <t>0.84 (WW)</t>
   </si>
   <si>
-    <t>Higher A0; no ignition by 1.83 ms</t>
-  </si>
-  <si>
     <t>0.85 (WW)</t>
   </si>
   <si>
@@ -447,6 +444,9 @@
   </si>
   <si>
     <t>0.89 (WU)</t>
+  </si>
+  <si>
+    <t>Higher A0; no ignition by 3.66 ms</t>
   </si>
 </sst>
 </file>
@@ -2576,15 +2576,15 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:tx>
-            <c:v>wave speed</c:v>
+            <c:v>ignition</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2595,11 +2595,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2624,33 +2624,35 @@
                   <c:v>156</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(ConstantProp!$N$25,ConstantProp!$N$19,ConstantProp!$N$34,ConstantProp!$N$31)</c:f>
+              <c:f>(ConstantProp!$M$25,ConstantProp!$M$19,ConstantProp!$M$34,ConstantProp!$M$31)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.6</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.6</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
           <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F6D2-4261-899A-D6BFBD62767B}"/>
+              <c16:uniqueId val="{00000000-F6D2-4261-899A-D6BFBD62767B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2668,15 +2670,15 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
+                <c:idx val="1"/>
+                <c:order val="1"/>
                 <c:tx>
-                  <c:v>ignition</c:v>
+                  <c:v>wave speed</c:v>
                 </c:tx>
                 <c:spPr>
                   <a:ln w="19050" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent1"/>
+                      <a:schemeClr val="accent2"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -2687,11 +2689,11 @@
                   <c:size val="5"/>
                   <c:spPr>
                     <a:solidFill>
-                      <a:schemeClr val="accent1"/>
+                      <a:schemeClr val="accent2"/>
                     </a:solidFill>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent1"/>
+                        <a:schemeClr val="accent2"/>
                       </a:solidFill>
                     </a:ln>
                     <a:effectLst/>
@@ -2729,7 +2731,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(ConstantProp!$M$25,ConstantProp!$M$19,ConstantProp!$M$34,ConstantProp!$M$31)</c15:sqref>
+                          <c15:sqref>(ConstantProp!$N$25,ConstantProp!$N$19,ConstantProp!$N$34,ConstantProp!$N$31)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2737,13 +2739,13 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>0.62</c:v>
+                        <c:v>9.6</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.85</c:v>
+                        <c:v>10.6</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>1.4</c:v>
+                        <c:v>12</c:v>
                       </c:pt>
                       <c:pt idx="3">
                         <c:v>0</c:v>
@@ -2754,7 +2756,7 @@
                 <c:smooth val="1"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-F6D2-4261-899A-D6BFBD62767B}"/>
+                    <c16:uniqueId val="{00000001-F6D2-4261-899A-D6BFBD62767B}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -9177,8 +9179,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10612,8 +10614,8 @@
       <c r="L31" s="14">
         <v>4.7</v>
       </c>
-      <c r="M31" t="s">
-        <v>79</v>
+      <c r="M31">
+        <v>4</v>
       </c>
       <c r="N31" t="s">
         <v>79</v>
@@ -10628,7 +10630,7 @@
         <v>131</v>
       </c>
       <c r="R31" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -10681,7 +10683,7 @@
         <v>500000</v>
       </c>
       <c r="Q32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -10787,10 +10789,10 @@
         <v>0</v>
       </c>
       <c r="Q34" t="s">
+        <v>133</v>
+      </c>
+      <c r="R34" t="s">
         <v>134</v>
-      </c>
-      <c r="R34" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -10843,7 +10845,7 @@
         <v>400000</v>
       </c>
       <c r="Q35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -11570,7 +11572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBE568B-3744-4C31-902D-5B6E8133C9BD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="I4" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update graphs with AlMoO3 case 2
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\School\Research\2D_Conduction\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982518B4-D7F3-46E0-B722-CD2E254347CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE723501-A665-4018-A0E1-A84EF86E8055}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
   </bookViews>
   <sheets>
     <sheet name="ConstantPropPlanar" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="140">
   <si>
     <t>Folder ID</t>
   </si>
@@ -456,6 +456,9 @@
   <si>
     <t>Axisymmetric</t>
   </si>
+  <si>
+    <t>RED-kJ/g or MJ/kg</t>
+  </si>
 </sst>
 </file>
 
@@ -719,7 +722,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21.2</c:v>
+                  <c:v>19.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>14.2</c:v>
@@ -794,7 +797,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.44</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.18</c:v>
@@ -1173,7 +1176,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.44</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1296,7 +1299,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>21.2</c:v>
+                  <c:v>19.3</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2735,10 +2738,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(ConstantPropPlanar!$D$26,ConstantPropPlanar!$D$21,ConstantPropPlanar!$D$27)</c:f>
+              <c:f>(ConstantPropPlanar!$D$26,ConstantPropPlanar!$D$21,ConstantPropPlanar!$D$27,ConstantPropPlanar!$D$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>65</c:v>
                 </c:pt>
@@ -2748,15 +2751,18 @@
                 <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>156</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(ConstantPropPlanar!$N$26,ConstantPropPlanar!$N$21,ConstantPropPlanar!$N$27)</c:f>
+              <c:f>(ConstantPropPlanar!$N$26,ConstantPropPlanar!$N$21,ConstantPropPlanar!$N$27,ConstantPropPlanar!$N$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>13.2</c:v>
                 </c:pt>
@@ -2765,6 +2771,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>16.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3676,10 +3685,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(ConstantPropPlanar!$D$26,ConstantPropPlanar!$D$21,ConstantPropPlanar!$D$27)</c:f>
+              <c:f>(ConstantPropPlanar!$D$26,ConstantPropPlanar!$D$21,ConstantPropPlanar!$D$27,ConstantPropPlanar!$D$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>65</c:v>
                 </c:pt>
@@ -3689,15 +3698,18 @@
                 <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>156</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(ConstantPropPlanar!$M$26,ConstantPropPlanar!$M$21,ConstantPropPlanar!$M$27)</c:f>
+              <c:f>(ConstantPropPlanar!$M$26,ConstantPropPlanar!$M$21,ConstantPropPlanar!$M$27,ConstantPropPlanar!$M$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.15</c:v>
                 </c:pt>
@@ -3706,6 +3718,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8885,11 +8900,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="11" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="11" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8926,7 +8941,7 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="3" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
@@ -9375,11 +9390,11 @@
       <c r="G13">
         <v>200</v>
       </c>
-      <c r="H13">
-        <v>1200</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="H13" t="s">
         <v>6</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.8</v>
       </c>
       <c r="J13" s="8">
         <v>48</v>
@@ -9391,16 +9406,16 @@
         <v>4.7</v>
       </c>
       <c r="M13">
-        <v>0.44</v>
+        <v>0.48</v>
       </c>
       <c r="N13">
-        <v>21.2</v>
+        <v>19.3</v>
       </c>
       <c r="O13">
-        <v>7800</v>
+        <v>6800</v>
       </c>
       <c r="P13" s="2">
-        <v>900000</v>
+        <v>800000</v>
       </c>
       <c r="Q13" s="4"/>
       <c r="R13" t="s">
@@ -11283,8 +11298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBE568B-3744-4C31-902D-5B6E8133C9BD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="I16" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="J19" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Axisymmetric test cases from planar cases
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\School\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE723501-A665-4018-A0E1-A84EF86E8055}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D76EF9A-4571-4225-A5A4-6F9260123A69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="2" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
   </bookViews>
   <sheets>
     <sheet name="ConstantPropPlanar" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="VarPropEta" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ConstantPropAxisym!$A$2:$R$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ConstantPropAxisym!$A$2:$R$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ConstantPropPlanar!$A$2:$R$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">VarPropEta!$A$2:$O$39</definedName>
   </definedNames>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="141">
   <si>
     <t>Folder ID</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>RED-kJ/g or MJ/kg</t>
+  </si>
+  <si>
+    <t>-Axisymmetric</t>
   </si>
 </sst>
 </file>
@@ -8901,10 +8904,10 @@
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="11" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="11" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13:L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11298,7 +11301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBE568B-3744-4C31-902D-5B6E8133C9BD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J19" workbookViewId="0">
+    <sheetView topLeftCell="J19" workbookViewId="0">
       <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
@@ -11311,10 +11314,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B099DE-69DA-496C-8376-9BFCA5F25F37}">
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11414,98 +11417,192 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="24"/>
+      <c r="A3" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
-      <c r="R3" s="21"/>
+      <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
+      <c r="A4" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C4" s="4">
+        <v>625</v>
+      </c>
+      <c r="D4" s="6">
+        <v>65</v>
+      </c>
+      <c r="E4" s="21">
+        <v>101</v>
+      </c>
+      <c r="F4" s="21">
+        <v>601</v>
+      </c>
+      <c r="G4" s="21">
+        <v>200</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="J4" s="21">
+        <v>70</v>
+      </c>
+      <c r="K4" s="23">
+        <v>4890000</v>
+      </c>
+      <c r="L4" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="21"/>
+      <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
+      <c r="A5" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C5" s="4">
+        <v>625</v>
+      </c>
+      <c r="D5" s="6">
+        <v>78</v>
+      </c>
+      <c r="E5" s="21">
+        <v>101</v>
+      </c>
+      <c r="F5" s="21">
+        <v>601</v>
+      </c>
+      <c r="G5" s="21">
+        <v>200</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="J5" s="21">
+        <v>70</v>
+      </c>
+      <c r="K5" s="23">
+        <v>4890000</v>
+      </c>
+      <c r="L5" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-      <c r="R5" s="21"/>
+      <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
+      <c r="A6" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C6" s="4">
+        <v>625</v>
+      </c>
+      <c r="D6" s="6">
+        <v>156</v>
+      </c>
+      <c r="E6" s="4">
+        <v>101</v>
+      </c>
+      <c r="F6" s="4">
+        <v>601</v>
+      </c>
+      <c r="G6" s="21">
+        <v>200</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J6" s="4">
+        <v>70</v>
+      </c>
+      <c r="K6" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L6" s="15">
+        <v>4.7</v>
+      </c>
+      <c r="M6" s="24"/>
+      <c r="N6" s="4"/>
       <c r="O6" s="21"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="21"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C7" s="4">
+        <v>625</v>
+      </c>
+      <c r="D7" s="6">
+        <v>100</v>
+      </c>
+      <c r="E7" s="4">
+        <v>101</v>
+      </c>
+      <c r="F7" s="4">
+        <v>601</v>
+      </c>
+      <c r="G7" s="21">
+        <v>200</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J7" s="4">
+        <v>70</v>
+      </c>
+      <c r="K7" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L7" s="15">
+        <v>4.7</v>
+      </c>
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
       <c r="O7" s="21"/>
@@ -11514,58 +11611,130 @@
       <c r="R7" s="21"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C8" s="4">
+        <v>625</v>
+      </c>
+      <c r="D8" s="6">
+        <v>65</v>
+      </c>
+      <c r="E8" s="4">
+        <v>101</v>
+      </c>
+      <c r="F8" s="4">
+        <v>601</v>
+      </c>
+      <c r="G8" s="21">
+        <v>200</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J8" s="4">
+        <v>70</v>
+      </c>
+      <c r="K8" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L8" s="15">
+        <v>3.5</v>
+      </c>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
       <c r="O8" s="21"/>
       <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
+      <c r="Q8" s="4"/>
       <c r="R8" s="21"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="6"/>
+      <c r="A9" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C9" s="4">
+        <v>625</v>
+      </c>
+      <c r="D9" s="6">
+        <v>65</v>
+      </c>
+      <c r="E9" s="4">
+        <v>101</v>
+      </c>
+      <c r="F9" s="4">
+        <v>601</v>
+      </c>
+      <c r="G9" s="21">
+        <v>200</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J9" s="21">
+        <v>70</v>
+      </c>
+      <c r="K9" s="23">
+        <v>4890000</v>
+      </c>
+      <c r="L9" s="15">
+        <v>4</v>
+      </c>
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
+      <c r="Q9" s="4"/>
       <c r="R9" s="21"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="6"/>
+      <c r="A10" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C10" s="4">
+        <v>625</v>
+      </c>
+      <c r="D10" s="6">
+        <v>65</v>
+      </c>
+      <c r="E10" s="4">
+        <v>101</v>
+      </c>
+      <c r="F10" s="4">
+        <v>601</v>
+      </c>
+      <c r="G10" s="21">
+        <v>200</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J10" s="21">
+        <v>70</v>
+      </c>
+      <c r="K10" s="23">
+        <v>4890000</v>
+      </c>
+      <c r="L10" s="15">
+        <v>5</v>
+      </c>
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
       <c r="O10" s="21"/>
@@ -11574,98 +11743,218 @@
       <c r="R10" s="21"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="6"/>
+      <c r="A11" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C11" s="4">
+        <v>625</v>
+      </c>
+      <c r="D11" s="6">
+        <v>65</v>
+      </c>
+      <c r="E11" s="21">
+        <v>101</v>
+      </c>
+      <c r="F11" s="21">
+        <v>601</v>
+      </c>
+      <c r="G11" s="21">
+        <v>200</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="J11" s="21">
+        <v>48</v>
+      </c>
+      <c r="K11" s="23">
+        <v>4890000</v>
+      </c>
+      <c r="L11" s="6">
+        <v>4.7</v>
+      </c>
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
       <c r="O11" s="21"/>
       <c r="P11" s="21"/>
-      <c r="Q11" s="4"/>
+      <c r="Q11" s="21"/>
       <c r="R11" s="21"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="15"/>
+      <c r="A12" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C12" s="4">
+        <v>625</v>
+      </c>
+      <c r="D12" s="6">
+        <v>100</v>
+      </c>
+      <c r="E12" s="21">
+        <v>101</v>
+      </c>
+      <c r="F12" s="21">
+        <v>601</v>
+      </c>
+      <c r="G12" s="21">
+        <v>200</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="J12" s="4">
+        <v>48</v>
+      </c>
+      <c r="K12" s="4">
+        <v>4890000</v>
+      </c>
+      <c r="L12" s="6">
+        <v>4.7</v>
+      </c>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
       <c r="O12" s="21"/>
       <c r="P12" s="21"/>
-      <c r="Q12" s="4"/>
+      <c r="Q12" s="21"/>
       <c r="R12" s="21"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="15"/>
+      <c r="A13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C13" s="4">
+        <v>625</v>
+      </c>
+      <c r="D13" s="6">
+        <v>156</v>
+      </c>
+      <c r="E13" s="21">
+        <v>101</v>
+      </c>
+      <c r="F13" s="21">
+        <v>601</v>
+      </c>
+      <c r="G13" s="21">
+        <v>200</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="J13" s="21">
+        <v>48</v>
+      </c>
+      <c r="K13" s="23">
+        <v>4890000</v>
+      </c>
+      <c r="L13" s="6">
+        <v>4.7</v>
+      </c>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
       <c r="O13" s="21"/>
-      <c r="P13" s="25"/>
+      <c r="P13" s="21"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="21"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="15"/>
+      <c r="A14" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C14" s="4">
+        <v>625</v>
+      </c>
+      <c r="D14" s="6">
+        <v>78</v>
+      </c>
+      <c r="E14" s="21">
+        <v>101</v>
+      </c>
+      <c r="F14" s="21">
+        <v>601</v>
+      </c>
+      <c r="G14" s="21">
+        <v>200</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="J14" s="21">
+        <v>48</v>
+      </c>
+      <c r="K14" s="23">
+        <v>4890000</v>
+      </c>
+      <c r="L14" s="6">
+        <v>4.7</v>
+      </c>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
       <c r="O14" s="21"/>
-      <c r="P14" s="25"/>
+      <c r="P14" s="21"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="21"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="15"/>
+      <c r="A15" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C15" s="4">
+        <v>625</v>
+      </c>
+      <c r="D15" s="6">
+        <v>65</v>
+      </c>
+      <c r="E15" s="4">
+        <v>101</v>
+      </c>
+      <c r="F15" s="4">
+        <v>601</v>
+      </c>
+      <c r="G15" s="21">
+        <v>200</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J15" s="21">
+        <v>48</v>
+      </c>
+      <c r="K15" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L15" s="15">
+        <v>3.5</v>
+      </c>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
       <c r="O15" s="21"/>
@@ -11674,44 +11963,92 @@
       <c r="R15" s="21"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="15"/>
+      <c r="A16" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C16" s="4">
+        <v>625</v>
+      </c>
+      <c r="D16" s="6">
+        <v>65</v>
+      </c>
+      <c r="E16" s="21">
+        <v>101</v>
+      </c>
+      <c r="F16" s="21">
+        <v>601</v>
+      </c>
+      <c r="G16" s="21">
+        <v>200</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="J16" s="4">
+        <v>48</v>
+      </c>
+      <c r="K16" s="4">
+        <v>4890000</v>
+      </c>
+      <c r="L16" s="6">
+        <v>4</v>
+      </c>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
       <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
+      <c r="P16" s="25"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="21"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="15"/>
+      <c r="A17" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1523</v>
+      </c>
+      <c r="C17" s="4">
+        <v>625</v>
+      </c>
+      <c r="D17" s="6">
+        <v>65</v>
+      </c>
+      <c r="E17" s="4">
+        <v>101</v>
+      </c>
+      <c r="F17" s="4">
+        <v>601</v>
+      </c>
+      <c r="G17" s="21">
+        <v>200</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J17" s="4">
+        <v>48</v>
+      </c>
+      <c r="K17" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L17" s="15">
+        <v>5</v>
+      </c>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
       <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
+      <c r="P17" s="25"/>
       <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
+      <c r="R17" s="21"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
@@ -11729,9 +12066,9 @@
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
       <c r="O18" s="21"/>
-      <c r="P18" s="25"/>
+      <c r="P18" s="21"/>
       <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
+      <c r="R18" s="21"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
@@ -11749,9 +12086,9 @@
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
       <c r="O19" s="21"/>
-      <c r="P19" s="25"/>
+      <c r="P19" s="21"/>
       <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
+      <c r="R19" s="21"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
@@ -11764,7 +12101,7 @@
       <c r="H20" s="21"/>
       <c r="I20" s="22"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="23"/>
+      <c r="K20" s="25"/>
       <c r="L20" s="15"/>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
@@ -11790,7 +12127,7 @@
       <c r="N21" s="21"/>
       <c r="O21" s="21"/>
       <c r="P21" s="25"/>
-      <c r="Q21" s="21"/>
+      <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -11851,7 +12188,7 @@
       <c r="O24" s="21"/>
       <c r="P24" s="25"/>
       <c r="Q24" s="21"/>
-      <c r="R24" s="4"/>
+      <c r="R24" s="21"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
@@ -11960,7 +12297,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="21"/>
+      <c r="G30" s="4"/>
       <c r="H30" s="21"/>
       <c r="I30" s="22"/>
       <c r="J30" s="4"/>
@@ -11969,7 +12306,7 @@
       <c r="M30" s="21"/>
       <c r="N30" s="21"/>
       <c r="O30" s="21"/>
-      <c r="P30" s="25"/>
+      <c r="P30" s="21"/>
       <c r="Q30" s="21"/>
       <c r="R30" s="21"/>
     </row>
@@ -11989,7 +12326,7 @@
       <c r="M31" s="21"/>
       <c r="N31" s="21"/>
       <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
+      <c r="P31" s="25"/>
       <c r="Q31" s="21"/>
       <c r="R31" s="21"/>
     </row>
@@ -12020,7 +12357,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="G33" s="21"/>
       <c r="H33" s="21"/>
       <c r="I33" s="22"/>
       <c r="J33" s="4"/>
@@ -12069,12 +12406,12 @@
       <c r="M35" s="21"/>
       <c r="N35" s="21"/>
       <c r="O35" s="21"/>
-      <c r="P35" s="25"/>
+      <c r="P35" s="21"/>
       <c r="Q35" s="21"/>
       <c r="R35" s="21"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="6"/>
@@ -12094,7 +12431,7 @@
       <c r="R36" s="21"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
+      <c r="A37" s="6"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="6"/>
@@ -12109,7 +12446,7 @@
       <c r="M37" s="21"/>
       <c r="N37" s="21"/>
       <c r="O37" s="21"/>
-      <c r="P37" s="21"/>
+      <c r="P37" s="25"/>
       <c r="Q37" s="21"/>
       <c r="R37" s="21"/>
     </row>
@@ -12194,9 +12531,9 @@
       <c r="R41" s="21"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
       <c r="D42" s="6"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -12209,14 +12546,14 @@
       <c r="M42" s="21"/>
       <c r="N42" s="21"/>
       <c r="O42" s="21"/>
-      <c r="P42" s="25"/>
+      <c r="P42" s="21"/>
       <c r="Q42" s="21"/>
       <c r="R42" s="21"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
       <c r="D43" s="6"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -12229,7 +12566,7 @@
       <c r="M43" s="21"/>
       <c r="N43" s="21"/>
       <c r="O43" s="21"/>
-      <c r="P43" s="21"/>
+      <c r="P43" s="25"/>
       <c r="Q43" s="21"/>
       <c r="R43" s="21"/>
     </row>
@@ -12249,7 +12586,7 @@
       <c r="M44" s="21"/>
       <c r="N44" s="21"/>
       <c r="O44" s="21"/>
-      <c r="P44" s="25"/>
+      <c r="P44" s="21"/>
       <c r="Q44" s="21"/>
       <c r="R44" s="21"/>
     </row>
@@ -12289,7 +12626,7 @@
       <c r="M46" s="21"/>
       <c r="N46" s="21"/>
       <c r="O46" s="21"/>
-      <c r="P46" s="21"/>
+      <c r="P46" s="25"/>
       <c r="Q46" s="21"/>
       <c r="R46" s="21"/>
     </row>
@@ -12298,23 +12635,23 @@
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="6"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
+      <c r="I47" s="21"/>
       <c r="J47" s="4"/>
-      <c r="K47" s="25"/>
-      <c r="L47" s="15"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="6"/>
       <c r="M47" s="21"/>
       <c r="N47" s="21"/>
       <c r="O47" s="21"/>
-      <c r="P47" s="25"/>
+      <c r="P47" s="21"/>
       <c r="Q47" s="21"/>
       <c r="R47" s="21"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+      <c r="A48" s="16"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="6"/>
@@ -12334,21 +12671,21 @@
       <c r="R48" s="21"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
+      <c r="A49" s="6"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="6"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
       <c r="H49" s="21"/>
       <c r="I49" s="21"/>
       <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
+      <c r="K49" s="23"/>
       <c r="L49" s="6"/>
-      <c r="M49" s="21"/>
-      <c r="N49" s="21"/>
-      <c r="O49" s="21"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
       <c r="P49" s="21"/>
       <c r="Q49" s="21"/>
       <c r="R49" s="21"/>
@@ -12366,32 +12703,21 @@
       <c r="J50" s="4"/>
       <c r="K50" s="23"/>
       <c r="L50" s="6"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="21"/>
       <c r="P50" s="21"/>
       <c r="Q50" s="21"/>
       <c r="R50" s="21"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="23"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="21"/>
-      <c r="O51" s="21"/>
-      <c r="P51" s="21"/>
-      <c r="Q51" s="21"/>
-      <c r="R51" s="21"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="3"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="3"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
@@ -12428,15 +12754,6 @@
       <c r="J55" s="8"/>
       <c r="K55" s="8"/>
       <c r="L55" s="3"/>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="3"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add axisymmetric data to graphs
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8573F401-0D6F-49EF-BC89-508B21B11B60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735C9C67-836E-4C31-BD83-04EBAB6A9E9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" firstSheet="1" activeTab="2" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
   </bookViews>
   <sheets>
     <sheet name="ConstantPropPlanar" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="146">
   <si>
     <t>Folder ID</t>
   </si>
@@ -448,9 +448,6 @@
     <t>0.89 (WU)</t>
   </si>
   <si>
-    <t>Higher A0; no ignition by 3.66 ms</t>
-  </si>
-  <si>
     <t>2D Planar Conduction</t>
   </si>
   <si>
@@ -463,16 +460,7 @@
     <t>-Axisymmetric</t>
   </si>
   <si>
-    <t>0.19 (WW)</t>
-  </si>
-  <si>
     <t>0.20 (WW)</t>
-  </si>
-  <si>
-    <t>No ignition 1ms, 880 K</t>
-  </si>
-  <si>
-    <t>No ignition 1.6 ms, 550 K</t>
   </si>
   <si>
     <t>No ignition 1.6 ms, 780 K</t>
@@ -482,6 +470,12 @@
   </si>
   <si>
     <t>No ignition 1.6 ms, 960 K</t>
+  </si>
+  <si>
+    <t>0.27 (WW)</t>
+  </si>
+  <si>
+    <t>◘</t>
   </si>
 </sst>
 </file>
@@ -552,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -589,6 +583,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1733,9 +1728,21 @@
               <c:f>(ConstantPropPlanar!$K$25,ConstantPropPlanar!$K$38,ConstantPropPlanar!$K$39,ConstantPropPlanar!$K$40,ConstantPropPlanar!$K$41)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4890000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1745,9 +1752,21 @@
               <c:f>(ConstantPropPlanar!$M$25,ConstantPropPlanar!$M$38,ConstantPropPlanar!$M$39,ConstantPropPlanar!$M$40,ConstantPropPlanar!$M$41)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1813,9 +1832,21 @@
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>0.00E+00</c:formatCode>
-                      <c:ptCount val="1"/>
+                      <c:ptCount val="5"/>
                       <c:pt idx="0">
                         <c:v>4890000</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>5000000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5500000</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6000000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>8000000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1831,9 +1862,21 @@
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="1"/>
+                      <c:ptCount val="5"/>
                       <c:pt idx="0">
                         <c:v>9.6</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>9.6</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>10.1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>10.4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11.7</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2288,6 +2331,146 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Ea=48,axi</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(ConstantPropAxisym!$L$15,ConstantPropAxisym!$L$16,ConstantPropAxisym!$L$11,ConstantPropAxisym!$L$17)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(ConstantPropAxisym!$N$15,ConstantPropAxisym!$N$16,ConstantPropAxisym!$N$11,ConstantPropAxisym!$N$17)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E2AA-468B-842B-D504A447A73F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Ea=70,axi</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ConstantPropAxisym!$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ConstantPropAxisym!$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>9.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E2AA-468B-842B-D504A447A73F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2443,6 +2626,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Wave Speed (m/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2719,7 +2957,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2806,6 +3044,146 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-28F6-448C-8745-E89CBB219AE3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Ea=48,axi</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(ConstantPropAxisym!$D$11,ConstantPropAxisym!$D$12,ConstantPropAxisym!$D$13,ConstantPropAxisym!$D$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>156</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(ConstantPropAxisym!$N$11,ConstantPropAxisym!$N$12,ConstantPropAxisym!$N$13,ConstantPropAxisym!$N$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0D9C-4227-A114-FB42154A396A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Ea=70,axi</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ConstantPropAxisym!$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ConstantPropAxisym!$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>9.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0D9C-4227-A114-FB42154A396A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3322,6 +3700,146 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Ea=48,axi</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(ConstantPropAxisym!$L$15,ConstantPropAxisym!$L$16,ConstantPropAxisym!$L$11,ConstantPropAxisym!$L$17)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(ConstantPropAxisym!$M$15,ConstantPropAxisym!$M$16,ConstantPropAxisym!$M$11,ConstantPropAxisym!$M$17)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D91-4FBB-8651-5701EF1E22B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Ea=70,axi</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ConstantPropAxisym!$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ConstantPropAxisym!$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2D91-4FBB-8651-5701EF1E22B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -3821,7 +4339,7 @@
                   <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3830,6 +4348,146 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6926-48B4-A13B-DC079EAA164D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Ea=48,axi</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(ConstantPropAxisym!$D$11,ConstantPropAxisym!$D$12,ConstantPropAxisym!$D$13,ConstantPropAxisym!$D$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>156</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(ConstantPropAxisym!$M$11,ConstantPropAxisym!$M$12,ConstantPropAxisym!$M$13,ConstantPropAxisym!$M$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB22-4104-A786-BA761AE19B72}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Ea=70,axi</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ConstantPropAxisym!$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ConstantPropAxisym!$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EB22-4104-A786-BA761AE19B72}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8925,10 +9583,10 @@
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="11" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="11" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
+      <selection pane="bottomRight" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8952,7 +9610,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>43</v>
@@ -8965,7 +9623,7 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
@@ -9500,7 +10158,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="8">
         <v>1523</v>
@@ -9755,7 +10413,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>94</v>
       </c>
@@ -10365,22 +11023,19 @@
         <v>4.7</v>
       </c>
       <c r="M31">
-        <v>4</v>
-      </c>
-      <c r="N31" t="s">
-        <v>79</v>
-      </c>
-      <c r="O31" t="s">
-        <v>79</v>
-      </c>
-      <c r="P31" t="s">
-        <v>79</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N31">
+        <v>15.3</v>
+      </c>
+      <c r="O31">
+        <v>7900</v>
+      </c>
+      <c r="P31" s="2">
+        <v>600000</v>
       </c>
       <c r="Q31" t="s">
         <v>131</v>
-      </c>
-      <c r="R31" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -10624,7 +11279,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="15"/>
     </row>
-    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>1</v>
       </c>
@@ -10677,7 +11332,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>2</v>
       </c>
@@ -10733,7 +11388,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>3</v>
       </c>
@@ -10789,7 +11444,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>4</v>
       </c>
@@ -10845,7 +11500,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>5</v>
       </c>
@@ -11307,11 +11962,6 @@
         <filter val="1523"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="10">
-      <filters>
-        <filter val="4.89E+06"/>
-      </filters>
-    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11320,14 +11970,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBE568B-3744-4C31-902D-5B6E8133C9BD}">
-  <dimension ref="A1"/>
+  <dimension ref="T20"/>
   <sheetViews>
-    <sheetView topLeftCell="J19" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="20" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -11337,11 +11993,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B099DE-69DA-496C-8376-9BFCA5F25F37}">
   <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
+      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11365,7 +12021,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>43</v>
@@ -11442,7 +12098,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -11459,52 +12115,52 @@
       <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="11">
         <v>1523</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="11">
         <v>625</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="10">
         <v>65</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="12">
         <v>101</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="12">
         <v>601</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="12">
         <v>200</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="12">
         <v>0.8</v>
       </c>
-      <c r="J4" s="21">
+      <c r="J4" s="12">
         <v>70</v>
       </c>
-      <c r="K4" s="23">
+      <c r="K4" s="26">
         <v>4890000</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="10">
         <v>4.7</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="M4" s="11">
+        <v>3.1</v>
+      </c>
+      <c r="N4" s="11">
+        <v>9.6</v>
+      </c>
+      <c r="O4" s="11"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="4" t="s">
-        <v>143</v>
-      </c>
+      <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -11551,7 +12207,7 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -11576,7 +12232,7 @@
       <c r="G6" s="21">
         <v>200</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="22">
@@ -11620,7 +12276,7 @@
       <c r="G7" s="21">
         <v>200</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="22">
@@ -11664,7 +12320,7 @@
       <c r="G8" s="21">
         <v>200</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I8" s="22">
@@ -11708,7 +12364,7 @@
       <c r="G9" s="21">
         <v>200</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="22">
@@ -11752,7 +12408,7 @@
       <c r="G10" s="21">
         <v>200</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="22">
@@ -11775,66 +12431,66 @@
       <c r="P10" s="21"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="11">
         <v>1523</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="11">
         <v>625</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="10">
         <v>65</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="12">
         <v>101</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="12">
         <v>601</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="12">
         <v>200</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="12">
         <v>0.8</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="12">
         <v>48</v>
       </c>
-      <c r="K11" s="23">
+      <c r="K11" s="26">
         <v>4890000</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="10">
         <v>4.7</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="11">
         <v>0.18</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="11">
         <v>13.5</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11" s="11">
         <v>7800</v>
       </c>
       <c r="P11" s="25">
         <v>700000</v>
       </c>
       <c r="Q11" s="21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="R11" s="21"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B12" s="4">
         <v>1523</v>
@@ -11843,7 +12499,7 @@
         <v>625</v>
       </c>
       <c r="D12" s="6">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E12" s="21">
         <v>101</v>
@@ -11854,41 +12510,37 @@
       <c r="G12" s="21">
         <v>200</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="21">
         <v>0.8</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="21">
         <v>48</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="23">
         <v>4890000</v>
       </c>
       <c r="L12" s="6">
         <v>4.7</v>
       </c>
       <c r="M12" s="4">
-        <v>0.45</v>
+        <v>0.24</v>
       </c>
       <c r="N12" s="4">
-        <v>17.2</v>
+        <v>15.1</v>
       </c>
       <c r="O12" s="4">
         <v>7800</v>
       </c>
-      <c r="P12" s="25">
-        <v>900000</v>
-      </c>
-      <c r="Q12" s="21" t="s">
-        <v>146</v>
-      </c>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="21"/>
       <c r="R12" s="21"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="B13" s="4">
         <v>1523</v>
@@ -11897,7 +12549,7 @@
         <v>625</v>
       </c>
       <c r="D13" s="6">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="E13" s="21">
         <v>101</v>
@@ -11914,29 +12566,35 @@
       <c r="I13" s="21">
         <v>0.8</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="4">
         <v>48</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="4">
         <v>4890000</v>
       </c>
       <c r="L13" s="6">
         <v>4.7</v>
       </c>
-      <c r="M13" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="21" t="s">
-        <v>144</v>
-      </c>
+      <c r="M13" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="N13" s="4">
+        <v>17.2</v>
+      </c>
+      <c r="O13" s="4">
+        <v>7800</v>
+      </c>
+      <c r="P13" s="25">
+        <v>900000</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="R13" s="21"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B14" s="4">
         <v>1523</v>
@@ -11945,7 +12603,7 @@
         <v>625</v>
       </c>
       <c r="D14" s="6">
-        <v>78</v>
+        <v>156</v>
       </c>
       <c r="E14" s="21">
         <v>101</v>
@@ -11971,21 +12629,15 @@
       <c r="L14" s="6">
         <v>4.7</v>
       </c>
-      <c r="M14" s="4">
-        <v>0.24</v>
+      <c r="M14" s="21">
+        <v>6.1</v>
       </c>
       <c r="N14" s="4">
-        <v>15.1</v>
-      </c>
-      <c r="O14" s="4">
-        <v>7800</v>
-      </c>
-      <c r="P14" s="25">
-        <v>900000</v>
-      </c>
-      <c r="Q14" s="4" t="s">
-        <v>141</v>
-      </c>
+        <v>19.3</v>
+      </c>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="4"/>
       <c r="R14" s="21"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -12010,7 +12662,7 @@
       <c r="G15" s="21">
         <v>200</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I15" s="22">
@@ -12025,11 +12677,21 @@
       <c r="L15" s="15">
         <v>3.5</v>
       </c>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="4"/>
+      <c r="M15" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="N15" s="4">
+        <v>10.7</v>
+      </c>
+      <c r="O15" s="4">
+        <v>6000</v>
+      </c>
+      <c r="P15" s="25">
+        <v>700000</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="R15" s="21"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -12054,7 +12716,7 @@
       <c r="G16" s="21">
         <v>200</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I16" s="21">
@@ -12069,11 +12731,21 @@
       <c r="L16" s="6">
         <v>4</v>
       </c>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="4"/>
+      <c r="M16" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="N16" s="4">
+        <v>12</v>
+      </c>
+      <c r="O16" s="4">
+        <v>6600</v>
+      </c>
+      <c r="P16" s="25">
+        <v>800000</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="R16" s="21"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -12098,7 +12770,7 @@
       <c r="G17" s="21">
         <v>200</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I17" s="22">
@@ -12113,11 +12785,21 @@
       <c r="L17" s="15">
         <v>5</v>
       </c>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="4"/>
+      <c r="M17" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="N17" s="4">
+        <v>14.2</v>
+      </c>
+      <c r="O17" s="4">
+        <v>8000</v>
+      </c>
+      <c r="P17" s="25">
+        <v>1000000</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="R17" s="21"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -12835,7 +13517,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9188EC-3268-404A-8733-94DAF537670F}">
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Sync in prep for merge with master
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7117C6-B5EC-4185-823A-FA222D8B88F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4548CB0D-7254-405F-8D73-12A7C58721AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" firstSheet="1" activeTab="2" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="150">
   <si>
     <t>Folder ID</t>
   </si>
@@ -295,9 +295,6 @@
     <t>dH from Kim 2014, A0 from Stacy 2013; diverge at 0.23 ms because of eta</t>
   </si>
   <si>
-    <t>RED-MJ/kg</t>
-  </si>
-  <si>
     <t>AlMoO3-6</t>
   </si>
   <si>
@@ -479,6 +476,18 @@
   </si>
   <si>
     <t>2D Planar w/ variable eta (First runs)</t>
+  </si>
+  <si>
+    <t>dH [MJ/kg]</t>
+  </si>
+  <si>
+    <t>RED-kJ/cm^3</t>
+  </si>
+  <si>
+    <t>Fully compact pellet</t>
+  </si>
+  <si>
+    <t>60% porosity</t>
   </si>
 </sst>
 </file>
@@ -9622,7 +9631,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>43</v>
@@ -9635,7 +9644,7 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
@@ -9688,7 +9697,7 @@
         <v>36</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>57</v>
@@ -9991,7 +10000,7 @@
     </row>
     <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -10003,7 +10012,7 @@
     </row>
     <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -10059,7 +10068,7 @@
       </c>
       <c r="Q12" s="4"/>
       <c r="R12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -10373,7 +10382,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="8">
         <v>1523</v>
@@ -10422,12 +10431,12 @@
       </c>
       <c r="Q19" s="4"/>
       <c r="R19" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" s="8">
         <v>1523</v>
@@ -10473,12 +10482,12 @@
       </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B21" s="8">
         <v>1523</v>
@@ -10526,7 +10535,7 @@
         <v>1000000</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -10579,7 +10588,7 @@
         <v>1000000</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -10632,12 +10641,12 @@
         <v>900000</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="8">
         <v>2020</v>
@@ -10685,12 +10694,12 @@
         <v>600000</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="11">
         <v>1523</v>
@@ -10740,7 +10749,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="4">
         <v>1523</v>
@@ -10790,7 +10799,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27" s="8">
         <v>1523</v>
@@ -10840,7 +10849,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B28" s="4">
         <v>1523</v>
@@ -10888,12 +10897,12 @@
         <v>800000</v>
       </c>
       <c r="Q28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" s="4">
         <v>1523</v>
@@ -10941,12 +10950,12 @@
         <v>700000</v>
       </c>
       <c r="Q29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B30" s="4">
         <v>1523</v>
@@ -10994,12 +11003,12 @@
         <v>1000000</v>
       </c>
       <c r="Q30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B31" s="4">
         <v>1523</v>
@@ -11047,12 +11056,12 @@
         <v>600000</v>
       </c>
       <c r="Q31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B32" s="4">
         <v>1523</v>
@@ -11100,12 +11109,12 @@
         <v>500000</v>
       </c>
       <c r="Q32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B33" s="4">
         <v>1523</v>
@@ -11153,12 +11162,12 @@
         <v>600000</v>
       </c>
       <c r="Q33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" s="8">
         <v>1523</v>
@@ -11206,15 +11215,15 @@
         <v>0</v>
       </c>
       <c r="Q34" t="s">
+        <v>132</v>
+      </c>
+      <c r="R34" t="s">
         <v>133</v>
-      </c>
-      <c r="R34" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B35" s="4">
         <v>1523</v>
@@ -11262,7 +11271,7 @@
         <v>400000</v>
       </c>
       <c r="Q35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -11279,7 +11288,7 @@
     </row>
     <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -11341,7 +11350,7 @@
         <v>680000</v>
       </c>
       <c r="R38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -11394,10 +11403,10 @@
         <v>700000</v>
       </c>
       <c r="Q39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -11450,10 +11459,10 @@
         <v>800000</v>
       </c>
       <c r="Q40" t="s">
+        <v>102</v>
+      </c>
+      <c r="R40" t="s">
         <v>103</v>
-      </c>
-      <c r="R40" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -11506,10 +11515,10 @@
         <v>1200000</v>
       </c>
       <c r="Q41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -11562,15 +11571,15 @@
         <v>1200000</v>
       </c>
       <c r="Q42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R42" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="8"/>
@@ -11582,7 +11591,7 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B44" s="4">
         <v>1523</v>
@@ -11632,7 +11641,7 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B45" s="4">
         <v>1523</v>
@@ -11679,7 +11688,7 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B46" s="4">
         <v>1523</v>
@@ -11726,7 +11735,7 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B47" s="8">
         <v>1523</v>
@@ -11774,7 +11783,7 @@
         <v>600000</v>
       </c>
       <c r="Q47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
@@ -11788,7 +11797,7 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -11799,7 +11808,7 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B50" s="4">
         <v>2043</v>
@@ -11844,12 +11853,12 @@
         <v>7600</v>
       </c>
       <c r="R50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B51" s="4">
         <v>2043</v>
@@ -11992,7 +12001,7 @@
   <sheetData>
     <row r="20" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -12006,10 +12015,10 @@
   <dimension ref="A1:R55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12033,7 +12042,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>43</v>
@@ -12046,7 +12055,7 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="3" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
@@ -12087,7 +12096,7 @@
         <v>4</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>9</v>
@@ -12099,7 +12108,7 @@
         <v>36</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>57</v>
@@ -12110,7 +12119,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -12128,7 +12137,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="11">
         <v>1523</v>
@@ -12176,7 +12185,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="4">
         <v>1523</v>
@@ -12219,12 +12228,12 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="4">
         <v>1523</v>
@@ -12268,7 +12277,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="4">
         <v>1523</v>
@@ -12312,7 +12321,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" s="4">
         <v>1523</v>
@@ -12356,7 +12365,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="4">
         <v>1523</v>
@@ -12400,7 +12409,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" s="4">
         <v>1523</v>
@@ -12443,12 +12452,12 @@
       <c r="P10" s="21"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="11">
         <v>1523</v>
@@ -12496,13 +12505,13 @@
         <v>700000</v>
       </c>
       <c r="Q11" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R11" s="21"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="4">
         <v>1523</v>
@@ -12552,7 +12561,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="4">
         <v>1523</v>
@@ -12600,7 +12609,7 @@
         <v>900000</v>
       </c>
       <c r="Q13" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="R13" s="21"/>
     </row>
@@ -12654,7 +12663,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15" s="4">
         <v>1523</v>
@@ -12702,13 +12711,13 @@
         <v>700000</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R15" s="21"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" s="4">
         <v>1523</v>
@@ -12756,13 +12765,13 @@
         <v>800000</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R16" s="21"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" s="4">
         <v>1523</v>
@@ -12810,7 +12819,7 @@
         <v>1000000</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R17" s="21"/>
     </row>
@@ -12836,25 +12845,45 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B19" s="4"/>
+        <v>127</v>
+      </c>
+      <c r="B19" s="4">
+        <v>5109</v>
+      </c>
       <c r="C19" s="4"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="15"/>
+      <c r="E19" s="4">
+        <v>101</v>
+      </c>
+      <c r="F19" s="4">
+        <v>601</v>
+      </c>
+      <c r="G19" s="21">
+        <v>200</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J19" s="4">
+        <v>48</v>
+      </c>
+      <c r="K19" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L19" s="15">
+        <v>4.07</v>
+      </c>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
       <c r="O19" s="21"/>
       <c r="P19" s="21"/>
       <c r="Q19" s="4"/>
-      <c r="R19" s="21"/>
+      <c r="R19" s="21" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
@@ -12878,23 +12907,43 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4">
+        <v>3065</v>
+      </c>
       <c r="C21" s="4"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="15"/>
+      <c r="E21" s="4">
+        <v>101</v>
+      </c>
+      <c r="F21" s="4">
+        <v>601</v>
+      </c>
+      <c r="G21" s="21">
+        <v>200</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J21" s="4">
+        <v>48</v>
+      </c>
+      <c r="K21" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L21" s="15">
+        <v>4.07</v>
+      </c>
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
       <c r="O21" s="21"/>
       <c r="P21" s="25"/>
       <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
+      <c r="R21" s="4" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
@@ -15120,7 +15169,7 @@
       <c r="A42" s="6"/>
       <c r="B42" s="4"/>
       <c r="C42" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I42" s="3"/>
     </row>

</xml_diff>

<commit_message>
Tests without source term
</commit_message>
<xml_diff>
--- a/Tests/All_Data.xlsx
+++ b/Tests/All_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepps\Documents\Research\2D_Conduction\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579A8848-805F-4964-821A-9843026B7D5D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1921BA1-2B71-4928-A352-04E7CA1527F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B2402E43-B038-44F0-8C18-7ACD788C4A69}"/>
   </bookViews>
   <sheets>
     <sheet name="Conserv" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Conserv!$A$2:$R$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'nano-Axi'!$A$2:$R$26</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Tests-Axi'!$A$2:$R$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Tests-Axi'!$A$2:$R$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">VarPropEta!$A$2:$O$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="242">
   <si>
     <t>Folder ID</t>
   </si>
@@ -603,12 +603,6 @@
     <t>[New ignition criteria, burn rate down r=0]</t>
   </si>
   <si>
-    <t>--ablation</t>
-  </si>
-  <si>
-    <t>base</t>
-  </si>
-  <si>
     <t>eta,601,998</t>
   </si>
   <si>
@@ -654,19 +648,10 @@
     <t>Florin flux with even higher k</t>
   </si>
   <si>
-    <t>Al</t>
-  </si>
-  <si>
     <t>comp</t>
   </si>
   <si>
     <t>CuO</t>
-  </si>
-  <si>
-    <t>0.061 (6)</t>
-  </si>
-  <si>
-    <t>Al thermal properties; Run for 100 ms; possible ign around 40 ms</t>
   </si>
   <si>
     <t>Al/CuO composite;</t>
@@ -760,6 +745,30 @@
   </si>
   <si>
     <t>--AlCuO</t>
+  </si>
+  <si>
+    <t>Al thermal properties;</t>
+  </si>
+  <si>
+    <t>--Al</t>
+  </si>
+  <si>
+    <t>Flipped dimensions of 1</t>
+  </si>
+  <si>
+    <t>--noSource</t>
+  </si>
+  <si>
+    <t>Temperature profile evolution; to 0.5 s</t>
+  </si>
+  <si>
+    <t>Laser heating 0.2mm from edge</t>
+  </si>
+  <si>
+    <t>Laser heating 0.05 mm from edge</t>
+  </si>
+  <si>
+    <t>Laser heating 0.05 mm from edge; higher flux; instabilities</t>
   </si>
 </sst>
 </file>
@@ -16566,13 +16575,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B099DE-69DA-496C-8376-9BFCA5F25F37}">
-  <dimension ref="A1:R62"/>
+  <dimension ref="A1:R58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="P18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R36" sqref="R36"/>
+      <selection pane="bottomRight" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16607,10 +16616,10 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
@@ -16621,7 +16630,7 @@
         <v>8</v>
       </c>
       <c r="O1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -16700,7 +16709,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -17406,7 +17415,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -17490,16 +17499,16 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B22" s="4">
-        <v>2702</v>
+        <v>5643</v>
       </c>
       <c r="C22" s="4">
-        <v>903</v>
+        <v>599</v>
       </c>
       <c r="D22" s="6">
-        <v>237</v>
+        <v>39</v>
       </c>
       <c r="E22" s="4">
         <v>100</v>
@@ -17525,19 +17534,19 @@
       <c r="L22" s="15">
         <v>2.78</v>
       </c>
-      <c r="M22" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="N22" s="21" t="s">
-        <v>79</v>
+      <c r="M22" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="N22" s="21">
+        <v>6.21</v>
       </c>
       <c r="O22" s="21"/>
       <c r="P22" s="21"/>
       <c r="Q22" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="R22" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
+      </c>
+      <c r="R22" s="21" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -17551,8 +17560,6 @@
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="15"/>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
       <c r="O23" s="21"/>
@@ -17562,16 +17569,16 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B24" s="4">
-        <v>5643</v>
+        <v>6315</v>
       </c>
       <c r="C24" s="4">
-        <v>599</v>
+        <v>529</v>
       </c>
       <c r="D24" s="6">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E24" s="4">
         <v>100</v>
@@ -17601,122 +17608,142 @@
         <v>0.5</v>
       </c>
       <c r="N24" s="21">
-        <v>6.21</v>
+        <v>10.8</v>
       </c>
       <c r="O24" s="21"/>
       <c r="P24" s="21"/>
       <c r="Q24" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="R24" s="21" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="6"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="22"/>
       <c r="J25" s="4"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="15"/>
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
       <c r="O25" s="21"/>
       <c r="P25" s="21"/>
       <c r="Q25" s="4"/>
-      <c r="R25" s="21"/>
+      <c r="R25" s="4"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="B26" s="4">
-        <v>6315</v>
-      </c>
-      <c r="C26" s="4">
-        <v>529</v>
-      </c>
-      <c r="D26" s="6">
-        <v>33</v>
-      </c>
-      <c r="E26" s="4">
+        <v>187</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4">
+        <v>3065</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D27" s="6">
+        <v>65</v>
+      </c>
+      <c r="E27" s="4">
         <v>100</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F27" s="4">
         <v>600</v>
       </c>
-      <c r="G26" s="4">
-        <v>200</v>
-      </c>
-      <c r="H26" s="22" t="s">
+      <c r="G27" s="4">
+        <v>20</v>
+      </c>
+      <c r="H27" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I27" s="22">
         <v>0.8</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J27" s="4">
         <v>48</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K27" s="25">
         <v>4890000</v>
       </c>
-      <c r="L26" s="15">
+      <c r="L27" s="15">
         <v>2.78</v>
       </c>
-      <c r="M26" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="N26" s="21">
-        <v>10.8</v>
-      </c>
-      <c r="O26" s="21"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="R26" s="21" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="15"/>
       <c r="M27" s="21"/>
       <c r="N27" s="21"/>
       <c r="O27" s="21"/>
-      <c r="P27" s="21"/>
+      <c r="P27" s="25"/>
       <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
+      <c r="R27" s="4" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="6">
+        <v>2</v>
+      </c>
+      <c r="B28" s="4">
+        <v>3065</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="15"/>
+      <c r="D28" s="6">
+        <v>65</v>
+      </c>
+      <c r="E28" s="4">
+        <v>100</v>
+      </c>
+      <c r="F28" s="4">
+        <v>600</v>
+      </c>
+      <c r="G28" s="4">
+        <v>60</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J28" s="4">
+        <v>48</v>
+      </c>
+      <c r="K28" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L28" s="15">
+        <v>2.78</v>
+      </c>
       <c r="M28" s="21"/>
       <c r="N28" s="21"/>
       <c r="O28" s="21"/>
@@ -17725,14 +17752,14 @@
       <c r="R28" s="4"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>187</v>
+      <c r="A29" s="6">
+        <v>3</v>
       </c>
       <c r="B29" s="4">
         <v>3065</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D29" s="6">
         <v>65</v>
@@ -17744,9 +17771,9 @@
         <v>600</v>
       </c>
       <c r="G29" s="4">
-        <v>200</v>
-      </c>
-      <c r="H29" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="H29" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I29" s="22">
@@ -17762,10 +17789,10 @@
         <v>2.78</v>
       </c>
       <c r="M29" s="21">
-        <v>0.38</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="N29" s="21">
-        <v>4.72</v>
+        <v>4.91</v>
       </c>
       <c r="O29" s="21"/>
       <c r="P29" s="25"/>
@@ -17773,13 +17800,15 @@
       <c r="R29" s="4"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+      <c r="A30" s="6" t="s">
+        <v>185</v>
+      </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="6"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="G30" s="21"/>
       <c r="H30" s="21"/>
       <c r="I30" s="22"/>
       <c r="J30" s="4"/>
@@ -17789,40 +17818,72 @@
       <c r="N30" s="21"/>
       <c r="O30" s="21"/>
       <c r="P30" s="25"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="6">
+        <v>5</v>
+      </c>
+      <c r="B31" s="4">
+        <v>3065</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31" s="6">
+        <v>65</v>
+      </c>
+      <c r="E31" s="4">
+        <v>100</v>
+      </c>
+      <c r="F31" s="4">
+        <v>600</v>
+      </c>
+      <c r="G31" s="4">
+        <v>400</v>
+      </c>
+      <c r="H31" s="21">
+        <v>10</v>
+      </c>
+      <c r="I31" s="22">
+        <v>15</v>
+      </c>
+      <c r="J31" s="4">
+        <v>48</v>
+      </c>
+      <c r="K31" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L31" s="15">
+        <v>2.78</v>
+      </c>
+      <c r="M31" s="21">
+        <v>0.13</v>
+      </c>
+      <c r="N31" s="21">
+        <v>3.92</v>
+      </c>
+      <c r="O31" s="4">
+        <v>2245</v>
+      </c>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="25"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
+      <c r="R31" s="21" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B32" s="4">
         <v>3065</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D32" s="6">
         <v>65</v>
@@ -17834,13 +17895,13 @@
         <v>600</v>
       </c>
       <c r="G32" s="4">
-        <v>20</v>
-      </c>
-      <c r="H32" s="22" t="s">
-        <v>6</v>
+        <v>100</v>
+      </c>
+      <c r="H32" s="21">
+        <v>10</v>
       </c>
       <c r="I32" s="22">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J32" s="4">
         <v>48</v>
@@ -17851,24 +17912,32 @@
       <c r="L32" s="15">
         <v>2.78</v>
       </c>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="21"/>
+      <c r="M32" s="21">
+        <v>2.41</v>
+      </c>
+      <c r="N32" s="21">
+        <v>3.73</v>
+      </c>
+      <c r="O32" s="4">
+        <v>877</v>
+      </c>
       <c r="P32" s="25"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4" t="s">
-        <v>190</v>
+      <c r="Q32" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="R32" s="21" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B33" s="4">
         <v>3065</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D33" s="6">
         <v>65</v>
@@ -17880,13 +17949,13 @@
         <v>600</v>
       </c>
       <c r="G33" s="4">
-        <v>60</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>6</v>
+        <v>50</v>
+      </c>
+      <c r="H33" s="21">
+        <v>10</v>
       </c>
       <c r="I33" s="22">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J33" s="4">
         <v>48</v>
@@ -17897,25 +17966,35 @@
       <c r="L33" s="15">
         <v>2.78</v>
       </c>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
+      <c r="M33" s="21">
+        <v>47.82</v>
+      </c>
+      <c r="N33" s="21">
+        <v>3.36</v>
+      </c>
+      <c r="O33" s="4">
+        <v>689</v>
+      </c>
       <c r="P33" s="25"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
+      <c r="Q33" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="R33" s="21" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B34" s="4">
         <v>3065</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D34" s="6">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="E34" s="4">
         <v>100</v>
@@ -17924,13 +18003,13 @@
         <v>600</v>
       </c>
       <c r="G34" s="4">
-        <v>100</v>
-      </c>
-      <c r="H34" s="22" t="s">
-        <v>6</v>
+        <v>400</v>
+      </c>
+      <c r="H34" s="21">
+        <v>10</v>
       </c>
       <c r="I34" s="22">
-        <v>0.8</v>
+        <v>15</v>
       </c>
       <c r="J34" s="4">
         <v>48</v>
@@ -17942,167 +18021,139 @@
         <v>2.78</v>
       </c>
       <c r="M34" s="21">
-        <v>2.4500000000000002</v>
+        <v>0.2</v>
       </c>
       <c r="N34" s="21">
-        <v>4.91</v>
-      </c>
-      <c r="O34" s="21"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="O34" s="4">
+        <v>1985</v>
+      </c>
       <c r="P34" s="25"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
+      <c r="Q34" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="R34" s="21" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21"/>
+      <c r="A35" s="6">
+        <v>8</v>
+      </c>
+      <c r="B35" s="4">
+        <v>3065</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" s="6">
+        <v>200</v>
+      </c>
+      <c r="E35" s="4">
+        <v>100</v>
+      </c>
+      <c r="F35" s="4">
+        <v>600</v>
+      </c>
+      <c r="G35" s="4">
+        <v>400</v>
+      </c>
+      <c r="H35" s="21">
+        <v>10</v>
+      </c>
+      <c r="I35" s="22">
+        <v>15</v>
+      </c>
+      <c r="J35" s="4">
+        <v>48</v>
+      </c>
+      <c r="K35" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L35" s="15">
+        <v>2.78</v>
+      </c>
+      <c r="M35" s="21">
+        <v>1.07</v>
+      </c>
+      <c r="N35" s="21">
+        <v>6.41</v>
+      </c>
+      <c r="O35" s="4">
+        <v>1004</v>
+      </c>
       <c r="P35" s="25"/>
-      <c r="Q35" s="21"/>
-      <c r="R35" s="21"/>
+      <c r="Q35" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="R35" s="21" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
-        <v>5</v>
-      </c>
-      <c r="B36" s="4">
-        <v>3065</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D36" s="6">
-        <v>65</v>
-      </c>
-      <c r="E36" s="4">
-        <v>100</v>
-      </c>
-      <c r="F36" s="4">
-        <v>600</v>
-      </c>
-      <c r="G36" s="4">
-        <v>400</v>
-      </c>
-      <c r="H36" s="21">
-        <v>10</v>
-      </c>
-      <c r="I36" s="22">
-        <v>15</v>
-      </c>
-      <c r="J36" s="4">
-        <v>48</v>
-      </c>
-      <c r="K36" s="25">
-        <v>4890000</v>
-      </c>
-      <c r="L36" s="15">
-        <v>2.78</v>
-      </c>
-      <c r="M36" s="21">
-        <v>0.13</v>
-      </c>
-      <c r="N36" s="21">
-        <v>3.92</v>
-      </c>
-      <c r="O36" s="4">
-        <v>2245</v>
-      </c>
+      <c r="A36" s="6"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="4"/>
       <c r="P36" s="25"/>
-      <c r="Q36" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="R36" s="21" t="s">
-        <v>192</v>
-      </c>
+      <c r="Q36" s="21"/>
+      <c r="R36" s="21"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
-        <v>4</v>
-      </c>
-      <c r="B37" s="4">
-        <v>3065</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D37" s="6">
-        <v>65</v>
-      </c>
-      <c r="E37" s="4">
-        <v>100</v>
-      </c>
-      <c r="F37" s="4">
-        <v>600</v>
-      </c>
-      <c r="G37" s="4">
-        <v>100</v>
-      </c>
-      <c r="H37" s="21">
-        <v>10</v>
-      </c>
-      <c r="I37" s="22">
+      <c r="A37" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
+      <c r="R37" s="21"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="16">
         <v>1</v>
-      </c>
-      <c r="J37" s="4">
-        <v>48</v>
-      </c>
-      <c r="K37" s="25">
-        <v>4890000</v>
-      </c>
-      <c r="L37" s="15">
-        <v>2.78</v>
-      </c>
-      <c r="M37" s="21">
-        <v>2.41</v>
-      </c>
-      <c r="N37" s="21">
-        <v>3.73</v>
-      </c>
-      <c r="O37" s="4">
-        <v>877</v>
-      </c>
-      <c r="P37" s="25"/>
-      <c r="Q37" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="R37" s="21" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
-        <v>6</v>
       </c>
       <c r="B38" s="4">
         <v>3065</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D38" s="6">
         <v>65</v>
       </c>
       <c r="E38" s="4">
+        <v>300</v>
+      </c>
+      <c r="F38" s="4">
         <v>100</v>
       </c>
-      <c r="F38" s="4">
-        <v>600</v>
-      </c>
       <c r="G38" s="4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H38" s="21">
         <v>10</v>
@@ -18120,40 +18171,40 @@
         <v>2.78</v>
       </c>
       <c r="M38" s="21">
-        <v>47.82</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="N38" s="21">
-        <v>3.36</v>
+        <v>3.18</v>
       </c>
       <c r="O38" s="4">
-        <v>689</v>
-      </c>
-      <c r="P38" s="25"/>
+        <v>876</v>
+      </c>
+      <c r="P38" s="21"/>
       <c r="Q38" s="21" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="R38" s="21" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B39" s="4">
         <v>3065</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D39" s="6">
+        <v>65</v>
+      </c>
+      <c r="E39" s="4">
+        <v>300</v>
+      </c>
+      <c r="F39" s="4">
         <v>100</v>
-      </c>
-      <c r="E39" s="4">
-        <v>100</v>
-      </c>
-      <c r="F39" s="4">
-        <v>600</v>
       </c>
       <c r="G39" s="4">
         <v>400</v>
@@ -18174,40 +18225,40 @@
         <v>2.78</v>
       </c>
       <c r="M39" s="21">
-        <v>0.2</v>
+        <v>0.13</v>
       </c>
       <c r="N39" s="21">
-        <v>4.9000000000000004</v>
+        <v>3.83</v>
       </c>
       <c r="O39" s="4">
-        <v>1985</v>
+        <v>2274</v>
       </c>
       <c r="P39" s="25"/>
       <c r="Q39" s="21" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="R39" s="21" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B40" s="4">
         <v>3065</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D40" s="6">
-        <v>200</v>
+        <v>65</v>
       </c>
       <c r="E40" s="4">
         <v>100</v>
       </c>
       <c r="F40" s="4">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="G40" s="4">
         <v>400</v>
@@ -18228,199 +18279,197 @@
         <v>2.78</v>
       </c>
       <c r="M40" s="21">
-        <v>1.07</v>
+        <v>0.13</v>
       </c>
       <c r="N40" s="21">
-        <v>6.41</v>
+        <v>3.88</v>
       </c>
       <c r="O40" s="4">
-        <v>1004</v>
+        <v>2248</v>
       </c>
       <c r="P40" s="25"/>
       <c r="Q40" s="21" t="s">
         <v>211</v>
       </c>
       <c r="R40" s="21" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
-      <c r="O41" s="21"/>
+      <c r="A41" s="6">
+        <v>4</v>
+      </c>
+      <c r="B41" s="4">
+        <v>3065</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D41" s="6">
+        <v>65</v>
+      </c>
+      <c r="E41" s="4">
+        <v>300</v>
+      </c>
+      <c r="F41" s="4">
+        <v>100</v>
+      </c>
+      <c r="G41" s="4">
+        <v>50</v>
+      </c>
+      <c r="H41" s="21">
+        <v>10</v>
+      </c>
+      <c r="I41" s="22">
+        <v>1</v>
+      </c>
+      <c r="J41" s="4">
+        <v>48</v>
+      </c>
+      <c r="K41" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L41" s="15">
+        <v>2.78</v>
+      </c>
+      <c r="M41" s="21">
+        <v>9.86</v>
+      </c>
+      <c r="N41" s="21">
+        <v>3.3</v>
+      </c>
+      <c r="O41" s="4">
+        <v>852</v>
+      </c>
       <c r="P41" s="25"/>
-      <c r="Q41" s="21"/>
-      <c r="R41" s="21"/>
+      <c r="Q41" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="R41" s="21" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="21"/>
-      <c r="N42" s="21"/>
+      <c r="A42" s="6">
+        <v>5</v>
+      </c>
+      <c r="B42" s="4">
+        <v>3065</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" s="6">
+        <v>65</v>
+      </c>
+      <c r="E42" s="4">
+        <v>300</v>
+      </c>
+      <c r="F42" s="4">
+        <v>300</v>
+      </c>
+      <c r="G42" s="4">
+        <v>400</v>
+      </c>
+      <c r="H42" s="21">
+        <v>10</v>
+      </c>
+      <c r="I42" s="22">
+        <v>1</v>
+      </c>
+      <c r="J42" s="4">
+        <v>48</v>
+      </c>
+      <c r="K42" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L42" s="15">
+        <v>2.78</v>
+      </c>
+      <c r="M42" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="N42" s="21">
+        <v>3.82</v>
+      </c>
       <c r="O42" s="21"/>
-      <c r="P42" s="21"/>
-      <c r="Q42" s="21"/>
-      <c r="R42" s="21"/>
+      <c r="P42" s="25"/>
+      <c r="Q42" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="R42" s="21" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="16">
+      <c r="A43" s="6"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="25"/>
+      <c r="Q43" s="21"/>
+      <c r="R43" s="21"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="21"/>
+      <c r="P44" s="25"/>
+      <c r="Q44" s="21"/>
+      <c r="R44" s="21"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" s="16">
         <v>1</v>
       </c>
-      <c r="B43" s="4">
-        <v>3065</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D43" s="6">
-        <v>65</v>
-      </c>
-      <c r="E43" s="4">
+      <c r="B45" s="4">
+        <v>2702</v>
+      </c>
+      <c r="C45" s="4">
+        <v>903</v>
+      </c>
+      <c r="D45" s="6">
+        <v>237</v>
+      </c>
+      <c r="E45" s="4">
         <v>300</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F45" s="4">
         <v>100</v>
       </c>
-      <c r="G43" s="4">
-        <v>100</v>
-      </c>
-      <c r="H43" s="21">
+      <c r="G45" s="4">
+        <v>200</v>
+      </c>
+      <c r="H45" s="22">
         <v>10</v>
       </c>
-      <c r="I43" s="22">
+      <c r="I45" s="22">
         <v>1</v>
-      </c>
-      <c r="J43" s="4">
-        <v>48</v>
-      </c>
-      <c r="K43" s="25">
-        <v>4890000</v>
-      </c>
-      <c r="L43" s="15">
-        <v>2.78</v>
-      </c>
-      <c r="M43" s="21">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="N43" s="21">
-        <v>3.18</v>
-      </c>
-      <c r="O43" s="4">
-        <v>876</v>
-      </c>
-      <c r="P43" s="21"/>
-      <c r="Q43" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="R43" s="21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="6">
-        <v>2</v>
-      </c>
-      <c r="B44" s="4">
-        <v>3065</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D44" s="6">
-        <v>65</v>
-      </c>
-      <c r="E44" s="4">
-        <v>300</v>
-      </c>
-      <c r="F44" s="4">
-        <v>100</v>
-      </c>
-      <c r="G44" s="4">
-        <v>400</v>
-      </c>
-      <c r="H44" s="21">
-        <v>10</v>
-      </c>
-      <c r="I44" s="22">
-        <v>15</v>
-      </c>
-      <c r="J44" s="4">
-        <v>48</v>
-      </c>
-      <c r="K44" s="25">
-        <v>4890000</v>
-      </c>
-      <c r="L44" s="15">
-        <v>2.78</v>
-      </c>
-      <c r="M44" s="21">
-        <v>0.13</v>
-      </c>
-      <c r="N44" s="21">
-        <v>3.83</v>
-      </c>
-      <c r="O44" s="4">
-        <v>2274</v>
-      </c>
-      <c r="P44" s="25"/>
-      <c r="Q44" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="R44" s="21" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="6">
-        <v>3</v>
-      </c>
-      <c r="B45" s="4">
-        <v>3065</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D45" s="6">
-        <v>65</v>
-      </c>
-      <c r="E45" s="4">
-        <v>100</v>
-      </c>
-      <c r="F45" s="4">
-        <v>300</v>
-      </c>
-      <c r="G45" s="4">
-        <v>400</v>
-      </c>
-      <c r="H45" s="21">
-        <v>10</v>
-      </c>
-      <c r="I45" s="22">
-        <v>15</v>
       </c>
       <c r="J45" s="4">
         <v>48</v>
@@ -18432,45 +18481,41 @@
         <v>2.78</v>
       </c>
       <c r="M45" s="21">
-        <v>0.13</v>
+        <v>86.65</v>
       </c>
       <c r="N45" s="21">
-        <v>3.88</v>
-      </c>
-      <c r="O45" s="4">
-        <v>2248</v>
-      </c>
-      <c r="P45" s="25"/>
-      <c r="Q45" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="R45" s="21" t="s">
-        <v>214</v>
+        <v>0.38</v>
+      </c>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B46" s="4">
-        <v>3065</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>188</v>
+        <v>2702</v>
+      </c>
+      <c r="C46" s="4">
+        <v>903</v>
       </c>
       <c r="D46" s="6">
-        <v>65</v>
+        <v>237</v>
       </c>
       <c r="E46" s="4">
+        <v>100</v>
+      </c>
+      <c r="F46" s="4">
         <v>300</v>
       </c>
-      <c r="F46" s="4">
-        <v>100</v>
-      </c>
       <c r="G46" s="4">
-        <v>50</v>
-      </c>
-      <c r="H46" s="21">
+        <v>200</v>
+      </c>
+      <c r="H46" s="22">
         <v>10</v>
       </c>
       <c r="I46" s="22">
@@ -18486,76 +18531,42 @@
         <v>2.78</v>
       </c>
       <c r="M46" s="21">
-        <v>9.86</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="N46" s="21">
-        <v>3.3</v>
-      </c>
-      <c r="O46" s="4">
-        <v>852</v>
-      </c>
+        <v>2.38</v>
+      </c>
+      <c r="O46" s="21"/>
       <c r="P46" s="25"/>
-      <c r="Q46" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="R46" s="21" t="s">
-        <v>218</v>
+      <c r="Q46" s="21"/>
+      <c r="R46" s="4" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="6">
-        <v>5</v>
-      </c>
-      <c r="B47" s="4">
-        <v>3065</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D47" s="6">
-        <v>65</v>
-      </c>
-      <c r="E47" s="4">
-        <v>300</v>
-      </c>
-      <c r="F47" s="4">
-        <v>300</v>
-      </c>
-      <c r="G47" s="4">
-        <v>400</v>
-      </c>
-      <c r="H47" s="21">
-        <v>10</v>
-      </c>
-      <c r="I47" s="22">
-        <v>1</v>
-      </c>
-      <c r="J47" s="4">
-        <v>48</v>
-      </c>
-      <c r="K47" s="25">
-        <v>4890000</v>
-      </c>
-      <c r="L47" s="15">
-        <v>2.78</v>
-      </c>
-      <c r="M47" s="21">
-        <v>0.25</v>
-      </c>
-      <c r="N47" s="21">
-        <v>3.82</v>
-      </c>
+      <c r="A47" s="6"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="25"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="21"/>
       <c r="O47" s="21"/>
-      <c r="P47" s="25"/>
-      <c r="Q47" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="R47" s="21" t="s">
-        <v>222</v>
-      </c>
+      <c r="P47" s="21"/>
+      <c r="Q47" s="21"/>
+      <c r="R47" s="21"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+      <c r="A48" s="16" t="s">
+        <v>237</v>
+      </c>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="6"/>
@@ -18570,89 +18581,193 @@
       <c r="M48" s="21"/>
       <c r="N48" s="21"/>
       <c r="O48" s="21"/>
-      <c r="P48" s="25"/>
+      <c r="P48" s="21"/>
       <c r="Q48" s="21"/>
       <c r="R48" s="21"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="15"/>
+      <c r="A49" s="6">
+        <v>1</v>
+      </c>
+      <c r="B49" s="4">
+        <v>3065</v>
+      </c>
+      <c r="C49" s="4">
+        <v>625</v>
+      </c>
+      <c r="D49" s="6">
+        <v>65</v>
+      </c>
+      <c r="E49" s="4">
+        <v>100</v>
+      </c>
+      <c r="F49" s="4">
+        <v>600</v>
+      </c>
+      <c r="G49" s="4">
+        <v>200</v>
+      </c>
+      <c r="H49" s="4">
+        <v>10</v>
+      </c>
+      <c r="I49" s="22">
+        <v>1</v>
+      </c>
+      <c r="J49" s="4">
+        <v>48</v>
+      </c>
+      <c r="K49" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L49" s="15">
+        <v>2.78</v>
+      </c>
       <c r="M49" s="21"/>
       <c r="N49" s="21"/>
       <c r="O49" s="21"/>
-      <c r="P49" s="21"/>
+      <c r="P49" s="25"/>
       <c r="Q49" s="21"/>
-      <c r="R49" s="21"/>
+      <c r="R49" s="21" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="25"/>
-      <c r="L50" s="15"/>
+      <c r="A50" s="6">
+        <v>2</v>
+      </c>
+      <c r="B50" s="4">
+        <v>3065</v>
+      </c>
+      <c r="C50" s="4">
+        <v>625</v>
+      </c>
+      <c r="D50" s="6">
+        <v>65</v>
+      </c>
+      <c r="E50" s="4">
+        <v>100</v>
+      </c>
+      <c r="F50" s="4">
+        <v>600</v>
+      </c>
+      <c r="G50" s="4">
+        <v>200</v>
+      </c>
+      <c r="H50" s="4">
+        <v>10</v>
+      </c>
+      <c r="I50" s="22">
+        <v>1</v>
+      </c>
+      <c r="J50" s="4">
+        <v>48</v>
+      </c>
+      <c r="K50" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L50" s="15">
+        <v>2.78</v>
+      </c>
       <c r="M50" s="21"/>
       <c r="N50" s="21"/>
       <c r="O50" s="21"/>
-      <c r="P50" s="25"/>
+      <c r="P50" s="21"/>
       <c r="Q50" s="21"/>
-      <c r="R50" s="21"/>
+      <c r="R50" s="21" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="25"/>
-      <c r="L51" s="15"/>
+      <c r="A51" s="16">
+        <v>3</v>
+      </c>
+      <c r="B51" s="4">
+        <v>3065</v>
+      </c>
+      <c r="C51" s="4">
+        <v>625</v>
+      </c>
+      <c r="D51" s="6">
+        <v>65</v>
+      </c>
+      <c r="E51" s="4">
+        <v>100</v>
+      </c>
+      <c r="F51" s="4">
+        <v>600</v>
+      </c>
+      <c r="G51" s="4">
+        <v>200</v>
+      </c>
+      <c r="H51" s="4">
+        <v>10</v>
+      </c>
+      <c r="I51" s="22">
+        <v>1</v>
+      </c>
+      <c r="J51" s="4">
+        <v>48</v>
+      </c>
+      <c r="K51" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L51" s="15">
+        <v>2.78</v>
+      </c>
       <c r="M51" s="21"/>
       <c r="N51" s="21"/>
       <c r="O51" s="21"/>
       <c r="P51" s="21"/>
       <c r="Q51" s="21"/>
-      <c r="R51" s="21"/>
+      <c r="R51" s="21" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="21"/>
-      <c r="H52" s="21"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="25"/>
-      <c r="L52" s="15"/>
-      <c r="M52" s="21"/>
-      <c r="N52" s="21"/>
-      <c r="O52" s="21"/>
+      <c r="A52" s="6">
+        <v>4</v>
+      </c>
+      <c r="B52" s="4">
+        <v>3065</v>
+      </c>
+      <c r="C52" s="4">
+        <v>625</v>
+      </c>
+      <c r="D52" s="6">
+        <v>65</v>
+      </c>
+      <c r="E52" s="4">
+        <v>100</v>
+      </c>
+      <c r="F52" s="4">
+        <v>600</v>
+      </c>
+      <c r="G52" s="4">
+        <v>2000</v>
+      </c>
+      <c r="H52" s="4">
+        <v>10</v>
+      </c>
+      <c r="I52" s="22">
+        <v>1</v>
+      </c>
+      <c r="J52" s="4">
+        <v>48</v>
+      </c>
+      <c r="K52" s="25">
+        <v>4890000</v>
+      </c>
+      <c r="L52" s="15">
+        <v>2.78</v>
+      </c>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
       <c r="P52" s="21"/>
       <c r="Q52" s="21"/>
-      <c r="R52" s="21"/>
+      <c r="R52" s="21" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
@@ -18661,98 +18776,54 @@
       <c r="D53" s="6"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
-      <c r="G53" s="21"/>
+      <c r="G53" s="4"/>
       <c r="H53" s="21"/>
-      <c r="I53" s="22"/>
+      <c r="I53" s="21"/>
       <c r="J53" s="4"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="15"/>
+      <c r="K53" s="23"/>
+      <c r="L53" s="6"/>
       <c r="M53" s="21"/>
       <c r="N53" s="21"/>
       <c r="O53" s="21"/>
-      <c r="P53" s="25"/>
+      <c r="P53" s="21"/>
       <c r="Q53" s="21"/>
       <c r="R53" s="21"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="6"/>
-      <c r="M54" s="21"/>
-      <c r="N54" s="21"/>
-      <c r="O54" s="21"/>
-      <c r="P54" s="21"/>
-      <c r="Q54" s="21"/>
-      <c r="R54" s="21"/>
+      <c r="A54" s="3"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="3"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="3"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="21"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="21"/>
-      <c r="H55" s="21"/>
-      <c r="I55" s="21"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="21"/>
-      <c r="N55" s="21"/>
-      <c r="O55" s="21"/>
-      <c r="P55" s="21"/>
-      <c r="Q55" s="21"/>
-      <c r="R55" s="21"/>
+      <c r="A55" s="3"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="3"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="3"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="23"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
-      <c r="P56" s="21"/>
-      <c r="Q56" s="21"/>
-      <c r="R56" s="21"/>
+      <c r="A56" s="3"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="3"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="3"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="21"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="23"/>
-      <c r="L57" s="6"/>
-      <c r="M57" s="21"/>
-      <c r="N57" s="21"/>
-      <c r="O57" s="21"/>
-      <c r="P57" s="21"/>
-      <c r="Q57" s="21"/>
-      <c r="R57" s="21"/>
+      <c r="A57" s="3"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="3"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="3"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
@@ -18762,42 +18833,6 @@
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
       <c r="L58" s="3"/>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="3"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
-      <c r="L59" s="3"/>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="3"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="8"/>
-      <c r="L60" s="3"/>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="3"/>
-      <c r="J61" s="8"/>
-      <c r="K61" s="8"/>
-      <c r="L61" s="3"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="3"/>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8"/>
-      <c r="L62" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18837,7 +18872,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>43</v>
@@ -18848,10 +18883,10 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
@@ -18924,7 +18959,7 @@
         <v>3065</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D3" s="6">
         <v>65</v>
@@ -18962,7 +18997,7 @@
       <c r="O3" s="21"/>
       <c r="P3" s="25"/>
       <c r="Q3" s="21" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="R3" s="4"/>
     </row>
@@ -18974,7 +19009,7 @@
         <v>3065</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D4" s="6">
         <v>65</v>
@@ -19014,10 +19049,10 @@
       </c>
       <c r="P4" s="25"/>
       <c r="Q4" s="4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="R4" s="21" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -19026,7 +19061,7 @@
         <v>3065</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D5" s="6">
         <v>65</v>
@@ -19066,10 +19101,10 @@
       </c>
       <c r="P5" s="25"/>
       <c r="Q5" s="21" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="R5" s="21" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -19077,7 +19112,7 @@
         <v>3065</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D6" s="6">
         <v>65</v>
@@ -19117,10 +19152,10 @@
       </c>
       <c r="P6" s="25"/>
       <c r="Q6" s="21" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -19129,7 +19164,7 @@
         <v>3065</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D7" s="6">
         <v>65</v>
@@ -19169,10 +19204,10 @@
       </c>
       <c r="P7" s="25"/>
       <c r="Q7" s="21" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="R7" s="21" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -19181,7 +19216,7 @@
         <v>3065</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D8" s="6">
         <v>65</v>
@@ -19219,10 +19254,10 @@
       <c r="O8" s="21"/>
       <c r="P8" s="25"/>
       <c r="Q8" s="21" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="R8" s="21" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -19233,7 +19268,7 @@
         <v>3065</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D9" s="6">
         <v>65</v>
@@ -19271,10 +19306,10 @@
       <c r="O9" s="21"/>
       <c r="P9" s="25"/>
       <c r="Q9" s="21" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="R9" s="21" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -19285,7 +19320,7 @@
         <v>3065</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D10" s="6">
         <v>65</v>
@@ -19320,7 +19355,7 @@
       <c r="P10" s="21"/>
       <c r="Q10" s="21"/>
       <c r="R10" s="21" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>